<commit_message>
LoS double frequence + report stepcase
</commit_message>
<xml_diff>
--- a/lib/PHPExcel/templates/FT Loa.xlsx
+++ b/lib/PHPExcel/templates/FT Loa.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18730"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -348,11 +348,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0.000"/>
     <numFmt numFmtId="166" formatCode="###\ ###\ ###\ ###\ ###\ "/>
     <numFmt numFmtId="167" formatCode="0.0##"/>
+    <numFmt numFmtId="168" formatCode="0.000"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -743,7 +744,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="130">
+  <cellXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -1014,6 +1015,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1039,7 +1048,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1598,20 +1612,20 @@
     </row>
     <row r="4" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="120" t="s">
+      <c r="A5" s="124" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="121"/>
-      <c r="C5" s="121"/>
-      <c r="D5" s="121"/>
-      <c r="E5" s="121"/>
-      <c r="F5" s="122"/>
-      <c r="H5" s="120" t="s">
+      <c r="B5" s="125"/>
+      <c r="C5" s="125"/>
+      <c r="D5" s="125"/>
+      <c r="E5" s="125"/>
+      <c r="F5" s="126"/>
+      <c r="H5" s="124" t="s">
         <v>1</v>
       </c>
-      <c r="I5" s="121"/>
-      <c r="J5" s="121"/>
-      <c r="K5" s="122"/>
+      <c r="I5" s="125"/>
+      <c r="J5" s="125"/>
+      <c r="K5" s="126"/>
     </row>
     <row r="6" spans="1:14" ht="6.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
@@ -1698,13 +1712,13 @@
       <c r="K11" s="60"/>
     </row>
     <row r="12" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="120" t="s">
+      <c r="A12" s="124" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="121"/>
-      <c r="C12" s="121"/>
-      <c r="D12" s="121"/>
-      <c r="E12" s="121"/>
+      <c r="B12" s="125"/>
+      <c r="C12" s="125"/>
+      <c r="D12" s="125"/>
+      <c r="E12" s="125"/>
       <c r="F12" s="23"/>
       <c r="H12" s="18" t="s">
         <v>8</v>
@@ -1771,12 +1785,12 @@
       </c>
       <c r="E16" s="24"/>
       <c r="F16" s="62"/>
-      <c r="H16" s="120" t="s">
+      <c r="H16" s="124" t="s">
         <v>15</v>
       </c>
-      <c r="I16" s="121"/>
-      <c r="J16" s="121"/>
-      <c r="K16" s="122"/>
+      <c r="I16" s="125"/>
+      <c r="J16" s="125"/>
+      <c r="K16" s="126"/>
       <c r="N16" s="24"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
@@ -1837,14 +1851,14 @@
       <c r="K20" s="86"/>
     </row>
     <row r="21" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="120" t="s">
+      <c r="A21" s="124" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="121"/>
-      <c r="C21" s="121"/>
-      <c r="D21" s="121"/>
-      <c r="E21" s="121"/>
-      <c r="F21" s="122"/>
+      <c r="B21" s="125"/>
+      <c r="C21" s="125"/>
+      <c r="D21" s="125"/>
+      <c r="E21" s="125"/>
+      <c r="F21" s="126"/>
       <c r="H21" s="6"/>
       <c r="I21" s="87"/>
       <c r="J21" s="53" t="s">
@@ -2061,10 +2075,10 @@
       <c r="K33" s="114"/>
     </row>
     <row r="34" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="125" t="s">
+      <c r="A34" s="129" t="s">
         <v>67</v>
       </c>
-      <c r="B34" s="126"/>
+      <c r="B34" s="130"/>
       <c r="C34" s="35"/>
       <c r="D34" s="55" t="s">
         <v>65</v>
@@ -2163,19 +2177,19 @@
       <c r="O39" s="32"/>
     </row>
     <row r="40" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="120" t="s">
+      <c r="A40" s="124" t="s">
         <v>42</v>
       </c>
-      <c r="B40" s="121"/>
-      <c r="C40" s="121"/>
-      <c r="D40" s="121"/>
-      <c r="E40" s="121"/>
-      <c r="F40" s="121"/>
-      <c r="G40" s="121"/>
-      <c r="H40" s="121"/>
-      <c r="I40" s="121"/>
-      <c r="J40" s="121"/>
-      <c r="K40" s="122"/>
+      <c r="B40" s="125"/>
+      <c r="C40" s="125"/>
+      <c r="D40" s="125"/>
+      <c r="E40" s="125"/>
+      <c r="F40" s="125"/>
+      <c r="G40" s="125"/>
+      <c r="H40" s="125"/>
+      <c r="I40" s="125"/>
+      <c r="J40" s="125"/>
+      <c r="K40" s="126"/>
       <c r="M40" s="32"/>
       <c r="N40" s="32"/>
       <c r="O40" s="32"/>
@@ -2238,21 +2252,21 @@
       <c r="S43" s="32"/>
     </row>
     <row r="44" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="120" t="s">
+      <c r="A44" s="124" t="s">
         <v>43</v>
       </c>
-      <c r="B44" s="121"/>
-      <c r="C44" s="121"/>
-      <c r="D44" s="121"/>
-      <c r="E44" s="121"/>
-      <c r="F44" s="121"/>
-      <c r="G44" s="121"/>
-      <c r="H44" s="121"/>
-      <c r="I44" s="122"/>
-      <c r="J44" s="127" t="s">
+      <c r="B44" s="125"/>
+      <c r="C44" s="125"/>
+      <c r="D44" s="125"/>
+      <c r="E44" s="125"/>
+      <c r="F44" s="125"/>
+      <c r="G44" s="125"/>
+      <c r="H44" s="125"/>
+      <c r="I44" s="126"/>
+      <c r="J44" s="131" t="s">
         <v>87</v>
       </c>
-      <c r="K44" s="128"/>
+      <c r="K44" s="132"/>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A45" s="18" t="s">
@@ -2348,8 +2362,8 @@
       <c r="G50" s="20"/>
       <c r="H50" s="20"/>
       <c r="I50" s="20"/>
-      <c r="J50" s="123"/>
-      <c r="K50" s="124"/>
+      <c r="J50" s="127"/>
+      <c r="K50" s="128"/>
     </row>
     <row r="51" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="52" spans="1:12" x14ac:dyDescent="0.2">
@@ -2372,7 +2386,7 @@
       <c r="K52" s="65"/>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A53" s="129"/>
+      <c r="A53" s="120"/>
       <c r="B53" s="32"/>
       <c r="C53" s="32"/>
       <c r="D53" s="32"/>
@@ -2382,7 +2396,7 @@
       <c r="H53" s="32"/>
       <c r="I53" s="32"/>
       <c r="J53" s="32"/>
-      <c r="K53" s="34"/>
+      <c r="K53" s="121"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" s="18"/>
@@ -2392,10 +2406,10 @@
       <c r="E54" s="32"/>
       <c r="F54" s="32"/>
       <c r="G54" s="32"/>
-      <c r="H54" s="32"/>
-      <c r="I54" s="32"/>
-      <c r="J54" s="32"/>
-      <c r="K54" s="34"/>
+      <c r="H54" s="22"/>
+      <c r="I54" s="22"/>
+      <c r="J54" s="22"/>
+      <c r="K54" s="122"/>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" s="18"/>
@@ -2405,10 +2419,10 @@
       <c r="E55" s="32"/>
       <c r="F55" s="32"/>
       <c r="G55" s="32"/>
-      <c r="H55" s="32"/>
-      <c r="I55" s="32"/>
-      <c r="J55" s="32"/>
-      <c r="K55" s="34"/>
+      <c r="H55" s="22"/>
+      <c r="I55" s="133"/>
+      <c r="J55" s="133"/>
+      <c r="K55" s="122"/>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" s="18"/>
@@ -2418,10 +2432,10 @@
       <c r="E56" s="32"/>
       <c r="F56" s="32"/>
       <c r="G56" s="32"/>
-      <c r="H56" s="32"/>
-      <c r="I56" s="32"/>
-      <c r="J56" s="32"/>
-      <c r="K56" s="34"/>
+      <c r="H56" s="22"/>
+      <c r="I56" s="133"/>
+      <c r="J56" s="133"/>
+      <c r="K56" s="122"/>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57" s="18"/>
@@ -2431,10 +2445,10 @@
       <c r="E57" s="32"/>
       <c r="F57" s="32"/>
       <c r="G57" s="32"/>
-      <c r="H57" s="32"/>
-      <c r="I57" s="32"/>
-      <c r="J57" s="32"/>
-      <c r="K57" s="34"/>
+      <c r="H57" s="22"/>
+      <c r="I57" s="133"/>
+      <c r="J57" s="133"/>
+      <c r="K57" s="122"/>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" s="18"/>
@@ -2444,10 +2458,10 @@
       <c r="E58" s="32"/>
       <c r="F58" s="32"/>
       <c r="G58" s="32"/>
-      <c r="H58" s="32"/>
-      <c r="I58" s="32"/>
-      <c r="J58" s="32"/>
-      <c r="K58" s="34"/>
+      <c r="H58" s="22"/>
+      <c r="I58" s="133"/>
+      <c r="J58" s="133"/>
+      <c r="K58" s="122"/>
     </row>
     <row r="59" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="19"/>
@@ -2457,10 +2471,10 @@
       <c r="E59" s="20"/>
       <c r="F59" s="20"/>
       <c r="G59" s="20"/>
-      <c r="H59" s="20"/>
-      <c r="I59" s="20"/>
-      <c r="J59" s="20"/>
-      <c r="K59" s="21"/>
+      <c r="H59" s="81"/>
+      <c r="I59" s="134"/>
+      <c r="J59" s="134"/>
+      <c r="K59" s="123"/>
       <c r="L59" s="32"/>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
new FT & Checklist (prestart)
</commit_message>
<xml_diff>
--- a/lib/PHPExcel/templates/FT Loa.xlsx
+++ b/lib/PHPExcel/templates/FT Loa.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,12 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="15" yWindow="0" windowWidth="9645" windowHeight="11955"/>
+    <workbookView xWindow="15" yWindow="0" windowWidth="9645" windowHeight="11955" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="FTLCFHCFEFF" sheetId="2" r:id="rId1"/>
+    <sheet name="FT" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">FT!$A$1:$P$71</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">FTLCFHCFEFF!$A$1:$K$60</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -22,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="181">
   <si>
     <t>DONNEES EPROUVETTE</t>
   </si>
@@ -343,19 +345,447 @@
   <si>
     <t>Grey cell: unused equipement or information, unless specified -- Instructions on GPM need to be checked if checker is empty</t>
   </si>
+  <si>
+    <t>Grey cell : unused equipment or information (unless specified) -- Instructions on GPM need to be checked if checker is empty</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Estimated</t>
+  </si>
+  <si>
+    <t>Checker</t>
+  </si>
+  <si>
+    <t>Technician</t>
+  </si>
+  <si>
+    <t>Fracture</t>
+  </si>
+  <si>
+    <r>
+      <t>Rupture-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF8497B0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>ERT(kN)</t>
+    </r>
+  </si>
+  <si>
+    <t>Duration (h)</t>
+  </si>
+  <si>
+    <t>Final Cycle</t>
+  </si>
+  <si>
+    <t>MINIMUM</t>
+  </si>
+  <si>
+    <t>End of test</t>
+  </si>
+  <si>
+    <t>BOT</t>
+  </si>
+  <si>
+    <t>STRAP</t>
+  </si>
+  <si>
+    <t>TOP</t>
+  </si>
+  <si>
+    <t>Load</t>
+  </si>
+  <si>
+    <t>Corrected</t>
+  </si>
+  <si>
+    <t>Cust</t>
+  </si>
+  <si>
+    <t>Temperature (°C)</t>
+  </si>
+  <si>
+    <t>Fréquency (Hz)</t>
+  </si>
+  <si>
+    <t>STL requirement</t>
+  </si>
+  <si>
+    <t>(%)</t>
+  </si>
+  <si>
+    <t>Strain</t>
+  </si>
+  <si>
+    <r>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color rgb="FF8497B0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>st</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF8497B0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Check</t>
+    </r>
+  </si>
+  <si>
+    <t>T° Alarm</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF8497B0"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t xml:space="preserve"> e </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF8497B0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Min (%)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF8497B0"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>e</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF8497B0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Max (%)</t>
+    </r>
+  </si>
+  <si>
+    <t>(mm)</t>
+  </si>
+  <si>
+    <t>Disp</t>
+  </si>
+  <si>
+    <t>UnderPeak</t>
+  </si>
+  <si>
+    <t>Cycle Counting</t>
+  </si>
+  <si>
+    <r>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color rgb="FF8497B0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>st</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF8497B0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> cycle</t>
+    </r>
+  </si>
+  <si>
+    <t>Limit</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>Top</t>
+  </si>
+  <si>
+    <t>Specimen Temperature</t>
+  </si>
+  <si>
+    <t>Stabilisation Time</t>
+  </si>
+  <si>
+    <t>Temperature Control</t>
+  </si>
+  <si>
+    <t>Nb strap</t>
+  </si>
+  <si>
+    <t>Control</t>
+  </si>
+  <si>
+    <t>ET</t>
+  </si>
+  <si>
+    <t>Ramp to Temp</t>
+  </si>
+  <si>
+    <r>
+      <t>Modulus</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="7"/>
+        <color rgb="FF8497B0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>ET</t>
+    </r>
+  </si>
+  <si>
+    <t>RT</t>
+  </si>
+  <si>
+    <r>
+      <t>Modulus</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="7"/>
+        <color rgb="FF8497B0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>RT</t>
+    </r>
+  </si>
+  <si>
+    <t>Lo</t>
+  </si>
+  <si>
+    <t>Measured</t>
+  </si>
+  <si>
+    <t>Dimension 3</t>
+  </si>
+  <si>
+    <t>Dimension 2</t>
+  </si>
+  <si>
+    <t>Dimension 1</t>
+  </si>
+  <si>
+    <t>Runout</t>
+  </si>
+  <si>
+    <t>Signal</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Material</t>
+  </si>
+  <si>
+    <t>Drawing</t>
+  </si>
+  <si>
+    <t>Test Informations</t>
+  </si>
+  <si>
+    <t>Str</t>
+  </si>
+  <si>
+    <t>Loa</t>
+  </si>
+  <si>
+    <t>Temp Acq</t>
+  </si>
+  <si>
+    <t>Oscilloscope</t>
+  </si>
+  <si>
+    <t>Computer</t>
+  </si>
+  <si>
+    <t>Sens.</t>
+  </si>
+  <si>
+    <t>Conv.</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>FS</t>
+  </si>
+  <si>
+    <t>NS</t>
+  </si>
+  <si>
+    <t>Cooling</t>
+  </si>
+  <si>
+    <t>Heating</t>
+  </si>
+  <si>
+    <t>Tool Bot</t>
+  </si>
+  <si>
+    <t>Tool Top</t>
+  </si>
+  <si>
+    <t>Frame Informations</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF8497B0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Date</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF8497B0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color rgb="FF8497B0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(YYYY-MM-DD)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF8497B0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(Specimen) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF8497B0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Checker</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF8497B0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (Test)</t>
+    </r>
+  </si>
+  <si>
+    <t>Raw Data</t>
+  </si>
+  <si>
+    <t>Frame</t>
+  </si>
+  <si>
+    <t>Test Number</t>
+  </si>
+  <si>
+    <t>File Number</t>
+  </si>
+  <si>
+    <t>Specimen</t>
+  </si>
+  <si>
+    <t>Prefixe</t>
+  </si>
+  <si>
+    <t>Job</t>
+  </si>
+  <si>
+    <t>FT - 48558</t>
+  </si>
+  <si>
+    <t>Load Control Fatigue Test</t>
+  </si>
+  <si>
+    <t>Frequency Change</t>
+  </si>
+  <si>
+    <t>End level</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="5">
+  <numFmts count="7">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0.000"/>
     <numFmt numFmtId="166" formatCode="###\ ###\ ###\ ###\ ###\ "/>
     <numFmt numFmtId="167" formatCode="0.0##"/>
     <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="170" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="39">
     <font>
       <sz val="10"/>
       <name val="MS Sans Serif"/>
@@ -415,8 +845,182 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="MS Sans Serif"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF223962"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF8E98A5"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF223962"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF203764"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF203764"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF223962"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF8497B0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF203764"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF8497B0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF8497B0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF8497B0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF8E98A5"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color rgb="FF8497B0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF8497B0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF203764"/>
+      <name val="Wingdings"/>
+      <charset val="2"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="10"/>
+      <color rgb="FF8497B0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF8497B0"/>
+      <name val="Arial"/>
+      <family val="1"/>
+      <charset val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF8497B0"/>
+      <name val="Symbol"/>
+      <family val="1"/>
+      <charset val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="3" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="7"/>
+      <color rgb="FF8497B0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF8E98A5"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF8497B0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF8497B0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF44546A"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -435,8 +1039,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="28">
+  <borders count="39">
     <border>
       <left/>
       <right/>
@@ -739,12 +1355,142 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="135">
+  <cellXfs count="220">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -1023,6 +1769,12 @@
     <xf numFmtId="166" fontId="3" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1048,16 +1800,232 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="22" fontId="18" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="18" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="34" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="170" fontId="21" fillId="0" borderId="29" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="21" fillId="0" borderId="32" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="169" fontId="21" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="38" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="21" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="28" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="36" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 3" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1229,6 +2197,95 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="742950" cy="762000"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A142A484-4C10-4B22-AA0A-3662C47E892A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="161925"/>
+          <a:ext cx="742950" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>66062</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="381811" cy="1938130"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE4FC251-732B-4BB3-A801-471BA00CDB86}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10924562" y="0"/>
+          <a:ext cx="381811" cy="1938130"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1585,9 +2642,9 @@
   </sheetPr>
   <dimension ref="A1:S60"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="98" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
+    <sheetView view="pageBreakPreview" zoomScaleNormal="98" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="14.7109375" style="10" customWidth="1"/>
     <col min="2" max="2" width="10" style="10" customWidth="1"/>
@@ -1602,32 +2659,32 @@
     <col min="12" max="16384" width="8.7109375" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14">
       <c r="G1" s="11"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14">
       <c r="G2" s="71" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="124" t="s">
+    <row r="4" spans="1:14" ht="13.5" thickBot="1"/>
+    <row r="5" spans="1:14" ht="13.5" thickBot="1">
+      <c r="A5" s="126" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="125"/>
-      <c r="C5" s="125"/>
-      <c r="D5" s="125"/>
-      <c r="E5" s="125"/>
-      <c r="F5" s="126"/>
-      <c r="H5" s="124" t="s">
+      <c r="B5" s="127"/>
+      <c r="C5" s="127"/>
+      <c r="D5" s="127"/>
+      <c r="E5" s="127"/>
+      <c r="F5" s="128"/>
+      <c r="H5" s="126" t="s">
         <v>1</v>
       </c>
-      <c r="I5" s="125"/>
-      <c r="J5" s="125"/>
-      <c r="K5" s="126"/>
-    </row>
-    <row r="6" spans="1:14" ht="6.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I5" s="127"/>
+      <c r="J5" s="127"/>
+      <c r="K5" s="128"/>
+    </row>
+    <row r="6" spans="1:14" ht="6.75" customHeight="1">
       <c r="A6" s="12"/>
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
@@ -1639,7 +2696,7 @@
       <c r="J6" s="16"/>
       <c r="K6" s="17"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14">
       <c r="A7" s="18" t="s">
         <v>25</v>
       </c>
@@ -1655,7 +2712,7 @@
       <c r="J7" s="59"/>
       <c r="K7" s="60"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14">
       <c r="A8" s="18" t="s">
         <v>26</v>
       </c>
@@ -1671,7 +2728,7 @@
       <c r="J8" s="61"/>
       <c r="K8" s="62"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14">
       <c r="A9" s="18" t="s">
         <v>4</v>
       </c>
@@ -1687,7 +2744,7 @@
       <c r="J9" s="61"/>
       <c r="K9" s="62"/>
     </row>
-    <row r="10" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="13.5" thickBot="1">
       <c r="A10" s="19"/>
       <c r="B10" s="20"/>
       <c r="C10" s="20"/>
@@ -1703,7 +2760,7 @@
       </c>
       <c r="K10" s="60"/>
     </row>
-    <row r="11" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="13.5" thickBot="1">
       <c r="H11" s="18" t="s">
         <v>7</v>
       </c>
@@ -1711,14 +2768,14 @@
       <c r="J11" s="59"/>
       <c r="K11" s="60"/>
     </row>
-    <row r="12" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="124" t="s">
+    <row r="12" spans="1:14" ht="13.5" thickBot="1">
+      <c r="A12" s="126" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="125"/>
-      <c r="C12" s="125"/>
-      <c r="D12" s="125"/>
-      <c r="E12" s="125"/>
+      <c r="B12" s="127"/>
+      <c r="C12" s="127"/>
+      <c r="D12" s="127"/>
+      <c r="E12" s="127"/>
       <c r="F12" s="23"/>
       <c r="H12" s="18" t="s">
         <v>8</v>
@@ -1727,7 +2784,7 @@
       <c r="J12" s="61"/>
       <c r="K12" s="62"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14">
       <c r="A13" s="18" t="s">
         <v>11</v>
       </c>
@@ -1745,7 +2802,7 @@
       <c r="J13" s="78"/>
       <c r="K13" s="79"/>
     </row>
-    <row r="14" spans="1:14" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="3" customHeight="1" thickBot="1">
       <c r="A14" s="18"/>
       <c r="B14" s="80"/>
       <c r="C14" s="76"/>
@@ -1757,7 +2814,7 @@
       <c r="J14" s="81"/>
       <c r="K14" s="21"/>
     </row>
-    <row r="15" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="13.5" thickBot="1">
       <c r="A15" s="25" t="s">
         <v>29</v>
       </c>
@@ -1774,7 +2831,7 @@
       <c r="K15" s="26"/>
       <c r="N15" s="24"/>
     </row>
-    <row r="16" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="13.5" thickBot="1">
       <c r="A16" s="18" t="s">
         <v>30</v>
       </c>
@@ -1785,15 +2842,15 @@
       </c>
       <c r="E16" s="24"/>
       <c r="F16" s="62"/>
-      <c r="H16" s="124" t="s">
+      <c r="H16" s="126" t="s">
         <v>15</v>
       </c>
-      <c r="I16" s="125"/>
-      <c r="J16" s="125"/>
-      <c r="K16" s="126"/>
+      <c r="I16" s="127"/>
+      <c r="J16" s="127"/>
+      <c r="K16" s="128"/>
       <c r="N16" s="24"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14">
       <c r="A17" s="18" t="s">
         <v>31</v>
       </c>
@@ -1814,7 +2871,7 @@
       <c r="K17" s="60"/>
       <c r="N17" s="24"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14">
       <c r="A18" s="18"/>
       <c r="B18" s="32"/>
       <c r="C18" s="32"/>
@@ -1828,7 +2885,7 @@
       <c r="J18" s="61"/>
       <c r="K18" s="62"/>
     </row>
-    <row r="19" spans="1:14" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="3" customHeight="1" thickBot="1">
       <c r="A19" s="28"/>
       <c r="B19" s="81"/>
       <c r="C19" s="81"/>
@@ -1840,7 +2897,7 @@
       <c r="J19" s="83"/>
       <c r="K19" s="84"/>
     </row>
-    <row r="20" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="13.5" thickBot="1">
       <c r="H20" s="18" t="s">
         <v>70</v>
       </c>
@@ -1850,15 +2907,15 @@
       </c>
       <c r="K20" s="86"/>
     </row>
-    <row r="21" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="124" t="s">
+    <row r="21" spans="1:14" ht="13.5" thickBot="1">
+      <c r="A21" s="126" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="125"/>
-      <c r="C21" s="125"/>
-      <c r="D21" s="125"/>
-      <c r="E21" s="125"/>
-      <c r="F21" s="126"/>
+      <c r="B21" s="127"/>
+      <c r="C21" s="127"/>
+      <c r="D21" s="127"/>
+      <c r="E21" s="127"/>
+      <c r="F21" s="128"/>
       <c r="H21" s="6"/>
       <c r="I21" s="87"/>
       <c r="J21" s="53" t="s">
@@ -1866,7 +2923,7 @@
       </c>
       <c r="K21" s="88"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14">
       <c r="A22" s="15"/>
       <c r="C22" s="32"/>
       <c r="D22" s="16"/>
@@ -1881,7 +2938,7 @@
       </c>
       <c r="K22" s="90"/>
     </row>
-    <row r="23" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" ht="14.25" customHeight="1">
       <c r="A23" s="6" t="s">
         <v>73</v>
       </c>
@@ -1902,7 +2959,7 @@
       </c>
       <c r="K23" s="92"/>
     </row>
-    <row r="24" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" ht="13.5" customHeight="1">
       <c r="A24" s="6" t="s">
         <v>71</v>
       </c>
@@ -1923,7 +2980,7 @@
       </c>
       <c r="K24" s="94"/>
     </row>
-    <row r="25" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" ht="13.5" customHeight="1">
       <c r="A25" s="6" t="s">
         <v>74</v>
       </c>
@@ -1944,7 +3001,7 @@
       </c>
       <c r="K25" s="7"/>
     </row>
-    <row r="26" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" ht="13.5" customHeight="1">
       <c r="A26" s="18"/>
       <c r="D26" s="32"/>
       <c r="E26" s="32"/>
@@ -1958,7 +3015,7 @@
       </c>
       <c r="K26" s="4"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14">
       <c r="A27" s="18"/>
       <c r="B27" s="33" t="s">
         <v>53</v>
@@ -1978,7 +3035,7 @@
       </c>
       <c r="K27" s="5"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14">
       <c r="A28" s="54" t="s">
         <v>62</v>
       </c>
@@ -1997,7 +3054,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14">
       <c r="A29" s="54" t="s">
         <v>61</v>
       </c>
@@ -2016,7 +3073,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14">
       <c r="A30" s="54" t="s">
         <v>63</v>
       </c>
@@ -2035,7 +3092,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14">
       <c r="A31" s="18"/>
       <c r="B31" s="32"/>
       <c r="C31" s="32"/>
@@ -2049,7 +3106,7 @@
       <c r="J31" s="111"/>
       <c r="K31" s="101"/>
     </row>
-    <row r="32" spans="1:14" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" ht="3" customHeight="1" thickBot="1">
       <c r="A32" s="28"/>
       <c r="B32" s="81"/>
       <c r="C32" s="81"/>
@@ -2061,7 +3118,7 @@
       <c r="J32" s="112"/>
       <c r="K32" s="113"/>
     </row>
-    <row r="33" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" ht="13.5" thickBot="1">
       <c r="A33" s="32"/>
       <c r="B33" s="32"/>
       <c r="C33" s="32"/>
@@ -2074,11 +3131,11 @@
       <c r="J33" s="20"/>
       <c r="K33" s="114"/>
     </row>
-    <row r="34" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="129" t="s">
+    <row r="34" spans="1:19" ht="13.5" thickBot="1">
+      <c r="A34" s="131" t="s">
         <v>67</v>
       </c>
-      <c r="B34" s="130"/>
+      <c r="B34" s="132"/>
       <c r="C34" s="35"/>
       <c r="D34" s="55" t="s">
         <v>65</v>
@@ -2093,7 +3150,7 @@
       <c r="J34" s="64"/>
       <c r="K34" s="37"/>
     </row>
-    <row r="35" spans="1:19" ht="6.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:19" ht="6.75" customHeight="1">
       <c r="A35" s="36"/>
       <c r="B35" s="37"/>
       <c r="C35" s="35"/>
@@ -2106,7 +3163,7 @@
       <c r="J35" s="22"/>
       <c r="K35" s="58"/>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:19">
       <c r="A36" s="18" t="s">
         <v>75</v>
       </c>
@@ -2129,7 +3186,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:19">
       <c r="A37" s="18" t="s">
         <v>76</v>
       </c>
@@ -2151,7 +3208,7 @@
       <c r="N37" s="32"/>
       <c r="O37" s="32"/>
     </row>
-    <row r="38" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" ht="13.5" thickBot="1">
       <c r="A38" s="19" t="s">
         <v>78</v>
       </c>
@@ -2171,30 +3228,30 @@
       <c r="N38" s="32"/>
       <c r="O38" s="32"/>
     </row>
-    <row r="39" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" ht="13.5" thickBot="1">
       <c r="M39" s="32"/>
       <c r="N39" s="32"/>
       <c r="O39" s="32"/>
     </row>
-    <row r="40" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="124" t="s">
+    <row r="40" spans="1:19" ht="13.5" thickBot="1">
+      <c r="A40" s="126" t="s">
         <v>42</v>
       </c>
-      <c r="B40" s="125"/>
-      <c r="C40" s="125"/>
-      <c r="D40" s="125"/>
-      <c r="E40" s="125"/>
-      <c r="F40" s="125"/>
-      <c r="G40" s="125"/>
-      <c r="H40" s="125"/>
-      <c r="I40" s="125"/>
-      <c r="J40" s="125"/>
-      <c r="K40" s="126"/>
+      <c r="B40" s="127"/>
+      <c r="C40" s="127"/>
+      <c r="D40" s="127"/>
+      <c r="E40" s="127"/>
+      <c r="F40" s="127"/>
+      <c r="G40" s="127"/>
+      <c r="H40" s="127"/>
+      <c r="I40" s="127"/>
+      <c r="J40" s="127"/>
+      <c r="K40" s="128"/>
       <c r="M40" s="32"/>
       <c r="N40" s="32"/>
       <c r="O40" s="32"/>
     </row>
-    <row r="41" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" ht="15.75">
       <c r="A41" s="51"/>
       <c r="B41" s="115"/>
       <c r="C41" s="116"/>
@@ -2214,7 +3271,7 @@
       <c r="N41" s="32"/>
       <c r="O41" s="32"/>
     </row>
-    <row r="42" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" ht="13.5" thickBot="1">
       <c r="A42" s="19" t="s">
         <v>60</v>
       </c>
@@ -2243,7 +3300,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="43" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:19" ht="16.5" thickBot="1">
       <c r="N43" s="46"/>
       <c r="O43" s="83"/>
       <c r="P43" s="83"/>
@@ -2251,24 +3308,24 @@
       <c r="R43" s="83"/>
       <c r="S43" s="32"/>
     </row>
-    <row r="44" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="124" t="s">
+    <row r="44" spans="1:19" ht="13.5" thickBot="1">
+      <c r="A44" s="126" t="s">
         <v>43</v>
       </c>
-      <c r="B44" s="125"/>
-      <c r="C44" s="125"/>
-      <c r="D44" s="125"/>
-      <c r="E44" s="125"/>
-      <c r="F44" s="125"/>
-      <c r="G44" s="125"/>
-      <c r="H44" s="125"/>
-      <c r="I44" s="126"/>
-      <c r="J44" s="131" t="s">
+      <c r="B44" s="127"/>
+      <c r="C44" s="127"/>
+      <c r="D44" s="127"/>
+      <c r="E44" s="127"/>
+      <c r="F44" s="127"/>
+      <c r="G44" s="127"/>
+      <c r="H44" s="127"/>
+      <c r="I44" s="128"/>
+      <c r="J44" s="133" t="s">
         <v>87</v>
       </c>
-      <c r="K44" s="132"/>
-    </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="K44" s="134"/>
+    </row>
+    <row r="45" spans="1:19">
       <c r="A45" s="18" t="s">
         <v>89</v>
       </c>
@@ -2288,7 +3345,7 @@
       </c>
       <c r="K45" s="49"/>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:19">
       <c r="A46" s="18"/>
       <c r="B46" s="32"/>
       <c r="C46" s="32"/>
@@ -2303,7 +3360,7 @@
       <c r="J46" s="69"/>
       <c r="K46" s="118"/>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:19">
       <c r="A47" s="18" t="s">
         <v>46</v>
       </c>
@@ -2322,7 +3379,7 @@
       </c>
       <c r="K47" s="34"/>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:19">
       <c r="A48" s="18"/>
       <c r="B48" s="32"/>
       <c r="C48" s="32"/>
@@ -2335,7 +3392,7 @@
       <c r="J48" s="48"/>
       <c r="K48" s="49"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:12">
       <c r="A49" s="6" t="s">
         <v>82</v>
       </c>
@@ -2352,7 +3409,7 @@
       <c r="J49" s="68"/>
       <c r="K49" s="63"/>
     </row>
-    <row r="50" spans="1:12" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" ht="5.25" customHeight="1" thickBot="1">
       <c r="A50" s="19"/>
       <c r="B50" s="20"/>
       <c r="C50" s="20"/>
@@ -2362,11 +3419,11 @@
       <c r="G50" s="20"/>
       <c r="H50" s="20"/>
       <c r="I50" s="20"/>
-      <c r="J50" s="127"/>
-      <c r="K50" s="128"/>
-    </row>
-    <row r="51" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J50" s="129"/>
+      <c r="K50" s="130"/>
+    </row>
+    <row r="51" spans="1:12" ht="13.5" thickBot="1"/>
+    <row r="52" spans="1:12">
       <c r="A52" s="50" t="s">
         <v>50</v>
       </c>
@@ -2385,7 +3442,7 @@
       </c>
       <c r="K52" s="65"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:12">
       <c r="A53" s="120"/>
       <c r="B53" s="32"/>
       <c r="C53" s="32"/>
@@ -2398,7 +3455,7 @@
       <c r="J53" s="32"/>
       <c r="K53" s="121"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:12">
       <c r="A54" s="18"/>
       <c r="B54" s="32"/>
       <c r="C54" s="32"/>
@@ -2411,7 +3468,7 @@
       <c r="J54" s="22"/>
       <c r="K54" s="122"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:12">
       <c r="A55" s="18"/>
       <c r="B55" s="32"/>
       <c r="C55" s="32"/>
@@ -2420,11 +3477,11 @@
       <c r="F55" s="32"/>
       <c r="G55" s="32"/>
       <c r="H55" s="22"/>
-      <c r="I55" s="133"/>
-      <c r="J55" s="133"/>
+      <c r="I55" s="124"/>
+      <c r="J55" s="124"/>
       <c r="K55" s="122"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:12">
       <c r="A56" s="18"/>
       <c r="B56" s="32"/>
       <c r="C56" s="32"/>
@@ -2433,11 +3490,11 @@
       <c r="F56" s="32"/>
       <c r="G56" s="32"/>
       <c r="H56" s="22"/>
-      <c r="I56" s="133"/>
-      <c r="J56" s="133"/>
+      <c r="I56" s="124"/>
+      <c r="J56" s="124"/>
       <c r="K56" s="122"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:12">
       <c r="A57" s="18"/>
       <c r="B57" s="32"/>
       <c r="C57" s="32"/>
@@ -2446,11 +3503,11 @@
       <c r="F57" s="32"/>
       <c r="G57" s="32"/>
       <c r="H57" s="22"/>
-      <c r="I57" s="133"/>
-      <c r="J57" s="133"/>
+      <c r="I57" s="124"/>
+      <c r="J57" s="124"/>
       <c r="K57" s="122"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:12">
       <c r="A58" s="18"/>
       <c r="B58" s="32"/>
       <c r="C58" s="32"/>
@@ -2459,11 +3516,11 @@
       <c r="F58" s="32"/>
       <c r="G58" s="32"/>
       <c r="H58" s="22"/>
-      <c r="I58" s="133"/>
-      <c r="J58" s="133"/>
+      <c r="I58" s="124"/>
+      <c r="J58" s="124"/>
       <c r="K58" s="122"/>
     </row>
-    <row r="59" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" ht="13.5" thickBot="1">
       <c r="A59" s="19"/>
       <c r="B59" s="20"/>
       <c r="C59" s="20"/>
@@ -2472,12 +3529,12 @@
       <c r="F59" s="20"/>
       <c r="G59" s="20"/>
       <c r="H59" s="81"/>
-      <c r="I59" s="134"/>
-      <c r="J59" s="134"/>
+      <c r="I59" s="125"/>
+      <c r="J59" s="125"/>
       <c r="K59" s="123"/>
       <c r="L59" s="32"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:12">
       <c r="A60" s="70" t="s">
         <v>93</v>
       </c>
@@ -2504,4 +3561,1121 @@
   </headerFooter>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U71"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56:XFD56"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="16" width="6.7109375" style="136" customWidth="1"/>
+    <col min="17" max="17" width="1.28515625" style="136" customWidth="1"/>
+    <col min="18" max="18" width="10.85546875" style="136"/>
+    <col min="19" max="16384" width="10.85546875" style="135"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="24.75" hidden="1" customHeight="1"/>
+    <row r="2" spans="1:18" ht="60.4" customHeight="1">
+      <c r="C2" s="209" t="s">
+        <v>178</v>
+      </c>
+      <c r="D2" s="208"/>
+      <c r="E2" s="208"/>
+      <c r="F2" s="208"/>
+      <c r="G2" s="208"/>
+      <c r="H2" s="208"/>
+      <c r="I2" s="208"/>
+      <c r="J2" s="208"/>
+      <c r="K2" s="208"/>
+      <c r="L2" s="208"/>
+      <c r="M2" s="208"/>
+      <c r="N2" s="207"/>
+      <c r="O2" s="200" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="18" customHeight="1">
+      <c r="O3" s="200"/>
+    </row>
+    <row r="4" spans="1:18" ht="18" customHeight="1">
+      <c r="A4" s="203" t="s">
+        <v>176</v>
+      </c>
+      <c r="B4" s="203"/>
+      <c r="C4" s="158"/>
+      <c r="D4" s="203" t="s">
+        <v>175</v>
+      </c>
+      <c r="E4" s="150"/>
+      <c r="F4" s="158"/>
+      <c r="G4" s="203" t="s">
+        <v>174</v>
+      </c>
+      <c r="H4" s="203"/>
+      <c r="I4" s="206"/>
+      <c r="J4" s="203" t="s">
+        <v>173</v>
+      </c>
+      <c r="K4" s="203"/>
+      <c r="L4" s="206"/>
+      <c r="M4" s="203"/>
+      <c r="N4" s="205" t="s">
+        <v>172</v>
+      </c>
+      <c r="O4" s="200"/>
+    </row>
+    <row r="5" spans="1:18" ht="18.95" customHeight="1">
+      <c r="A5" s="180"/>
+      <c r="B5" s="180"/>
+      <c r="C5" s="218"/>
+      <c r="D5" s="180"/>
+      <c r="E5" s="180"/>
+      <c r="F5" s="218"/>
+      <c r="G5" s="180"/>
+      <c r="H5" s="180"/>
+      <c r="I5" s="218"/>
+      <c r="J5" s="180"/>
+      <c r="K5" s="180"/>
+      <c r="L5" s="218"/>
+      <c r="M5" s="180"/>
+      <c r="N5" s="180"/>
+      <c r="O5" s="200"/>
+    </row>
+    <row r="6" spans="1:18" ht="18.95" customHeight="1">
+      <c r="A6" s="203" t="s">
+        <v>171</v>
+      </c>
+      <c r="B6" s="203"/>
+      <c r="C6" s="158"/>
+      <c r="D6" s="203" t="s">
+        <v>170</v>
+      </c>
+      <c r="E6" s="203"/>
+      <c r="F6" s="158"/>
+      <c r="G6" s="203" t="s">
+        <v>99</v>
+      </c>
+      <c r="H6" s="150"/>
+      <c r="I6" s="204"/>
+      <c r="J6" s="203" t="s">
+        <v>169</v>
+      </c>
+      <c r="K6" s="150"/>
+      <c r="L6" s="202"/>
+      <c r="M6" s="150"/>
+      <c r="N6" s="201" t="s">
+        <v>168</v>
+      </c>
+      <c r="O6" s="200"/>
+    </row>
+    <row r="7" spans="1:18" ht="18.95" customHeight="1">
+      <c r="A7" s="180"/>
+      <c r="B7" s="180"/>
+      <c r="C7" s="218"/>
+      <c r="D7" s="180"/>
+      <c r="E7" s="180"/>
+      <c r="F7" s="218" t="s">
+        <v>96</v>
+      </c>
+      <c r="G7" s="180"/>
+      <c r="H7" s="180"/>
+      <c r="I7" s="218" t="s">
+        <v>96</v>
+      </c>
+      <c r="J7" s="180"/>
+      <c r="K7" s="180"/>
+      <c r="L7" s="180"/>
+      <c r="M7" s="180"/>
+      <c r="N7" s="180"/>
+      <c r="O7" s="200"/>
+    </row>
+    <row r="8" spans="1:18" ht="6" customHeight="1"/>
+    <row r="9" spans="1:18" ht="15" customHeight="1">
+      <c r="A9" s="140" t="s">
+        <v>167</v>
+      </c>
+      <c r="B9" s="140"/>
+      <c r="C9" s="140"/>
+      <c r="D9" s="140"/>
+      <c r="E9" s="140"/>
+      <c r="F9" s="140"/>
+      <c r="G9" s="140"/>
+      <c r="H9" s="140"/>
+      <c r="I9" s="140"/>
+      <c r="J9" s="140"/>
+      <c r="K9" s="140"/>
+      <c r="L9" s="140"/>
+      <c r="M9" s="140"/>
+      <c r="N9" s="140"/>
+      <c r="O9" s="140"/>
+      <c r="P9" s="140"/>
+    </row>
+    <row r="10" spans="1:18" ht="5.25" customHeight="1"/>
+    <row r="11" spans="1:18" s="157" customFormat="1">
+      <c r="A11" s="150" t="s">
+        <v>166</v>
+      </c>
+      <c r="B11" s="150"/>
+      <c r="C11" s="150" t="s">
+        <v>165</v>
+      </c>
+      <c r="D11" s="150"/>
+      <c r="E11" s="150" t="s">
+        <v>164</v>
+      </c>
+      <c r="F11" s="150"/>
+      <c r="G11" s="150" t="s">
+        <v>163</v>
+      </c>
+      <c r="H11" s="150"/>
+      <c r="I11" s="199"/>
+      <c r="J11" s="156" t="s">
+        <v>162</v>
+      </c>
+      <c r="K11" s="156" t="s">
+        <v>161</v>
+      </c>
+      <c r="L11" s="156" t="s">
+        <v>160</v>
+      </c>
+      <c r="M11" s="156" t="s">
+        <v>159</v>
+      </c>
+      <c r="N11" s="156" t="s">
+        <v>158</v>
+      </c>
+      <c r="O11" s="156" t="s">
+        <v>157</v>
+      </c>
+      <c r="P11" s="155" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q11" s="138"/>
+      <c r="R11" s="138"/>
+    </row>
+    <row r="12" spans="1:18" ht="14.25">
+      <c r="A12" s="180"/>
+      <c r="B12" s="180"/>
+      <c r="C12" s="180"/>
+      <c r="D12" s="180"/>
+      <c r="E12" s="180"/>
+      <c r="F12" s="180"/>
+      <c r="G12" s="160" t="s">
+        <v>57</v>
+      </c>
+      <c r="H12" s="149"/>
+      <c r="I12" s="198" t="s">
+        <v>123</v>
+      </c>
+      <c r="J12" s="196" t="s">
+        <v>96</v>
+      </c>
+      <c r="K12" s="196" t="s">
+        <v>96</v>
+      </c>
+      <c r="L12" s="196" t="s">
+        <v>96</v>
+      </c>
+      <c r="M12" s="196" t="s">
+        <v>96</v>
+      </c>
+      <c r="N12" s="196" t="s">
+        <v>96</v>
+      </c>
+      <c r="O12" s="196" t="s">
+        <v>96</v>
+      </c>
+      <c r="P12" s="195" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" s="157" customFormat="1">
+      <c r="A13" s="150" t="s">
+        <v>155</v>
+      </c>
+      <c r="B13" s="150"/>
+      <c r="C13" s="150" t="s">
+        <v>154</v>
+      </c>
+      <c r="D13" s="150"/>
+      <c r="E13" s="150" t="s">
+        <v>153</v>
+      </c>
+      <c r="F13" s="150"/>
+      <c r="G13" s="150"/>
+      <c r="H13" s="150"/>
+      <c r="I13" s="197" t="s">
+        <v>152</v>
+      </c>
+      <c r="J13" s="196" t="s">
+        <v>96</v>
+      </c>
+      <c r="K13" s="196" t="s">
+        <v>96</v>
+      </c>
+      <c r="L13" s="196" t="s">
+        <v>96</v>
+      </c>
+      <c r="M13" s="196" t="s">
+        <v>96</v>
+      </c>
+      <c r="N13" s="196" t="s">
+        <v>96</v>
+      </c>
+      <c r="O13" s="196" t="s">
+        <v>96</v>
+      </c>
+      <c r="P13" s="195" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q13" s="138"/>
+      <c r="R13" s="138"/>
+    </row>
+    <row r="14" spans="1:18" ht="14.25">
+      <c r="A14" s="180"/>
+      <c r="B14" s="180"/>
+      <c r="C14" s="180"/>
+      <c r="D14" s="180"/>
+      <c r="E14" s="180"/>
+      <c r="F14" s="180"/>
+      <c r="G14" s="180"/>
+      <c r="H14" s="180"/>
+      <c r="I14" s="194" t="s">
+        <v>151</v>
+      </c>
+      <c r="J14" s="193" t="s">
+        <v>96</v>
+      </c>
+      <c r="K14" s="193" t="s">
+        <v>96</v>
+      </c>
+      <c r="L14" s="193" t="s">
+        <v>96</v>
+      </c>
+      <c r="M14" s="193" t="s">
+        <v>96</v>
+      </c>
+      <c r="N14" s="193" t="s">
+        <v>96</v>
+      </c>
+      <c r="O14" s="193" t="s">
+        <v>96</v>
+      </c>
+      <c r="P14" s="192"/>
+    </row>
+    <row r="15" spans="1:18" ht="6" customHeight="1">
+      <c r="A15" s="191"/>
+    </row>
+    <row r="16" spans="1:18" ht="15" customHeight="1">
+      <c r="A16" s="141" t="s">
+        <v>150</v>
+      </c>
+      <c r="B16" s="140"/>
+      <c r="C16" s="140"/>
+      <c r="D16" s="140"/>
+      <c r="E16" s="140"/>
+      <c r="F16" s="140"/>
+      <c r="G16" s="140"/>
+      <c r="H16" s="140"/>
+      <c r="I16" s="140"/>
+      <c r="J16" s="140"/>
+      <c r="K16" s="140"/>
+      <c r="L16" s="140"/>
+      <c r="M16" s="140"/>
+      <c r="N16" s="140"/>
+      <c r="O16" s="140"/>
+      <c r="P16" s="140"/>
+    </row>
+    <row r="17" spans="1:21" ht="5.25" customHeight="1">
+      <c r="K17" s="182"/>
+      <c r="L17" s="182"/>
+      <c r="M17" s="182"/>
+      <c r="N17" s="182"/>
+    </row>
+    <row r="18" spans="1:21" s="157" customFormat="1">
+      <c r="A18" s="150" t="s">
+        <v>149</v>
+      </c>
+      <c r="B18" s="150"/>
+      <c r="C18" s="150" t="s">
+        <v>148</v>
+      </c>
+      <c r="D18" s="150"/>
+      <c r="E18" s="150" t="s">
+        <v>147</v>
+      </c>
+      <c r="F18" s="150"/>
+      <c r="G18" s="150" t="s">
+        <v>146</v>
+      </c>
+      <c r="H18" s="150"/>
+      <c r="I18" s="150" t="s">
+        <v>145</v>
+      </c>
+      <c r="J18" s="150"/>
+      <c r="K18" s="150" t="s">
+        <v>144</v>
+      </c>
+      <c r="L18" s="150"/>
+      <c r="M18" s="150" t="s">
+        <v>143</v>
+      </c>
+      <c r="N18" s="150"/>
+      <c r="O18" s="150" t="s">
+        <v>142</v>
+      </c>
+      <c r="P18" s="150"/>
+      <c r="Q18" s="138"/>
+    </row>
+    <row r="19" spans="1:21" ht="12.75" customHeight="1">
+      <c r="A19" s="180"/>
+      <c r="B19" s="180"/>
+      <c r="C19" s="180"/>
+      <c r="D19" s="180"/>
+      <c r="E19" s="180"/>
+      <c r="F19" s="180"/>
+      <c r="G19" s="180"/>
+      <c r="H19" s="180"/>
+      <c r="I19" s="180"/>
+      <c r="J19" s="180"/>
+      <c r="K19" s="180"/>
+      <c r="L19" s="180"/>
+      <c r="M19" s="180"/>
+      <c r="N19" s="180"/>
+      <c r="O19" s="180"/>
+      <c r="P19" s="180"/>
+      <c r="R19" s="135"/>
+    </row>
+    <row r="20" spans="1:21" hidden="1">
+      <c r="A20" s="149"/>
+      <c r="B20" s="149"/>
+      <c r="C20" s="149"/>
+      <c r="D20" s="149"/>
+      <c r="E20" s="150" t="s">
+        <v>112</v>
+      </c>
+      <c r="F20" s="150"/>
+      <c r="G20" s="150"/>
+      <c r="H20" s="150"/>
+      <c r="I20" s="158"/>
+      <c r="J20" s="149"/>
+      <c r="K20" s="149"/>
+      <c r="L20" s="149"/>
+      <c r="M20" s="190"/>
+      <c r="N20" s="149"/>
+      <c r="O20" s="149"/>
+      <c r="P20" s="149"/>
+      <c r="R20" s="149" t="s">
+        <v>96</v>
+      </c>
+      <c r="S20" s="149"/>
+      <c r="T20" s="149" t="s">
+        <v>96</v>
+      </c>
+      <c r="U20" s="149"/>
+    </row>
+    <row r="21" spans="1:21" s="157" customFormat="1">
+      <c r="A21" s="150"/>
+      <c r="B21" s="189" t="s">
+        <v>97</v>
+      </c>
+      <c r="C21" s="150" t="s">
+        <v>141</v>
+      </c>
+      <c r="D21" s="150"/>
+      <c r="E21" s="150" t="s">
+        <v>111</v>
+      </c>
+      <c r="F21" s="150"/>
+      <c r="G21" s="150" t="s">
+        <v>110</v>
+      </c>
+      <c r="H21" s="150"/>
+      <c r="I21" s="188"/>
+      <c r="J21" s="187" t="s">
+        <v>180</v>
+      </c>
+      <c r="K21" s="150" t="s">
+        <v>53</v>
+      </c>
+      <c r="L21" s="150"/>
+      <c r="M21" s="150" t="s">
+        <v>54</v>
+      </c>
+      <c r="N21" s="150"/>
+      <c r="O21" s="150" t="s">
+        <v>140</v>
+      </c>
+      <c r="P21" s="150"/>
+      <c r="Q21" s="138"/>
+      <c r="R21" s="138"/>
+    </row>
+    <row r="22" spans="1:21">
+      <c r="A22" s="186" t="s">
+        <v>139</v>
+      </c>
+      <c r="B22" s="185" t="s">
+        <v>96</v>
+      </c>
+      <c r="C22" s="184" t="s">
+        <v>96</v>
+      </c>
+      <c r="D22" s="184"/>
+      <c r="E22" s="180"/>
+      <c r="F22" s="180"/>
+      <c r="G22" s="183"/>
+      <c r="H22" s="180"/>
+      <c r="I22" s="182" t="s">
+        <v>96</v>
+      </c>
+      <c r="J22" s="181" t="s">
+        <v>138</v>
+      </c>
+      <c r="K22" s="180" t="s">
+        <v>96</v>
+      </c>
+      <c r="L22" s="180"/>
+      <c r="M22" s="180" t="s">
+        <v>96</v>
+      </c>
+      <c r="N22" s="180"/>
+      <c r="O22" s="180" t="s">
+        <v>96</v>
+      </c>
+      <c r="P22" s="180"/>
+    </row>
+    <row r="23" spans="1:21" ht="15.75">
+      <c r="A23" s="147" t="s">
+        <v>137</v>
+      </c>
+      <c r="B23" s="179" t="s">
+        <v>96</v>
+      </c>
+      <c r="C23" s="175" t="s">
+        <v>96</v>
+      </c>
+      <c r="D23" s="175"/>
+      <c r="E23" s="178" t="s">
+        <v>136</v>
+      </c>
+      <c r="F23" s="178"/>
+      <c r="G23" s="177"/>
+      <c r="H23" s="178"/>
+      <c r="I23" s="177"/>
+      <c r="J23" s="176" t="s">
+        <v>135</v>
+      </c>
+      <c r="K23" s="175" t="s">
+        <v>96</v>
+      </c>
+      <c r="L23" s="175"/>
+      <c r="M23" s="175" t="s">
+        <v>96</v>
+      </c>
+      <c r="N23" s="175"/>
+      <c r="O23" s="175" t="s">
+        <v>96</v>
+      </c>
+      <c r="P23" s="175"/>
+    </row>
+    <row r="24" spans="1:21" ht="5.25" customHeight="1">
+      <c r="A24" s="153"/>
+      <c r="B24" s="152"/>
+      <c r="C24" s="152"/>
+      <c r="D24" s="152"/>
+      <c r="E24" s="152"/>
+      <c r="F24" s="152"/>
+      <c r="G24" s="152"/>
+      <c r="H24" s="152"/>
+      <c r="I24" s="152"/>
+      <c r="J24" s="152"/>
+      <c r="K24" s="151"/>
+      <c r="L24" s="151"/>
+      <c r="M24" s="151"/>
+      <c r="N24" s="151"/>
+      <c r="O24" s="151"/>
+      <c r="P24" s="151"/>
+    </row>
+    <row r="25" spans="1:21">
+      <c r="A25" s="153" t="s">
+        <v>134</v>
+      </c>
+      <c r="B25" s="153"/>
+      <c r="C25" s="153" t="s">
+        <v>133</v>
+      </c>
+      <c r="D25" s="174"/>
+      <c r="E25" s="153" t="s">
+        <v>132</v>
+      </c>
+      <c r="F25" s="153"/>
+      <c r="G25" s="174"/>
+      <c r="H25" s="173" t="s">
+        <v>131</v>
+      </c>
+      <c r="I25" s="173"/>
+      <c r="J25" s="150" t="s">
+        <v>81</v>
+      </c>
+      <c r="K25" s="150"/>
+      <c r="L25" s="153" t="s">
+        <v>130</v>
+      </c>
+      <c r="M25" s="153"/>
+      <c r="N25" s="153"/>
+      <c r="O25" s="153"/>
+      <c r="P25" s="153"/>
+    </row>
+    <row r="26" spans="1:21">
+      <c r="A26" s="153" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="160" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="148" t="s">
+        <v>96</v>
+      </c>
+      <c r="D26" s="148" t="s">
+        <v>96</v>
+      </c>
+      <c r="E26" s="148" t="s">
+        <v>96</v>
+      </c>
+      <c r="F26" s="148"/>
+      <c r="G26" s="148"/>
+      <c r="H26" s="148" t="s">
+        <v>96</v>
+      </c>
+      <c r="I26" s="148"/>
+      <c r="J26" s="148" t="s">
+        <v>96</v>
+      </c>
+      <c r="K26" s="148"/>
+      <c r="L26" s="153" t="s">
+        <v>108</v>
+      </c>
+      <c r="M26" s="153"/>
+      <c r="N26" s="154" t="s">
+        <v>107</v>
+      </c>
+      <c r="O26" s="153" t="s">
+        <v>106</v>
+      </c>
+      <c r="P26" s="153"/>
+    </row>
+    <row r="27" spans="1:21">
+      <c r="A27" s="153" t="s">
+        <v>129</v>
+      </c>
+      <c r="B27" s="160" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="172"/>
+      <c r="D27" s="172"/>
+      <c r="E27" s="172"/>
+      <c r="F27" s="172"/>
+      <c r="G27" s="172"/>
+      <c r="H27" s="172"/>
+      <c r="I27" s="172"/>
+      <c r="J27" s="171"/>
+      <c r="K27" s="171"/>
+      <c r="L27" s="148" t="s">
+        <v>96</v>
+      </c>
+      <c r="M27" s="148" t="s">
+        <v>96</v>
+      </c>
+      <c r="N27" s="148" t="s">
+        <v>96</v>
+      </c>
+      <c r="O27" s="148"/>
+      <c r="P27" s="170"/>
+    </row>
+    <row r="28" spans="1:21" ht="6" customHeight="1"/>
+    <row r="29" spans="1:21" ht="15.75">
+      <c r="A29" s="141" t="s">
+        <v>128</v>
+      </c>
+      <c r="B29" s="140"/>
+      <c r="C29" s="140"/>
+      <c r="D29" s="140"/>
+      <c r="E29" s="140"/>
+      <c r="F29" s="140"/>
+      <c r="G29" s="140"/>
+      <c r="H29" s="140"/>
+      <c r="I29" s="140"/>
+      <c r="J29" s="140"/>
+      <c r="K29" s="140"/>
+      <c r="L29" s="140"/>
+      <c r="M29" s="140"/>
+      <c r="N29" s="140"/>
+      <c r="O29" s="140"/>
+      <c r="P29" s="140"/>
+    </row>
+    <row r="30" spans="1:21" ht="5.25" customHeight="1">
+      <c r="K30" s="158"/>
+      <c r="L30" s="158"/>
+      <c r="M30" s="158"/>
+      <c r="N30" s="158"/>
+      <c r="O30" s="158"/>
+      <c r="P30" s="158"/>
+    </row>
+    <row r="31" spans="1:21" ht="14.25">
+      <c r="A31" s="169" t="s">
+        <v>127</v>
+      </c>
+      <c r="B31" s="156" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" s="156" t="s">
+        <v>54</v>
+      </c>
+      <c r="F31" s="153" t="s">
+        <v>126</v>
+      </c>
+      <c r="G31" s="153"/>
+      <c r="H31" s="153"/>
+      <c r="I31" s="158"/>
+      <c r="K31" s="150" t="s">
+        <v>125</v>
+      </c>
+      <c r="L31" s="150"/>
+      <c r="M31" s="150" t="s">
+        <v>60</v>
+      </c>
+      <c r="N31" s="150"/>
+      <c r="O31" s="150" t="s">
+        <v>124</v>
+      </c>
+      <c r="P31" s="150"/>
+    </row>
+    <row r="32" spans="1:21">
+      <c r="A32" s="165" t="s">
+        <v>123</v>
+      </c>
+      <c r="B32" s="168" t="s">
+        <v>96</v>
+      </c>
+      <c r="C32" s="168" t="s">
+        <v>96</v>
+      </c>
+      <c r="D32" s="219" t="s">
+        <v>122</v>
+      </c>
+      <c r="F32" s="167" t="s">
+        <v>121</v>
+      </c>
+      <c r="G32" s="150"/>
+      <c r="H32" s="166" t="s">
+        <v>120</v>
+      </c>
+      <c r="I32" s="158"/>
+      <c r="K32" s="160" t="s">
+        <v>57</v>
+      </c>
+      <c r="L32" s="149"/>
+      <c r="M32" s="160" t="s">
+        <v>57</v>
+      </c>
+      <c r="N32" s="149"/>
+      <c r="O32" s="160" t="s">
+        <v>57</v>
+      </c>
+      <c r="P32" s="149"/>
+    </row>
+    <row r="33" spans="1:18" ht="14.25" customHeight="1">
+      <c r="A33" s="165" t="s">
+        <v>109</v>
+      </c>
+      <c r="B33" s="162" t="s">
+        <v>96</v>
+      </c>
+      <c r="C33" s="162" t="s">
+        <v>96</v>
+      </c>
+      <c r="D33" s="164" t="s">
+        <v>19</v>
+      </c>
+      <c r="F33" s="148"/>
+      <c r="G33" s="148" t="s">
+        <v>119</v>
+      </c>
+      <c r="H33" s="148" t="s">
+        <v>96</v>
+      </c>
+      <c r="K33" s="150" t="s">
+        <v>118</v>
+      </c>
+      <c r="L33" s="150"/>
+      <c r="M33" s="150" t="s">
+        <v>88</v>
+      </c>
+      <c r="N33" s="150"/>
+      <c r="O33" s="150" t="s">
+        <v>117</v>
+      </c>
+      <c r="P33" s="150"/>
+    </row>
+    <row r="34" spans="1:18">
+      <c r="A34" s="163" t="s">
+        <v>116</v>
+      </c>
+      <c r="B34" s="162" t="s">
+        <v>96</v>
+      </c>
+      <c r="C34" s="162" t="s">
+        <v>96</v>
+      </c>
+      <c r="D34" s="161" t="s">
+        <v>115</v>
+      </c>
+      <c r="E34" s="138"/>
+      <c r="K34" s="160" t="s">
+        <v>57</v>
+      </c>
+      <c r="L34" s="149"/>
+      <c r="M34" s="160" t="s">
+        <v>57</v>
+      </c>
+      <c r="N34" s="149"/>
+      <c r="O34" s="160" t="s">
+        <v>57</v>
+      </c>
+      <c r="P34" s="149"/>
+    </row>
+    <row r="35" spans="1:18" ht="6" customHeight="1">
+      <c r="A35" s="138"/>
+      <c r="C35" s="138"/>
+    </row>
+    <row r="36" spans="1:18" ht="15.75">
+      <c r="A36" s="141" t="s">
+        <v>179</v>
+      </c>
+      <c r="B36" s="140"/>
+      <c r="C36" s="140"/>
+      <c r="D36" s="140"/>
+      <c r="E36" s="140"/>
+      <c r="F36" s="140"/>
+      <c r="G36" s="140"/>
+      <c r="H36" s="140"/>
+      <c r="I36" s="140"/>
+      <c r="J36" s="140"/>
+      <c r="K36" s="140"/>
+      <c r="L36" s="140"/>
+      <c r="M36" s="140"/>
+      <c r="N36" s="140"/>
+      <c r="O36" s="140"/>
+      <c r="P36" s="140"/>
+    </row>
+    <row r="37" spans="1:18" ht="5.25" customHeight="1"/>
+    <row r="38" spans="1:18" s="157" customFormat="1">
+      <c r="A38" s="159" t="s">
+        <v>114</v>
+      </c>
+      <c r="B38" s="150"/>
+      <c r="C38" s="158"/>
+      <c r="D38" s="150" t="s">
+        <v>113</v>
+      </c>
+      <c r="E38" s="158"/>
+      <c r="F38" s="150" t="s">
+        <v>5</v>
+      </c>
+      <c r="G38" s="150"/>
+      <c r="H38" s="150" t="s">
+        <v>99</v>
+      </c>
+      <c r="I38" s="150"/>
+      <c r="K38" s="136"/>
+      <c r="L38" s="136"/>
+      <c r="M38" s="187"/>
+      <c r="N38" s="217"/>
+      <c r="O38" s="217"/>
+      <c r="P38" s="217"/>
+      <c r="Q38" s="138"/>
+      <c r="R38" s="138"/>
+    </row>
+    <row r="39" spans="1:18">
+      <c r="A39" s="149" t="s">
+        <v>96</v>
+      </c>
+      <c r="B39" s="149"/>
+      <c r="C39" s="149" t="s">
+        <v>96</v>
+      </c>
+      <c r="D39" s="149"/>
+      <c r="E39" s="149"/>
+      <c r="F39" s="148" t="s">
+        <v>96</v>
+      </c>
+      <c r="G39" s="148"/>
+      <c r="H39" s="148" t="s">
+        <v>96</v>
+      </c>
+      <c r="I39" s="148"/>
+      <c r="M39" s="215"/>
+      <c r="N39" s="216" t="s">
+        <v>96</v>
+      </c>
+      <c r="O39" s="216" t="s">
+        <v>96</v>
+      </c>
+      <c r="P39" s="216" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18">
+      <c r="A40" s="210"/>
+      <c r="B40" s="211"/>
+      <c r="C40" s="153"/>
+      <c r="D40" s="153"/>
+      <c r="E40" s="153"/>
+      <c r="F40" s="153"/>
+      <c r="G40" s="151"/>
+      <c r="M40" s="215"/>
+      <c r="N40" s="216" t="s">
+        <v>96</v>
+      </c>
+      <c r="O40" s="216" t="s">
+        <v>96</v>
+      </c>
+      <c r="P40" s="216" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18">
+      <c r="A41" s="210"/>
+      <c r="B41" s="211"/>
+      <c r="C41" s="153"/>
+      <c r="D41" s="153"/>
+      <c r="E41" s="153"/>
+      <c r="F41" s="153"/>
+      <c r="G41" s="151"/>
+      <c r="M41" s="215"/>
+      <c r="N41" s="216" t="s">
+        <v>96</v>
+      </c>
+      <c r="O41" s="216" t="s">
+        <v>96</v>
+      </c>
+      <c r="P41" s="216" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" ht="14.25">
+      <c r="A42" s="212"/>
+      <c r="B42" s="213"/>
+      <c r="C42" s="214"/>
+      <c r="D42" s="214"/>
+      <c r="E42" s="214"/>
+      <c r="F42" s="214"/>
+      <c r="G42" s="151"/>
+      <c r="M42" s="215"/>
+      <c r="N42" s="216" t="s">
+        <v>96</v>
+      </c>
+      <c r="O42" s="216" t="s">
+        <v>96</v>
+      </c>
+      <c r="P42" s="216" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" ht="14.25">
+      <c r="A43" s="212"/>
+      <c r="B43" s="213"/>
+      <c r="C43" s="214"/>
+      <c r="D43" s="214"/>
+      <c r="E43" s="214"/>
+      <c r="F43" s="214"/>
+      <c r="G43" s="151"/>
+      <c r="H43" s="142"/>
+      <c r="I43" s="142"/>
+      <c r="M43" s="215"/>
+      <c r="N43" s="216" t="s">
+        <v>96</v>
+      </c>
+      <c r="O43" s="216" t="s">
+        <v>96</v>
+      </c>
+      <c r="P43" s="216" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" ht="6" customHeight="1"/>
+    <row r="45" spans="1:18" ht="15.75">
+      <c r="A45" s="141" t="s">
+        <v>105</v>
+      </c>
+      <c r="B45" s="140"/>
+      <c r="C45" s="140"/>
+      <c r="D45" s="140"/>
+      <c r="E45" s="140"/>
+      <c r="F45" s="140"/>
+      <c r="G45" s="140"/>
+      <c r="H45" s="140"/>
+      <c r="I45" s="140"/>
+      <c r="J45" s="140"/>
+      <c r="K45" s="140"/>
+      <c r="L45" s="140"/>
+      <c r="M45" s="140"/>
+      <c r="N45" s="140"/>
+      <c r="O45" s="140"/>
+      <c r="P45" s="140"/>
+    </row>
+    <row r="46" spans="1:18" ht="5.25" customHeight="1"/>
+    <row r="47" spans="1:18">
+      <c r="A47" s="150" t="s">
+        <v>104</v>
+      </c>
+      <c r="B47" s="150"/>
+      <c r="C47" s="150" t="s">
+        <v>103</v>
+      </c>
+      <c r="D47" s="150"/>
+      <c r="E47" s="150" t="s">
+        <v>102</v>
+      </c>
+      <c r="F47" s="150"/>
+      <c r="G47" s="150" t="s">
+        <v>101</v>
+      </c>
+      <c r="H47" s="150"/>
+      <c r="I47" s="150" t="s">
+        <v>100</v>
+      </c>
+      <c r="J47" s="150"/>
+      <c r="K47" s="150" t="s">
+        <v>5</v>
+      </c>
+      <c r="L47" s="150"/>
+      <c r="M47" s="150" t="s">
+        <v>99</v>
+      </c>
+      <c r="N47" s="150"/>
+      <c r="O47" s="150" t="s">
+        <v>98</v>
+      </c>
+      <c r="P47" s="150"/>
+    </row>
+    <row r="48" spans="1:18">
+      <c r="A48" s="149"/>
+      <c r="B48" s="149"/>
+      <c r="C48" s="148" t="s">
+        <v>96</v>
+      </c>
+      <c r="D48" s="148"/>
+      <c r="E48" s="148" t="s">
+        <v>96</v>
+      </c>
+      <c r="F48" s="148"/>
+      <c r="G48" s="148" t="s">
+        <v>96</v>
+      </c>
+      <c r="H48" s="148"/>
+      <c r="I48" s="148" t="s">
+        <v>96</v>
+      </c>
+      <c r="J48" s="148"/>
+      <c r="K48" s="148" t="s">
+        <v>96</v>
+      </c>
+      <c r="L48" s="148"/>
+      <c r="M48" s="148" t="s">
+        <v>96</v>
+      </c>
+      <c r="N48" s="148"/>
+      <c r="O48" s="148" t="s">
+        <v>96</v>
+      </c>
+      <c r="P48" s="148"/>
+    </row>
+    <row r="49" spans="1:16">
+      <c r="B49" s="147" t="s">
+        <v>97</v>
+      </c>
+      <c r="C49" s="146" t="s">
+        <v>96</v>
+      </c>
+      <c r="D49" s="143"/>
+      <c r="E49" s="143" t="s">
+        <v>96</v>
+      </c>
+      <c r="F49" s="143"/>
+      <c r="G49" s="145" t="s">
+        <v>96</v>
+      </c>
+      <c r="H49" s="145"/>
+      <c r="I49" s="145" t="s">
+        <v>96</v>
+      </c>
+      <c r="J49" s="145"/>
+      <c r="K49" s="144"/>
+      <c r="L49" s="143"/>
+      <c r="M49" s="142"/>
+      <c r="N49" s="142"/>
+      <c r="O49" s="142"/>
+      <c r="P49" s="142"/>
+    </row>
+    <row r="50" spans="1:16" ht="5.25" customHeight="1">
+      <c r="K50" s="138"/>
+    </row>
+    <row r="51" spans="1:16" ht="15.75">
+      <c r="A51" s="141" t="s">
+        <v>95</v>
+      </c>
+      <c r="B51" s="140"/>
+      <c r="C51" s="140"/>
+      <c r="D51" s="140"/>
+      <c r="E51" s="140"/>
+      <c r="F51" s="140"/>
+      <c r="G51" s="140"/>
+      <c r="H51" s="140"/>
+      <c r="I51" s="140"/>
+      <c r="J51" s="140"/>
+      <c r="K51" s="140"/>
+      <c r="L51" s="140"/>
+      <c r="M51" s="140"/>
+      <c r="N51" s="140"/>
+      <c r="O51" s="140"/>
+      <c r="P51" s="140"/>
+    </row>
+    <row r="52" spans="1:16" ht="5.25" customHeight="1"/>
+    <row r="53" spans="1:16">
+      <c r="A53" s="139"/>
+    </row>
+    <row r="55" spans="1:16">
+      <c r="A55" s="138"/>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" s="137"/>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" s="137" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" s="137"/>
+    </row>
+  </sheetData>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <mergeCells count="1">
+    <mergeCell ref="O2:O7"/>
+  </mergeCells>
+  <pageMargins left="0.62992125984252001" right="0.23622047244093999" top="0.35433070866142002" bottom="0.55118110236219997" header="0.11811023622047" footer="0.31496062992126"/>
+  <pageSetup paperSize="9" scale="89" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;K04-044M&amp;"Arial,Normal"&amp;8ETCUT RECHERCHES S.A.S.
+22 rue du Moulin de la Garde – 44477 CARQUEFOU Cedex  (Nantes) FRANCE – Tel. +33 240 252 507 – www.metcutfrance.com
+S.A.S. au capital de 206 250€ - VAT FR10388107443 000 11</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix bug $def sur new FT
</commit_message>
<xml_diff>
--- a/lib/PHPExcel/templates/FT Loa.xlsx
+++ b/lib/PHPExcel/templates/FT Loa.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="181">
   <si>
     <t>DONNEES EPROUVETTE</t>
   </si>
@@ -854,6 +854,7 @@
       <sz val="10"/>
       <color rgb="FF223962"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -872,6 +873,7 @@
       <sz val="12"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -995,6 +997,7 @@
       <sz val="10"/>
       <color rgb="FF8E98A5"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -1018,6 +1021,7 @@
       <sz val="14"/>
       <color rgb="FF44546A"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1490,7 +1494,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="220">
+  <cellXfs count="219">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -1775,31 +1779,6 @@
     <xf numFmtId="168" fontId="3" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1965,9 +1944,6 @@
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="36" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -2015,11 +1991,36 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2669,20 +2670,20 @@
     </row>
     <row r="4" spans="1:14" ht="13.5" thickBot="1"/>
     <row r="5" spans="1:14" ht="13.5" thickBot="1">
-      <c r="A5" s="126" t="s">
+      <c r="A5" s="209" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="127"/>
-      <c r="C5" s="127"/>
-      <c r="D5" s="127"/>
-      <c r="E5" s="127"/>
-      <c r="F5" s="128"/>
-      <c r="H5" s="126" t="s">
+      <c r="B5" s="210"/>
+      <c r="C5" s="210"/>
+      <c r="D5" s="210"/>
+      <c r="E5" s="210"/>
+      <c r="F5" s="211"/>
+      <c r="H5" s="209" t="s">
         <v>1</v>
       </c>
-      <c r="I5" s="127"/>
-      <c r="J5" s="127"/>
-      <c r="K5" s="128"/>
+      <c r="I5" s="210"/>
+      <c r="J5" s="210"/>
+      <c r="K5" s="211"/>
     </row>
     <row r="6" spans="1:14" ht="6.75" customHeight="1">
       <c r="A6" s="12"/>
@@ -2769,13 +2770,13 @@
       <c r="K11" s="60"/>
     </row>
     <row r="12" spans="1:14" ht="13.5" thickBot="1">
-      <c r="A12" s="126" t="s">
+      <c r="A12" s="209" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="127"/>
-      <c r="C12" s="127"/>
-      <c r="D12" s="127"/>
-      <c r="E12" s="127"/>
+      <c r="B12" s="210"/>
+      <c r="C12" s="210"/>
+      <c r="D12" s="210"/>
+      <c r="E12" s="210"/>
       <c r="F12" s="23"/>
       <c r="H12" s="18" t="s">
         <v>8</v>
@@ -2842,12 +2843,12 @@
       </c>
       <c r="E16" s="24"/>
       <c r="F16" s="62"/>
-      <c r="H16" s="126" t="s">
+      <c r="H16" s="209" t="s">
         <v>15</v>
       </c>
-      <c r="I16" s="127"/>
-      <c r="J16" s="127"/>
-      <c r="K16" s="128"/>
+      <c r="I16" s="210"/>
+      <c r="J16" s="210"/>
+      <c r="K16" s="211"/>
       <c r="N16" s="24"/>
     </row>
     <row r="17" spans="1:14">
@@ -2908,14 +2909,14 @@
       <c r="K20" s="86"/>
     </row>
     <row r="21" spans="1:14" ht="13.5" thickBot="1">
-      <c r="A21" s="126" t="s">
+      <c r="A21" s="209" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="127"/>
-      <c r="C21" s="127"/>
-      <c r="D21" s="127"/>
-      <c r="E21" s="127"/>
-      <c r="F21" s="128"/>
+      <c r="B21" s="210"/>
+      <c r="C21" s="210"/>
+      <c r="D21" s="210"/>
+      <c r="E21" s="210"/>
+      <c r="F21" s="211"/>
       <c r="H21" s="6"/>
       <c r="I21" s="87"/>
       <c r="J21" s="53" t="s">
@@ -3132,10 +3133,10 @@
       <c r="K33" s="114"/>
     </row>
     <row r="34" spans="1:19" ht="13.5" thickBot="1">
-      <c r="A34" s="131" t="s">
+      <c r="A34" s="214" t="s">
         <v>67</v>
       </c>
-      <c r="B34" s="132"/>
+      <c r="B34" s="215"/>
       <c r="C34" s="35"/>
       <c r="D34" s="55" t="s">
         <v>65</v>
@@ -3234,19 +3235,19 @@
       <c r="O39" s="32"/>
     </row>
     <row r="40" spans="1:19" ht="13.5" thickBot="1">
-      <c r="A40" s="126" t="s">
+      <c r="A40" s="209" t="s">
         <v>42</v>
       </c>
-      <c r="B40" s="127"/>
-      <c r="C40" s="127"/>
-      <c r="D40" s="127"/>
-      <c r="E40" s="127"/>
-      <c r="F40" s="127"/>
-      <c r="G40" s="127"/>
-      <c r="H40" s="127"/>
-      <c r="I40" s="127"/>
-      <c r="J40" s="127"/>
-      <c r="K40" s="128"/>
+      <c r="B40" s="210"/>
+      <c r="C40" s="210"/>
+      <c r="D40" s="210"/>
+      <c r="E40" s="210"/>
+      <c r="F40" s="210"/>
+      <c r="G40" s="210"/>
+      <c r="H40" s="210"/>
+      <c r="I40" s="210"/>
+      <c r="J40" s="210"/>
+      <c r="K40" s="211"/>
       <c r="M40" s="32"/>
       <c r="N40" s="32"/>
       <c r="O40" s="32"/>
@@ -3309,21 +3310,21 @@
       <c r="S43" s="32"/>
     </row>
     <row r="44" spans="1:19" ht="13.5" thickBot="1">
-      <c r="A44" s="126" t="s">
+      <c r="A44" s="209" t="s">
         <v>43</v>
       </c>
-      <c r="B44" s="127"/>
-      <c r="C44" s="127"/>
-      <c r="D44" s="127"/>
-      <c r="E44" s="127"/>
-      <c r="F44" s="127"/>
-      <c r="G44" s="127"/>
-      <c r="H44" s="127"/>
-      <c r="I44" s="128"/>
-      <c r="J44" s="133" t="s">
+      <c r="B44" s="210"/>
+      <c r="C44" s="210"/>
+      <c r="D44" s="210"/>
+      <c r="E44" s="210"/>
+      <c r="F44" s="210"/>
+      <c r="G44" s="210"/>
+      <c r="H44" s="210"/>
+      <c r="I44" s="211"/>
+      <c r="J44" s="216" t="s">
         <v>87</v>
       </c>
-      <c r="K44" s="134"/>
+      <c r="K44" s="217"/>
     </row>
     <row r="45" spans="1:19">
       <c r="A45" s="18" t="s">
@@ -3419,8 +3420,8 @@
       <c r="G50" s="20"/>
       <c r="H50" s="20"/>
       <c r="I50" s="20"/>
-      <c r="J50" s="129"/>
-      <c r="K50" s="130"/>
+      <c r="J50" s="212"/>
+      <c r="K50" s="213"/>
     </row>
     <row r="51" spans="1:12" ht="13.5" thickBot="1"/>
     <row r="52" spans="1:12">
@@ -3567,1102 +3568,1114 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56:XFD56"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="16" width="6.7109375" style="136" customWidth="1"/>
-    <col min="17" max="17" width="1.28515625" style="136" customWidth="1"/>
-    <col min="18" max="18" width="10.85546875" style="136"/>
-    <col min="19" max="16384" width="10.85546875" style="135"/>
+    <col min="1" max="16" width="6.7109375" style="127" customWidth="1"/>
+    <col min="17" max="17" width="1.28515625" style="127" customWidth="1"/>
+    <col min="18" max="18" width="10.85546875" style="127"/>
+    <col min="19" max="16384" width="10.85546875" style="126"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="24.75" hidden="1" customHeight="1"/>
     <row r="2" spans="1:18" ht="60.4" customHeight="1">
-      <c r="C2" s="209" t="s">
+      <c r="C2" s="199" t="s">
         <v>178</v>
       </c>
-      <c r="D2" s="208"/>
-      <c r="E2" s="208"/>
-      <c r="F2" s="208"/>
-      <c r="G2" s="208"/>
-      <c r="H2" s="208"/>
-      <c r="I2" s="208"/>
-      <c r="J2" s="208"/>
-      <c r="K2" s="208"/>
-      <c r="L2" s="208"/>
-      <c r="M2" s="208"/>
-      <c r="N2" s="207"/>
-      <c r="O2" s="200" t="s">
+      <c r="D2" s="198"/>
+      <c r="E2" s="198"/>
+      <c r="F2" s="198"/>
+      <c r="G2" s="198"/>
+      <c r="H2" s="198"/>
+      <c r="I2" s="198"/>
+      <c r="J2" s="198"/>
+      <c r="K2" s="198"/>
+      <c r="L2" s="198"/>
+      <c r="M2" s="198"/>
+      <c r="N2" s="197"/>
+      <c r="O2" s="218" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="18" customHeight="1">
-      <c r="O3" s="200"/>
+      <c r="O3" s="218"/>
     </row>
     <row r="4" spans="1:18" ht="18" customHeight="1">
-      <c r="A4" s="203" t="s">
+      <c r="A4" s="193" t="s">
         <v>176</v>
       </c>
-      <c r="B4" s="203"/>
-      <c r="C4" s="158"/>
-      <c r="D4" s="203" t="s">
+      <c r="B4" s="193"/>
+      <c r="C4" s="149"/>
+      <c r="D4" s="193" t="s">
         <v>175</v>
       </c>
-      <c r="E4" s="150"/>
-      <c r="F4" s="158"/>
-      <c r="G4" s="203" t="s">
+      <c r="E4" s="141"/>
+      <c r="F4" s="149"/>
+      <c r="G4" s="193" t="s">
         <v>174</v>
       </c>
-      <c r="H4" s="203"/>
-      <c r="I4" s="206"/>
-      <c r="J4" s="203" t="s">
+      <c r="H4" s="193"/>
+      <c r="I4" s="196"/>
+      <c r="J4" s="193" t="s">
         <v>173</v>
       </c>
-      <c r="K4" s="203"/>
-      <c r="L4" s="206"/>
-      <c r="M4" s="203"/>
-      <c r="N4" s="205" t="s">
+      <c r="K4" s="193"/>
+      <c r="L4" s="196"/>
+      <c r="M4" s="193"/>
+      <c r="N4" s="195" t="s">
         <v>172</v>
       </c>
-      <c r="O4" s="200"/>
+      <c r="O4" s="218"/>
     </row>
     <row r="5" spans="1:18" ht="18.95" customHeight="1">
-      <c r="A5" s="180"/>
-      <c r="B5" s="180"/>
-      <c r="C5" s="218"/>
-      <c r="D5" s="180"/>
-      <c r="E5" s="180"/>
-      <c r="F5" s="218"/>
-      <c r="G5" s="180"/>
-      <c r="H5" s="180"/>
-      <c r="I5" s="218"/>
-      <c r="J5" s="180"/>
-      <c r="K5" s="180"/>
-      <c r="L5" s="218"/>
-      <c r="M5" s="180"/>
-      <c r="N5" s="180"/>
-      <c r="O5" s="200"/>
+      <c r="A5" s="171"/>
+      <c r="B5" s="171"/>
+      <c r="C5" s="171" t="s">
+        <v>96</v>
+      </c>
+      <c r="D5" s="171"/>
+      <c r="E5" s="171"/>
+      <c r="F5" s="171" t="s">
+        <v>96</v>
+      </c>
+      <c r="G5" s="171"/>
+      <c r="H5" s="171"/>
+      <c r="I5" s="171" t="s">
+        <v>96</v>
+      </c>
+      <c r="J5" s="171"/>
+      <c r="K5" s="171"/>
+      <c r="L5" s="171" t="s">
+        <v>96</v>
+      </c>
+      <c r="M5" s="171"/>
+      <c r="N5" s="171"/>
+      <c r="O5" s="218"/>
     </row>
     <row r="6" spans="1:18" ht="18.95" customHeight="1">
-      <c r="A6" s="203" t="s">
+      <c r="A6" s="193" t="s">
         <v>171</v>
       </c>
-      <c r="B6" s="203"/>
-      <c r="C6" s="158"/>
-      <c r="D6" s="203" t="s">
+      <c r="B6" s="193"/>
+      <c r="C6" s="149"/>
+      <c r="D6" s="193" t="s">
         <v>170</v>
       </c>
-      <c r="E6" s="203"/>
-      <c r="F6" s="158"/>
-      <c r="G6" s="203" t="s">
+      <c r="E6" s="193"/>
+      <c r="F6" s="149"/>
+      <c r="G6" s="193" t="s">
         <v>99</v>
       </c>
-      <c r="H6" s="150"/>
-      <c r="I6" s="204"/>
-      <c r="J6" s="203" t="s">
+      <c r="H6" s="141"/>
+      <c r="I6" s="194"/>
+      <c r="J6" s="193" t="s">
         <v>169</v>
       </c>
-      <c r="K6" s="150"/>
-      <c r="L6" s="202"/>
-      <c r="M6" s="150"/>
-      <c r="N6" s="201" t="s">
+      <c r="K6" s="141"/>
+      <c r="L6" s="192"/>
+      <c r="M6" s="141"/>
+      <c r="N6" s="191" t="s">
         <v>168</v>
       </c>
-      <c r="O6" s="200"/>
+      <c r="O6" s="218"/>
     </row>
     <row r="7" spans="1:18" ht="18.95" customHeight="1">
-      <c r="A7" s="180"/>
-      <c r="B7" s="180"/>
-      <c r="C7" s="218"/>
-      <c r="D7" s="180"/>
-      <c r="E7" s="180"/>
-      <c r="F7" s="218" t="s">
-        <v>96</v>
-      </c>
-      <c r="G7" s="180"/>
-      <c r="H7" s="180"/>
-      <c r="I7" s="218" t="s">
-        <v>96</v>
-      </c>
-      <c r="J7" s="180"/>
-      <c r="K7" s="180"/>
-      <c r="L7" s="180"/>
-      <c r="M7" s="180"/>
-      <c r="N7" s="180"/>
-      <c r="O7" s="200"/>
+      <c r="A7" s="171"/>
+      <c r="B7" s="171"/>
+      <c r="C7" s="171" t="s">
+        <v>96</v>
+      </c>
+      <c r="D7" s="171"/>
+      <c r="E7" s="171"/>
+      <c r="F7" s="171" t="s">
+        <v>96</v>
+      </c>
+      <c r="G7" s="171"/>
+      <c r="H7" s="171"/>
+      <c r="I7" s="171" t="s">
+        <v>96</v>
+      </c>
+      <c r="J7" s="171"/>
+      <c r="K7" s="171"/>
+      <c r="L7" s="171" t="s">
+        <v>96</v>
+      </c>
+      <c r="M7" s="171"/>
+      <c r="N7" s="171"/>
+      <c r="O7" s="218"/>
     </row>
     <row r="8" spans="1:18" ht="6" customHeight="1"/>
     <row r="9" spans="1:18" ht="15" customHeight="1">
-      <c r="A9" s="140" t="s">
+      <c r="A9" s="131" t="s">
         <v>167</v>
       </c>
-      <c r="B9" s="140"/>
-      <c r="C9" s="140"/>
-      <c r="D9" s="140"/>
-      <c r="E9" s="140"/>
-      <c r="F9" s="140"/>
-      <c r="G9" s="140"/>
-      <c r="H9" s="140"/>
-      <c r="I9" s="140"/>
-      <c r="J9" s="140"/>
-      <c r="K9" s="140"/>
-      <c r="L9" s="140"/>
-      <c r="M9" s="140"/>
-      <c r="N9" s="140"/>
-      <c r="O9" s="140"/>
-      <c r="P9" s="140"/>
+      <c r="B9" s="131"/>
+      <c r="C9" s="131"/>
+      <c r="D9" s="131"/>
+      <c r="E9" s="131"/>
+      <c r="F9" s="131"/>
+      <c r="G9" s="131"/>
+      <c r="H9" s="131"/>
+      <c r="I9" s="131"/>
+      <c r="J9" s="131"/>
+      <c r="K9" s="131"/>
+      <c r="L9" s="131"/>
+      <c r="M9" s="131"/>
+      <c r="N9" s="131"/>
+      <c r="O9" s="131"/>
+      <c r="P9" s="131"/>
     </row>
     <row r="10" spans="1:18" ht="5.25" customHeight="1"/>
-    <row r="11" spans="1:18" s="157" customFormat="1">
-      <c r="A11" s="150" t="s">
+    <row r="11" spans="1:18" s="148" customFormat="1">
+      <c r="A11" s="141" t="s">
         <v>166</v>
       </c>
-      <c r="B11" s="150"/>
-      <c r="C11" s="150" t="s">
+      <c r="B11" s="141"/>
+      <c r="C11" s="141" t="s">
         <v>165</v>
       </c>
-      <c r="D11" s="150"/>
-      <c r="E11" s="150" t="s">
+      <c r="D11" s="141"/>
+      <c r="E11" s="141" t="s">
         <v>164</v>
       </c>
-      <c r="F11" s="150"/>
-      <c r="G11" s="150" t="s">
+      <c r="F11" s="141"/>
+      <c r="G11" s="141" t="s">
         <v>163</v>
       </c>
-      <c r="H11" s="150"/>
-      <c r="I11" s="199"/>
-      <c r="J11" s="156" t="s">
+      <c r="H11" s="141"/>
+      <c r="I11" s="190"/>
+      <c r="J11" s="147" t="s">
         <v>162</v>
       </c>
-      <c r="K11" s="156" t="s">
+      <c r="K11" s="147" t="s">
         <v>161</v>
       </c>
-      <c r="L11" s="156" t="s">
+      <c r="L11" s="147" t="s">
         <v>160</v>
       </c>
-      <c r="M11" s="156" t="s">
+      <c r="M11" s="147" t="s">
         <v>159</v>
       </c>
-      <c r="N11" s="156" t="s">
+      <c r="N11" s="147" t="s">
         <v>158</v>
       </c>
-      <c r="O11" s="156" t="s">
+      <c r="O11" s="147" t="s">
         <v>157</v>
       </c>
-      <c r="P11" s="155" t="s">
+      <c r="P11" s="146" t="s">
         <v>156</v>
       </c>
-      <c r="Q11" s="138"/>
-      <c r="R11" s="138"/>
+      <c r="Q11" s="129"/>
+      <c r="R11" s="129"/>
     </row>
     <row r="12" spans="1:18" ht="14.25">
-      <c r="A12" s="180"/>
-      <c r="B12" s="180"/>
-      <c r="C12" s="180"/>
-      <c r="D12" s="180"/>
-      <c r="E12" s="180"/>
-      <c r="F12" s="180"/>
-      <c r="G12" s="160" t="s">
+      <c r="A12" s="171"/>
+      <c r="B12" s="171"/>
+      <c r="C12" s="171"/>
+      <c r="D12" s="171"/>
+      <c r="E12" s="171"/>
+      <c r="F12" s="171"/>
+      <c r="G12" s="151" t="s">
         <v>57</v>
       </c>
-      <c r="H12" s="149"/>
-      <c r="I12" s="198" t="s">
+      <c r="H12" s="140"/>
+      <c r="I12" s="189" t="s">
         <v>123</v>
       </c>
-      <c r="J12" s="196" t="s">
-        <v>96</v>
-      </c>
-      <c r="K12" s="196" t="s">
-        <v>96</v>
-      </c>
-      <c r="L12" s="196" t="s">
-        <v>96</v>
-      </c>
-      <c r="M12" s="196" t="s">
-        <v>96</v>
-      </c>
-      <c r="N12" s="196" t="s">
-        <v>96</v>
-      </c>
-      <c r="O12" s="196" t="s">
-        <v>96</v>
-      </c>
-      <c r="P12" s="195" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" s="157" customFormat="1">
-      <c r="A13" s="150" t="s">
+      <c r="J12" s="187" t="s">
+        <v>96</v>
+      </c>
+      <c r="K12" s="187" t="s">
+        <v>96</v>
+      </c>
+      <c r="L12" s="187" t="s">
+        <v>96</v>
+      </c>
+      <c r="M12" s="187" t="s">
+        <v>96</v>
+      </c>
+      <c r="N12" s="187" t="s">
+        <v>96</v>
+      </c>
+      <c r="O12" s="187" t="s">
+        <v>96</v>
+      </c>
+      <c r="P12" s="186" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" s="148" customFormat="1">
+      <c r="A13" s="141" t="s">
         <v>155</v>
       </c>
-      <c r="B13" s="150"/>
-      <c r="C13" s="150" t="s">
+      <c r="B13" s="141"/>
+      <c r="C13" s="141" t="s">
         <v>154</v>
       </c>
-      <c r="D13" s="150"/>
-      <c r="E13" s="150" t="s">
+      <c r="D13" s="141"/>
+      <c r="E13" s="141" t="s">
         <v>153</v>
       </c>
-      <c r="F13" s="150"/>
-      <c r="G13" s="150"/>
-      <c r="H13" s="150"/>
-      <c r="I13" s="197" t="s">
+      <c r="F13" s="141"/>
+      <c r="G13" s="141"/>
+      <c r="H13" s="141"/>
+      <c r="I13" s="188" t="s">
         <v>152</v>
       </c>
-      <c r="J13" s="196" t="s">
-        <v>96</v>
-      </c>
-      <c r="K13" s="196" t="s">
-        <v>96</v>
-      </c>
-      <c r="L13" s="196" t="s">
-        <v>96</v>
-      </c>
-      <c r="M13" s="196" t="s">
-        <v>96</v>
-      </c>
-      <c r="N13" s="196" t="s">
-        <v>96</v>
-      </c>
-      <c r="O13" s="196" t="s">
-        <v>96</v>
-      </c>
-      <c r="P13" s="195" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q13" s="138"/>
-      <c r="R13" s="138"/>
+      <c r="J13" s="187" t="s">
+        <v>96</v>
+      </c>
+      <c r="K13" s="187" t="s">
+        <v>96</v>
+      </c>
+      <c r="L13" s="187" t="s">
+        <v>96</v>
+      </c>
+      <c r="M13" s="187" t="s">
+        <v>96</v>
+      </c>
+      <c r="N13" s="187" t="s">
+        <v>96</v>
+      </c>
+      <c r="O13" s="187" t="s">
+        <v>96</v>
+      </c>
+      <c r="P13" s="186" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q13" s="129"/>
+      <c r="R13" s="129"/>
     </row>
     <row r="14" spans="1:18" ht="14.25">
-      <c r="A14" s="180"/>
-      <c r="B14" s="180"/>
-      <c r="C14" s="180"/>
-      <c r="D14" s="180"/>
-      <c r="E14" s="180"/>
-      <c r="F14" s="180"/>
-      <c r="G14" s="180"/>
-      <c r="H14" s="180"/>
-      <c r="I14" s="194" t="s">
+      <c r="A14" s="171"/>
+      <c r="B14" s="171"/>
+      <c r="C14" s="171"/>
+      <c r="D14" s="171"/>
+      <c r="E14" s="171"/>
+      <c r="F14" s="171"/>
+      <c r="G14" s="171"/>
+      <c r="H14" s="171"/>
+      <c r="I14" s="185" t="s">
         <v>151</v>
       </c>
-      <c r="J14" s="193" t="s">
-        <v>96</v>
-      </c>
-      <c r="K14" s="193" t="s">
-        <v>96</v>
-      </c>
-      <c r="L14" s="193" t="s">
-        <v>96</v>
-      </c>
-      <c r="M14" s="193" t="s">
-        <v>96</v>
-      </c>
-      <c r="N14" s="193" t="s">
-        <v>96</v>
-      </c>
-      <c r="O14" s="193" t="s">
-        <v>96</v>
-      </c>
-      <c r="P14" s="192"/>
+      <c r="J14" s="184" t="s">
+        <v>96</v>
+      </c>
+      <c r="K14" s="184" t="s">
+        <v>96</v>
+      </c>
+      <c r="L14" s="184" t="s">
+        <v>96</v>
+      </c>
+      <c r="M14" s="184" t="s">
+        <v>96</v>
+      </c>
+      <c r="N14" s="184" t="s">
+        <v>96</v>
+      </c>
+      <c r="O14" s="184" t="s">
+        <v>96</v>
+      </c>
+      <c r="P14" s="183"/>
     </row>
     <row r="15" spans="1:18" ht="6" customHeight="1">
-      <c r="A15" s="191"/>
+      <c r="A15" s="182"/>
     </row>
     <row r="16" spans="1:18" ht="15" customHeight="1">
-      <c r="A16" s="141" t="s">
+      <c r="A16" s="132" t="s">
         <v>150</v>
       </c>
-      <c r="B16" s="140"/>
-      <c r="C16" s="140"/>
-      <c r="D16" s="140"/>
-      <c r="E16" s="140"/>
-      <c r="F16" s="140"/>
-      <c r="G16" s="140"/>
-      <c r="H16" s="140"/>
-      <c r="I16" s="140"/>
-      <c r="J16" s="140"/>
-      <c r="K16" s="140"/>
-      <c r="L16" s="140"/>
-      <c r="M16" s="140"/>
-      <c r="N16" s="140"/>
-      <c r="O16" s="140"/>
-      <c r="P16" s="140"/>
+      <c r="B16" s="131"/>
+      <c r="C16" s="131"/>
+      <c r="D16" s="131"/>
+      <c r="E16" s="131"/>
+      <c r="F16" s="131"/>
+      <c r="G16" s="131"/>
+      <c r="H16" s="131"/>
+      <c r="I16" s="131"/>
+      <c r="J16" s="131"/>
+      <c r="K16" s="131"/>
+      <c r="L16" s="131"/>
+      <c r="M16" s="131"/>
+      <c r="N16" s="131"/>
+      <c r="O16" s="131"/>
+      <c r="P16" s="131"/>
     </row>
     <row r="17" spans="1:21" ht="5.25" customHeight="1">
-      <c r="K17" s="182"/>
-      <c r="L17" s="182"/>
-      <c r="M17" s="182"/>
-      <c r="N17" s="182"/>
-    </row>
-    <row r="18" spans="1:21" s="157" customFormat="1">
-      <c r="A18" s="150" t="s">
+      <c r="K17" s="173"/>
+      <c r="L17" s="173"/>
+      <c r="M17" s="173"/>
+      <c r="N17" s="173"/>
+    </row>
+    <row r="18" spans="1:21" s="148" customFormat="1">
+      <c r="A18" s="141" t="s">
         <v>149</v>
       </c>
-      <c r="B18" s="150"/>
-      <c r="C18" s="150" t="s">
+      <c r="B18" s="141"/>
+      <c r="C18" s="141" t="s">
         <v>148</v>
       </c>
-      <c r="D18" s="150"/>
-      <c r="E18" s="150" t="s">
+      <c r="D18" s="141"/>
+      <c r="E18" s="141" t="s">
         <v>147</v>
       </c>
-      <c r="F18" s="150"/>
-      <c r="G18" s="150" t="s">
+      <c r="F18" s="141"/>
+      <c r="G18" s="141" t="s">
         <v>146</v>
       </c>
-      <c r="H18" s="150"/>
-      <c r="I18" s="150" t="s">
+      <c r="H18" s="141"/>
+      <c r="I18" s="141" t="s">
         <v>145</v>
       </c>
-      <c r="J18" s="150"/>
-      <c r="K18" s="150" t="s">
+      <c r="J18" s="141"/>
+      <c r="K18" s="141" t="s">
         <v>144</v>
       </c>
-      <c r="L18" s="150"/>
-      <c r="M18" s="150" t="s">
+      <c r="L18" s="141"/>
+      <c r="M18" s="141" t="s">
         <v>143</v>
       </c>
-      <c r="N18" s="150"/>
-      <c r="O18" s="150" t="s">
+      <c r="N18" s="141"/>
+      <c r="O18" s="141" t="s">
         <v>142</v>
       </c>
-      <c r="P18" s="150"/>
-      <c r="Q18" s="138"/>
+      <c r="P18" s="141"/>
+      <c r="Q18" s="129"/>
     </row>
     <row r="19" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A19" s="180"/>
-      <c r="B19" s="180"/>
-      <c r="C19" s="180"/>
-      <c r="D19" s="180"/>
-      <c r="E19" s="180"/>
-      <c r="F19" s="180"/>
-      <c r="G19" s="180"/>
-      <c r="H19" s="180"/>
-      <c r="I19" s="180"/>
-      <c r="J19" s="180"/>
-      <c r="K19" s="180"/>
-      <c r="L19" s="180"/>
-      <c r="M19" s="180"/>
-      <c r="N19" s="180"/>
-      <c r="O19" s="180"/>
-      <c r="P19" s="180"/>
-      <c r="R19" s="135"/>
+      <c r="A19" s="171"/>
+      <c r="B19" s="171"/>
+      <c r="C19" s="171"/>
+      <c r="D19" s="171"/>
+      <c r="E19" s="171"/>
+      <c r="F19" s="171"/>
+      <c r="G19" s="171"/>
+      <c r="H19" s="171"/>
+      <c r="I19" s="171"/>
+      <c r="J19" s="171"/>
+      <c r="K19" s="171"/>
+      <c r="L19" s="171"/>
+      <c r="M19" s="171"/>
+      <c r="N19" s="171"/>
+      <c r="O19" s="171"/>
+      <c r="P19" s="171"/>
+      <c r="R19" s="126"/>
     </row>
     <row r="20" spans="1:21" hidden="1">
-      <c r="A20" s="149"/>
-      <c r="B20" s="149"/>
-      <c r="C20" s="149"/>
-      <c r="D20" s="149"/>
-      <c r="E20" s="150" t="s">
+      <c r="A20" s="140"/>
+      <c r="B20" s="140"/>
+      <c r="C20" s="140"/>
+      <c r="D20" s="140"/>
+      <c r="E20" s="141" t="s">
         <v>112</v>
       </c>
-      <c r="F20" s="150"/>
-      <c r="G20" s="150"/>
-      <c r="H20" s="150"/>
-      <c r="I20" s="158"/>
-      <c r="J20" s="149"/>
-      <c r="K20" s="149"/>
-      <c r="L20" s="149"/>
-      <c r="M20" s="190"/>
-      <c r="N20" s="149"/>
-      <c r="O20" s="149"/>
-      <c r="P20" s="149"/>
-      <c r="R20" s="149" t="s">
-        <v>96</v>
-      </c>
-      <c r="S20" s="149"/>
-      <c r="T20" s="149" t="s">
-        <v>96</v>
-      </c>
-      <c r="U20" s="149"/>
-    </row>
-    <row r="21" spans="1:21" s="157" customFormat="1">
-      <c r="A21" s="150"/>
-      <c r="B21" s="189" t="s">
+      <c r="F20" s="141"/>
+      <c r="G20" s="141"/>
+      <c r="H20" s="141"/>
+      <c r="I20" s="149"/>
+      <c r="J20" s="140"/>
+      <c r="K20" s="140"/>
+      <c r="L20" s="140"/>
+      <c r="M20" s="181"/>
+      <c r="N20" s="140"/>
+      <c r="O20" s="140"/>
+      <c r="P20" s="140"/>
+      <c r="R20" s="140" t="s">
+        <v>96</v>
+      </c>
+      <c r="S20" s="140"/>
+      <c r="T20" s="140" t="s">
+        <v>96</v>
+      </c>
+      <c r="U20" s="140"/>
+    </row>
+    <row r="21" spans="1:21" s="148" customFormat="1">
+      <c r="A21" s="141"/>
+      <c r="B21" s="180" t="s">
         <v>97</v>
       </c>
-      <c r="C21" s="150" t="s">
+      <c r="C21" s="141" t="s">
         <v>141</v>
       </c>
-      <c r="D21" s="150"/>
-      <c r="E21" s="150" t="s">
+      <c r="D21" s="141"/>
+      <c r="E21" s="141" t="s">
         <v>111</v>
       </c>
-      <c r="F21" s="150"/>
-      <c r="G21" s="150" t="s">
+      <c r="F21" s="141"/>
+      <c r="G21" s="141" t="s">
         <v>110</v>
       </c>
-      <c r="H21" s="150"/>
-      <c r="I21" s="188"/>
-      <c r="J21" s="187" t="s">
+      <c r="H21" s="141"/>
+      <c r="I21" s="179"/>
+      <c r="J21" s="178" t="s">
         <v>180</v>
       </c>
-      <c r="K21" s="150" t="s">
+      <c r="K21" s="141" t="s">
         <v>53</v>
       </c>
-      <c r="L21" s="150"/>
-      <c r="M21" s="150" t="s">
+      <c r="L21" s="141"/>
+      <c r="M21" s="141" t="s">
         <v>54</v>
       </c>
-      <c r="N21" s="150"/>
-      <c r="O21" s="150" t="s">
+      <c r="N21" s="141"/>
+      <c r="O21" s="141" t="s">
         <v>140</v>
       </c>
-      <c r="P21" s="150"/>
-      <c r="Q21" s="138"/>
-      <c r="R21" s="138"/>
+      <c r="P21" s="141"/>
+      <c r="Q21" s="129"/>
+      <c r="R21" s="129"/>
     </row>
     <row r="22" spans="1:21">
-      <c r="A22" s="186" t="s">
+      <c r="A22" s="177" t="s">
         <v>139</v>
       </c>
-      <c r="B22" s="185" t="s">
-        <v>96</v>
-      </c>
-      <c r="C22" s="184" t="s">
-        <v>96</v>
-      </c>
-      <c r="D22" s="184"/>
-      <c r="E22" s="180"/>
-      <c r="F22" s="180"/>
-      <c r="G22" s="183"/>
-      <c r="H22" s="180"/>
-      <c r="I22" s="182" t="s">
-        <v>96</v>
-      </c>
-      <c r="J22" s="181" t="s">
+      <c r="B22" s="176" t="s">
+        <v>96</v>
+      </c>
+      <c r="C22" s="175" t="s">
+        <v>96</v>
+      </c>
+      <c r="D22" s="175"/>
+      <c r="E22" s="171"/>
+      <c r="F22" s="171"/>
+      <c r="G22" s="174"/>
+      <c r="H22" s="171"/>
+      <c r="I22" s="173" t="s">
+        <v>96</v>
+      </c>
+      <c r="J22" s="172" t="s">
         <v>138</v>
       </c>
-      <c r="K22" s="180" t="s">
-        <v>96</v>
-      </c>
-      <c r="L22" s="180"/>
-      <c r="M22" s="180" t="s">
-        <v>96</v>
-      </c>
-      <c r="N22" s="180"/>
-      <c r="O22" s="180" t="s">
-        <v>96</v>
-      </c>
-      <c r="P22" s="180"/>
+      <c r="K22" s="171" t="s">
+        <v>96</v>
+      </c>
+      <c r="L22" s="171"/>
+      <c r="M22" s="171" t="s">
+        <v>96</v>
+      </c>
+      <c r="N22" s="171"/>
+      <c r="O22" s="171" t="s">
+        <v>96</v>
+      </c>
+      <c r="P22" s="171"/>
     </row>
     <row r="23" spans="1:21" ht="15.75">
-      <c r="A23" s="147" t="s">
+      <c r="A23" s="138" t="s">
         <v>137</v>
       </c>
-      <c r="B23" s="179" t="s">
-        <v>96</v>
-      </c>
-      <c r="C23" s="175" t="s">
-        <v>96</v>
-      </c>
-      <c r="D23" s="175"/>
-      <c r="E23" s="178" t="s">
+      <c r="B23" s="170" t="s">
+        <v>96</v>
+      </c>
+      <c r="C23" s="166" t="s">
+        <v>96</v>
+      </c>
+      <c r="D23" s="166"/>
+      <c r="E23" s="169" t="s">
         <v>136</v>
       </c>
-      <c r="F23" s="178"/>
-      <c r="G23" s="177"/>
-      <c r="H23" s="178"/>
-      <c r="I23" s="177"/>
-      <c r="J23" s="176" t="s">
+      <c r="F23" s="169"/>
+      <c r="G23" s="168"/>
+      <c r="H23" s="169"/>
+      <c r="I23" s="168"/>
+      <c r="J23" s="167" t="s">
         <v>135</v>
       </c>
-      <c r="K23" s="175" t="s">
-        <v>96</v>
-      </c>
-      <c r="L23" s="175"/>
-      <c r="M23" s="175" t="s">
-        <v>96</v>
-      </c>
-      <c r="N23" s="175"/>
-      <c r="O23" s="175" t="s">
-        <v>96</v>
-      </c>
-      <c r="P23" s="175"/>
+      <c r="K23" s="166" t="s">
+        <v>96</v>
+      </c>
+      <c r="L23" s="166"/>
+      <c r="M23" s="166" t="s">
+        <v>96</v>
+      </c>
+      <c r="N23" s="166"/>
+      <c r="O23" s="166" t="s">
+        <v>96</v>
+      </c>
+      <c r="P23" s="166"/>
     </row>
     <row r="24" spans="1:21" ht="5.25" customHeight="1">
-      <c r="A24" s="153"/>
-      <c r="B24" s="152"/>
-      <c r="C24" s="152"/>
-      <c r="D24" s="152"/>
-      <c r="E24" s="152"/>
-      <c r="F24" s="152"/>
-      <c r="G24" s="152"/>
-      <c r="H24" s="152"/>
-      <c r="I24" s="152"/>
-      <c r="J24" s="152"/>
-      <c r="K24" s="151"/>
-      <c r="L24" s="151"/>
-      <c r="M24" s="151"/>
-      <c r="N24" s="151"/>
-      <c r="O24" s="151"/>
-      <c r="P24" s="151"/>
+      <c r="A24" s="144"/>
+      <c r="B24" s="143"/>
+      <c r="C24" s="143"/>
+      <c r="D24" s="143"/>
+      <c r="E24" s="143"/>
+      <c r="F24" s="143"/>
+      <c r="G24" s="143"/>
+      <c r="H24" s="143"/>
+      <c r="I24" s="143"/>
+      <c r="J24" s="143"/>
+      <c r="K24" s="142"/>
+      <c r="L24" s="142"/>
+      <c r="M24" s="142"/>
+      <c r="N24" s="142"/>
+      <c r="O24" s="142"/>
+      <c r="P24" s="142"/>
     </row>
     <row r="25" spans="1:21">
-      <c r="A25" s="153" t="s">
+      <c r="A25" s="144" t="s">
         <v>134</v>
       </c>
-      <c r="B25" s="153"/>
-      <c r="C25" s="153" t="s">
+      <c r="B25" s="144"/>
+      <c r="C25" s="144" t="s">
         <v>133</v>
       </c>
-      <c r="D25" s="174"/>
-      <c r="E25" s="153" t="s">
+      <c r="D25" s="165"/>
+      <c r="E25" s="144" t="s">
         <v>132</v>
       </c>
-      <c r="F25" s="153"/>
-      <c r="G25" s="174"/>
-      <c r="H25" s="173" t="s">
+      <c r="F25" s="144"/>
+      <c r="G25" s="165"/>
+      <c r="H25" s="164" t="s">
         <v>131</v>
       </c>
-      <c r="I25" s="173"/>
-      <c r="J25" s="150" t="s">
+      <c r="I25" s="164"/>
+      <c r="J25" s="141" t="s">
         <v>81</v>
       </c>
-      <c r="K25" s="150"/>
-      <c r="L25" s="153" t="s">
+      <c r="K25" s="141"/>
+      <c r="L25" s="144" t="s">
         <v>130</v>
       </c>
-      <c r="M25" s="153"/>
-      <c r="N25" s="153"/>
-      <c r="O25" s="153"/>
-      <c r="P25" s="153"/>
+      <c r="M25" s="144"/>
+      <c r="N25" s="144"/>
+      <c r="O25" s="144"/>
+      <c r="P25" s="144"/>
     </row>
     <row r="26" spans="1:21">
-      <c r="A26" s="153" t="s">
+      <c r="A26" s="144" t="s">
         <v>40</v>
       </c>
-      <c r="B26" s="160" t="s">
+      <c r="B26" s="151" t="s">
         <v>57</v>
       </c>
-      <c r="C26" s="148" t="s">
-        <v>96</v>
-      </c>
-      <c r="D26" s="148" t="s">
-        <v>96</v>
-      </c>
-      <c r="E26" s="148" t="s">
-        <v>96</v>
-      </c>
-      <c r="F26" s="148"/>
-      <c r="G26" s="148"/>
-      <c r="H26" s="148" t="s">
-        <v>96</v>
-      </c>
-      <c r="I26" s="148"/>
-      <c r="J26" s="148" t="s">
-        <v>96</v>
-      </c>
-      <c r="K26" s="148"/>
-      <c r="L26" s="153" t="s">
+      <c r="C26" s="139" t="s">
+        <v>96</v>
+      </c>
+      <c r="D26" s="139" t="s">
+        <v>96</v>
+      </c>
+      <c r="E26" s="139" t="s">
+        <v>96</v>
+      </c>
+      <c r="F26" s="139"/>
+      <c r="G26" s="139"/>
+      <c r="H26" s="139" t="s">
+        <v>96</v>
+      </c>
+      <c r="I26" s="139"/>
+      <c r="J26" s="139" t="s">
+        <v>96</v>
+      </c>
+      <c r="K26" s="139"/>
+      <c r="L26" s="144" t="s">
         <v>108</v>
       </c>
-      <c r="M26" s="153"/>
-      <c r="N26" s="154" t="s">
+      <c r="M26" s="144"/>
+      <c r="N26" s="145" t="s">
         <v>107</v>
       </c>
-      <c r="O26" s="153" t="s">
+      <c r="O26" s="144" t="s">
         <v>106</v>
       </c>
-      <c r="P26" s="153"/>
+      <c r="P26" s="144"/>
     </row>
     <row r="27" spans="1:21">
-      <c r="A27" s="153" t="s">
+      <c r="A27" s="144" t="s">
         <v>129</v>
       </c>
-      <c r="B27" s="160" t="s">
+      <c r="B27" s="151" t="s">
         <v>57</v>
       </c>
-      <c r="C27" s="172"/>
-      <c r="D27" s="172"/>
-      <c r="E27" s="172"/>
-      <c r="F27" s="172"/>
-      <c r="G27" s="172"/>
-      <c r="H27" s="172"/>
-      <c r="I27" s="172"/>
-      <c r="J27" s="171"/>
-      <c r="K27" s="171"/>
-      <c r="L27" s="148" t="s">
-        <v>96</v>
-      </c>
-      <c r="M27" s="148" t="s">
-        <v>96</v>
-      </c>
-      <c r="N27" s="148" t="s">
-        <v>96</v>
-      </c>
-      <c r="O27" s="148"/>
-      <c r="P27" s="170"/>
+      <c r="C27" s="163"/>
+      <c r="D27" s="163"/>
+      <c r="E27" s="163"/>
+      <c r="F27" s="163"/>
+      <c r="G27" s="163"/>
+      <c r="H27" s="163"/>
+      <c r="I27" s="163"/>
+      <c r="J27" s="162"/>
+      <c r="K27" s="162"/>
+      <c r="L27" s="139" t="s">
+        <v>96</v>
+      </c>
+      <c r="M27" s="139" t="s">
+        <v>96</v>
+      </c>
+      <c r="N27" s="139" t="s">
+        <v>96</v>
+      </c>
+      <c r="O27" s="139"/>
+      <c r="P27" s="161"/>
     </row>
     <row r="28" spans="1:21" ht="6" customHeight="1"/>
     <row r="29" spans="1:21" ht="15.75">
-      <c r="A29" s="141" t="s">
+      <c r="A29" s="132" t="s">
         <v>128</v>
       </c>
-      <c r="B29" s="140"/>
-      <c r="C29" s="140"/>
-      <c r="D29" s="140"/>
-      <c r="E29" s="140"/>
-      <c r="F29" s="140"/>
-      <c r="G29" s="140"/>
-      <c r="H29" s="140"/>
-      <c r="I29" s="140"/>
-      <c r="J29" s="140"/>
-      <c r="K29" s="140"/>
-      <c r="L29" s="140"/>
-      <c r="M29" s="140"/>
-      <c r="N29" s="140"/>
-      <c r="O29" s="140"/>
-      <c r="P29" s="140"/>
+      <c r="B29" s="131"/>
+      <c r="C29" s="131"/>
+      <c r="D29" s="131"/>
+      <c r="E29" s="131"/>
+      <c r="F29" s="131"/>
+      <c r="G29" s="131"/>
+      <c r="H29" s="131"/>
+      <c r="I29" s="131"/>
+      <c r="J29" s="131"/>
+      <c r="K29" s="131"/>
+      <c r="L29" s="131"/>
+      <c r="M29" s="131"/>
+      <c r="N29" s="131"/>
+      <c r="O29" s="131"/>
+      <c r="P29" s="131"/>
     </row>
     <row r="30" spans="1:21" ht="5.25" customHeight="1">
-      <c r="K30" s="158"/>
-      <c r="L30" s="158"/>
-      <c r="M30" s="158"/>
-      <c r="N30" s="158"/>
-      <c r="O30" s="158"/>
-      <c r="P30" s="158"/>
+      <c r="K30" s="149"/>
+      <c r="L30" s="149"/>
+      <c r="M30" s="149"/>
+      <c r="N30" s="149"/>
+      <c r="O30" s="149"/>
+      <c r="P30" s="149"/>
     </row>
     <row r="31" spans="1:21" ht="14.25">
-      <c r="A31" s="169" t="s">
+      <c r="A31" s="160" t="s">
         <v>127</v>
       </c>
-      <c r="B31" s="156" t="s">
+      <c r="B31" s="147" t="s">
         <v>53</v>
       </c>
-      <c r="C31" s="156" t="s">
+      <c r="C31" s="147" t="s">
         <v>54</v>
       </c>
-      <c r="F31" s="153" t="s">
+      <c r="F31" s="144" t="s">
         <v>126</v>
       </c>
-      <c r="G31" s="153"/>
-      <c r="H31" s="153"/>
-      <c r="I31" s="158"/>
-      <c r="K31" s="150" t="s">
+      <c r="G31" s="144"/>
+      <c r="H31" s="144"/>
+      <c r="I31" s="149"/>
+      <c r="K31" s="141" t="s">
         <v>125</v>
       </c>
-      <c r="L31" s="150"/>
-      <c r="M31" s="150" t="s">
+      <c r="L31" s="141"/>
+      <c r="M31" s="141" t="s">
         <v>60</v>
       </c>
-      <c r="N31" s="150"/>
-      <c r="O31" s="150" t="s">
+      <c r="N31" s="141"/>
+      <c r="O31" s="141" t="s">
         <v>124</v>
       </c>
-      <c r="P31" s="150"/>
+      <c r="P31" s="141"/>
     </row>
     <row r="32" spans="1:21">
-      <c r="A32" s="165" t="s">
+      <c r="A32" s="156" t="s">
         <v>123</v>
       </c>
-      <c r="B32" s="168" t="s">
-        <v>96</v>
-      </c>
-      <c r="C32" s="168" t="s">
-        <v>96</v>
-      </c>
-      <c r="D32" s="219" t="s">
+      <c r="B32" s="159" t="s">
+        <v>96</v>
+      </c>
+      <c r="C32" s="159" t="s">
+        <v>96</v>
+      </c>
+      <c r="D32" s="208" t="s">
         <v>122</v>
       </c>
-      <c r="F32" s="167" t="s">
+      <c r="F32" s="158" t="s">
         <v>121</v>
       </c>
-      <c r="G32" s="150"/>
-      <c r="H32" s="166" t="s">
+      <c r="G32" s="141"/>
+      <c r="H32" s="157" t="s">
         <v>120</v>
       </c>
-      <c r="I32" s="158"/>
-      <c r="K32" s="160" t="s">
+      <c r="I32" s="149"/>
+      <c r="K32" s="151" t="s">
         <v>57</v>
       </c>
-      <c r="L32" s="149"/>
-      <c r="M32" s="160" t="s">
+      <c r="L32" s="140"/>
+      <c r="M32" s="151" t="s">
         <v>57</v>
       </c>
-      <c r="N32" s="149"/>
-      <c r="O32" s="160" t="s">
+      <c r="N32" s="140"/>
+      <c r="O32" s="151" t="s">
         <v>57</v>
       </c>
-      <c r="P32" s="149"/>
+      <c r="P32" s="140"/>
     </row>
     <row r="33" spans="1:18" ht="14.25" customHeight="1">
-      <c r="A33" s="165" t="s">
+      <c r="A33" s="156" t="s">
         <v>109</v>
       </c>
-      <c r="B33" s="162" t="s">
-        <v>96</v>
-      </c>
-      <c r="C33" s="162" t="s">
-        <v>96</v>
-      </c>
-      <c r="D33" s="164" t="s">
+      <c r="B33" s="153" t="s">
+        <v>96</v>
+      </c>
+      <c r="C33" s="153" t="s">
+        <v>96</v>
+      </c>
+      <c r="D33" s="155" t="s">
         <v>19</v>
       </c>
-      <c r="F33" s="148"/>
-      <c r="G33" s="148" t="s">
+      <c r="F33" s="139"/>
+      <c r="G33" s="139" t="s">
         <v>119</v>
       </c>
-      <c r="H33" s="148" t="s">
-        <v>96</v>
-      </c>
-      <c r="K33" s="150" t="s">
+      <c r="H33" s="139" t="s">
+        <v>96</v>
+      </c>
+      <c r="K33" s="141" t="s">
         <v>118</v>
       </c>
-      <c r="L33" s="150"/>
-      <c r="M33" s="150" t="s">
+      <c r="L33" s="141"/>
+      <c r="M33" s="141" t="s">
         <v>88</v>
       </c>
-      <c r="N33" s="150"/>
-      <c r="O33" s="150" t="s">
+      <c r="N33" s="141"/>
+      <c r="O33" s="141" t="s">
         <v>117</v>
       </c>
-      <c r="P33" s="150"/>
+      <c r="P33" s="141"/>
     </row>
     <row r="34" spans="1:18">
-      <c r="A34" s="163" t="s">
+      <c r="A34" s="154" t="s">
         <v>116</v>
       </c>
-      <c r="B34" s="162" t="s">
-        <v>96</v>
-      </c>
-      <c r="C34" s="162" t="s">
-        <v>96</v>
-      </c>
-      <c r="D34" s="161" t="s">
+      <c r="B34" s="153" t="s">
+        <v>96</v>
+      </c>
+      <c r="C34" s="153" t="s">
+        <v>96</v>
+      </c>
+      <c r="D34" s="152" t="s">
         <v>115</v>
       </c>
-      <c r="E34" s="138"/>
-      <c r="K34" s="160" t="s">
+      <c r="E34" s="129"/>
+      <c r="K34" s="151" t="s">
         <v>57</v>
       </c>
-      <c r="L34" s="149"/>
-      <c r="M34" s="160" t="s">
+      <c r="L34" s="140"/>
+      <c r="M34" s="151" t="s">
         <v>57</v>
       </c>
-      <c r="N34" s="149"/>
-      <c r="O34" s="160" t="s">
+      <c r="N34" s="140"/>
+      <c r="O34" s="151" t="s">
         <v>57</v>
       </c>
-      <c r="P34" s="149"/>
+      <c r="P34" s="140"/>
     </row>
     <row r="35" spans="1:18" ht="6" customHeight="1">
-      <c r="A35" s="138"/>
-      <c r="C35" s="138"/>
+      <c r="A35" s="129"/>
+      <c r="C35" s="129"/>
     </row>
     <row r="36" spans="1:18" ht="15.75">
-      <c r="A36" s="141" t="s">
+      <c r="A36" s="132" t="s">
         <v>179</v>
       </c>
-      <c r="B36" s="140"/>
-      <c r="C36" s="140"/>
-      <c r="D36" s="140"/>
-      <c r="E36" s="140"/>
-      <c r="F36" s="140"/>
-      <c r="G36" s="140"/>
-      <c r="H36" s="140"/>
-      <c r="I36" s="140"/>
-      <c r="J36" s="140"/>
-      <c r="K36" s="140"/>
-      <c r="L36" s="140"/>
-      <c r="M36" s="140"/>
-      <c r="N36" s="140"/>
-      <c r="O36" s="140"/>
-      <c r="P36" s="140"/>
+      <c r="B36" s="131"/>
+      <c r="C36" s="131"/>
+      <c r="D36" s="131"/>
+      <c r="E36" s="131"/>
+      <c r="F36" s="131"/>
+      <c r="G36" s="131"/>
+      <c r="H36" s="131"/>
+      <c r="I36" s="131"/>
+      <c r="J36" s="131"/>
+      <c r="K36" s="131"/>
+      <c r="L36" s="131"/>
+      <c r="M36" s="131"/>
+      <c r="N36" s="131"/>
+      <c r="O36" s="131"/>
+      <c r="P36" s="131"/>
     </row>
     <row r="37" spans="1:18" ht="5.25" customHeight="1"/>
-    <row r="38" spans="1:18" s="157" customFormat="1">
-      <c r="A38" s="159" t="s">
+    <row r="38" spans="1:18" s="148" customFormat="1">
+      <c r="A38" s="150" t="s">
         <v>114</v>
       </c>
-      <c r="B38" s="150"/>
-      <c r="C38" s="158"/>
-      <c r="D38" s="150" t="s">
+      <c r="B38" s="141"/>
+      <c r="C38" s="149"/>
+      <c r="D38" s="141" t="s">
         <v>113</v>
       </c>
-      <c r="E38" s="158"/>
-      <c r="F38" s="150" t="s">
+      <c r="E38" s="149"/>
+      <c r="F38" s="141" t="s">
         <v>5</v>
       </c>
-      <c r="G38" s="150"/>
-      <c r="H38" s="150" t="s">
+      <c r="G38" s="141"/>
+      <c r="H38" s="141" t="s">
         <v>99</v>
       </c>
-      <c r="I38" s="150"/>
-      <c r="K38" s="136"/>
-      <c r="L38" s="136"/>
-      <c r="M38" s="187"/>
-      <c r="N38" s="217"/>
-      <c r="O38" s="217"/>
-      <c r="P38" s="217"/>
-      <c r="Q38" s="138"/>
-      <c r="R38" s="138"/>
+      <c r="I38" s="141"/>
+      <c r="K38" s="127"/>
+      <c r="L38" s="127"/>
+      <c r="M38" s="178"/>
+      <c r="N38" s="207"/>
+      <c r="O38" s="207"/>
+      <c r="P38" s="207"/>
+      <c r="Q38" s="129"/>
+      <c r="R38" s="129"/>
     </row>
     <row r="39" spans="1:18">
-      <c r="A39" s="149" t="s">
-        <v>96</v>
-      </c>
-      <c r="B39" s="149"/>
-      <c r="C39" s="149" t="s">
-        <v>96</v>
-      </c>
-      <c r="D39" s="149"/>
-      <c r="E39" s="149"/>
-      <c r="F39" s="148" t="s">
-        <v>96</v>
-      </c>
-      <c r="G39" s="148"/>
-      <c r="H39" s="148" t="s">
-        <v>96</v>
-      </c>
-      <c r="I39" s="148"/>
-      <c r="M39" s="215"/>
-      <c r="N39" s="216" t="s">
-        <v>96</v>
-      </c>
-      <c r="O39" s="216" t="s">
-        <v>96</v>
-      </c>
-      <c r="P39" s="216" t="s">
+      <c r="A39" s="140" t="s">
+        <v>96</v>
+      </c>
+      <c r="B39" s="140"/>
+      <c r="C39" s="140" t="s">
+        <v>96</v>
+      </c>
+      <c r="D39" s="140"/>
+      <c r="E39" s="140"/>
+      <c r="F39" s="139" t="s">
+        <v>96</v>
+      </c>
+      <c r="G39" s="139"/>
+      <c r="H39" s="139" t="s">
+        <v>96</v>
+      </c>
+      <c r="I39" s="139"/>
+      <c r="M39" s="205"/>
+      <c r="N39" s="206" t="s">
+        <v>96</v>
+      </c>
+      <c r="O39" s="206" t="s">
+        <v>96</v>
+      </c>
+      <c r="P39" s="206" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="40" spans="1:18">
-      <c r="A40" s="210"/>
-      <c r="B40" s="211"/>
-      <c r="C40" s="153"/>
-      <c r="D40" s="153"/>
-      <c r="E40" s="153"/>
-      <c r="F40" s="153"/>
-      <c r="G40" s="151"/>
-      <c r="M40" s="215"/>
-      <c r="N40" s="216" t="s">
-        <v>96</v>
-      </c>
-      <c r="O40" s="216" t="s">
-        <v>96</v>
-      </c>
-      <c r="P40" s="216" t="s">
+      <c r="A40" s="200"/>
+      <c r="B40" s="201"/>
+      <c r="C40" s="144"/>
+      <c r="D40" s="144"/>
+      <c r="E40" s="144"/>
+      <c r="F40" s="144"/>
+      <c r="G40" s="142"/>
+      <c r="M40" s="205"/>
+      <c r="N40" s="206" t="s">
+        <v>96</v>
+      </c>
+      <c r="O40" s="206" t="s">
+        <v>96</v>
+      </c>
+      <c r="P40" s="206" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="41" spans="1:18">
-      <c r="A41" s="210"/>
-      <c r="B41" s="211"/>
-      <c r="C41" s="153"/>
-      <c r="D41" s="153"/>
-      <c r="E41" s="153"/>
-      <c r="F41" s="153"/>
-      <c r="G41" s="151"/>
-      <c r="M41" s="215"/>
-      <c r="N41" s="216" t="s">
-        <v>96</v>
-      </c>
-      <c r="O41" s="216" t="s">
-        <v>96</v>
-      </c>
-      <c r="P41" s="216" t="s">
+      <c r="A41" s="200"/>
+      <c r="B41" s="201"/>
+      <c r="C41" s="144"/>
+      <c r="D41" s="144"/>
+      <c r="E41" s="144"/>
+      <c r="F41" s="144"/>
+      <c r="G41" s="142"/>
+      <c r="M41" s="205"/>
+      <c r="N41" s="206" t="s">
+        <v>96</v>
+      </c>
+      <c r="O41" s="206" t="s">
+        <v>96</v>
+      </c>
+      <c r="P41" s="206" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="42" spans="1:18" ht="14.25">
-      <c r="A42" s="212"/>
-      <c r="B42" s="213"/>
-      <c r="C42" s="214"/>
-      <c r="D42" s="214"/>
-      <c r="E42" s="214"/>
-      <c r="F42" s="214"/>
-      <c r="G42" s="151"/>
-      <c r="M42" s="215"/>
-      <c r="N42" s="216" t="s">
-        <v>96</v>
-      </c>
-      <c r="O42" s="216" t="s">
-        <v>96</v>
-      </c>
-      <c r="P42" s="216" t="s">
+      <c r="A42" s="202"/>
+      <c r="B42" s="203"/>
+      <c r="C42" s="204"/>
+      <c r="D42" s="204"/>
+      <c r="E42" s="204"/>
+      <c r="F42" s="204"/>
+      <c r="G42" s="142"/>
+      <c r="M42" s="205"/>
+      <c r="N42" s="206" t="s">
+        <v>96</v>
+      </c>
+      <c r="O42" s="206" t="s">
+        <v>96</v>
+      </c>
+      <c r="P42" s="206" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="43" spans="1:18" ht="14.25">
-      <c r="A43" s="212"/>
-      <c r="B43" s="213"/>
-      <c r="C43" s="214"/>
-      <c r="D43" s="214"/>
-      <c r="E43" s="214"/>
-      <c r="F43" s="214"/>
-      <c r="G43" s="151"/>
-      <c r="H43" s="142"/>
-      <c r="I43" s="142"/>
-      <c r="M43" s="215"/>
-      <c r="N43" s="216" t="s">
-        <v>96</v>
-      </c>
-      <c r="O43" s="216" t="s">
-        <v>96</v>
-      </c>
-      <c r="P43" s="216" t="s">
+      <c r="A43" s="202"/>
+      <c r="B43" s="203"/>
+      <c r="C43" s="204"/>
+      <c r="D43" s="204"/>
+      <c r="E43" s="204"/>
+      <c r="F43" s="204"/>
+      <c r="G43" s="142"/>
+      <c r="H43" s="133"/>
+      <c r="I43" s="133"/>
+      <c r="M43" s="205"/>
+      <c r="N43" s="206" t="s">
+        <v>96</v>
+      </c>
+      <c r="O43" s="206" t="s">
+        <v>96</v>
+      </c>
+      <c r="P43" s="206" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="44" spans="1:18" ht="6" customHeight="1"/>
     <row r="45" spans="1:18" ht="15.75">
-      <c r="A45" s="141" t="s">
+      <c r="A45" s="132" t="s">
         <v>105</v>
       </c>
-      <c r="B45" s="140"/>
-      <c r="C45" s="140"/>
-      <c r="D45" s="140"/>
-      <c r="E45" s="140"/>
-      <c r="F45" s="140"/>
-      <c r="G45" s="140"/>
-      <c r="H45" s="140"/>
-      <c r="I45" s="140"/>
-      <c r="J45" s="140"/>
-      <c r="K45" s="140"/>
-      <c r="L45" s="140"/>
-      <c r="M45" s="140"/>
-      <c r="N45" s="140"/>
-      <c r="O45" s="140"/>
-      <c r="P45" s="140"/>
+      <c r="B45" s="131"/>
+      <c r="C45" s="131"/>
+      <c r="D45" s="131"/>
+      <c r="E45" s="131"/>
+      <c r="F45" s="131"/>
+      <c r="G45" s="131"/>
+      <c r="H45" s="131"/>
+      <c r="I45" s="131"/>
+      <c r="J45" s="131"/>
+      <c r="K45" s="131"/>
+      <c r="L45" s="131"/>
+      <c r="M45" s="131"/>
+      <c r="N45" s="131"/>
+      <c r="O45" s="131"/>
+      <c r="P45" s="131"/>
     </row>
     <row r="46" spans="1:18" ht="5.25" customHeight="1"/>
     <row r="47" spans="1:18">
-      <c r="A47" s="150" t="s">
+      <c r="A47" s="141" t="s">
         <v>104</v>
       </c>
-      <c r="B47" s="150"/>
-      <c r="C47" s="150" t="s">
+      <c r="B47" s="141"/>
+      <c r="C47" s="141" t="s">
         <v>103</v>
       </c>
-      <c r="D47" s="150"/>
-      <c r="E47" s="150" t="s">
+      <c r="D47" s="141"/>
+      <c r="E47" s="141" t="s">
         <v>102</v>
       </c>
-      <c r="F47" s="150"/>
-      <c r="G47" s="150" t="s">
+      <c r="F47" s="141"/>
+      <c r="G47" s="141" t="s">
         <v>101</v>
       </c>
-      <c r="H47" s="150"/>
-      <c r="I47" s="150" t="s">
+      <c r="H47" s="141"/>
+      <c r="I47" s="141" t="s">
         <v>100</v>
       </c>
-      <c r="J47" s="150"/>
-      <c r="K47" s="150" t="s">
+      <c r="J47" s="141"/>
+      <c r="K47" s="141" t="s">
         <v>5</v>
       </c>
-      <c r="L47" s="150"/>
-      <c r="M47" s="150" t="s">
+      <c r="L47" s="141"/>
+      <c r="M47" s="141" t="s">
         <v>99</v>
       </c>
-      <c r="N47" s="150"/>
-      <c r="O47" s="150" t="s">
+      <c r="N47" s="141"/>
+      <c r="O47" s="141" t="s">
         <v>98</v>
       </c>
-      <c r="P47" s="150"/>
+      <c r="P47" s="141"/>
     </row>
     <row r="48" spans="1:18">
-      <c r="A48" s="149"/>
-      <c r="B48" s="149"/>
-      <c r="C48" s="148" t="s">
-        <v>96</v>
-      </c>
-      <c r="D48" s="148"/>
-      <c r="E48" s="148" t="s">
-        <v>96</v>
-      </c>
-      <c r="F48" s="148"/>
-      <c r="G48" s="148" t="s">
-        <v>96</v>
-      </c>
-      <c r="H48" s="148"/>
-      <c r="I48" s="148" t="s">
-        <v>96</v>
-      </c>
-      <c r="J48" s="148"/>
-      <c r="K48" s="148" t="s">
-        <v>96</v>
-      </c>
-      <c r="L48" s="148"/>
-      <c r="M48" s="148" t="s">
-        <v>96</v>
-      </c>
-      <c r="N48" s="148"/>
-      <c r="O48" s="148" t="s">
-        <v>96</v>
-      </c>
-      <c r="P48" s="148"/>
+      <c r="A48" s="140"/>
+      <c r="B48" s="140"/>
+      <c r="C48" s="139" t="s">
+        <v>96</v>
+      </c>
+      <c r="D48" s="139"/>
+      <c r="E48" s="139" t="s">
+        <v>96</v>
+      </c>
+      <c r="F48" s="139"/>
+      <c r="G48" s="139" t="s">
+        <v>96</v>
+      </c>
+      <c r="H48" s="139"/>
+      <c r="I48" s="139" t="s">
+        <v>96</v>
+      </c>
+      <c r="J48" s="139"/>
+      <c r="K48" s="139" t="s">
+        <v>96</v>
+      </c>
+      <c r="L48" s="139"/>
+      <c r="M48" s="139" t="s">
+        <v>96</v>
+      </c>
+      <c r="N48" s="139"/>
+      <c r="O48" s="139" t="s">
+        <v>96</v>
+      </c>
+      <c r="P48" s="139"/>
     </row>
     <row r="49" spans="1:16">
-      <c r="B49" s="147" t="s">
+      <c r="B49" s="138" t="s">
         <v>97</v>
       </c>
-      <c r="C49" s="146" t="s">
-        <v>96</v>
-      </c>
-      <c r="D49" s="143"/>
-      <c r="E49" s="143" t="s">
-        <v>96</v>
-      </c>
-      <c r="F49" s="143"/>
-      <c r="G49" s="145" t="s">
-        <v>96</v>
-      </c>
-      <c r="H49" s="145"/>
-      <c r="I49" s="145" t="s">
-        <v>96</v>
-      </c>
-      <c r="J49" s="145"/>
-      <c r="K49" s="144"/>
-      <c r="L49" s="143"/>
-      <c r="M49" s="142"/>
-      <c r="N49" s="142"/>
-      <c r="O49" s="142"/>
-      <c r="P49" s="142"/>
+      <c r="C49" s="137" t="s">
+        <v>96</v>
+      </c>
+      <c r="D49" s="134"/>
+      <c r="E49" s="134" t="s">
+        <v>96</v>
+      </c>
+      <c r="F49" s="134"/>
+      <c r="G49" s="136" t="s">
+        <v>96</v>
+      </c>
+      <c r="H49" s="136"/>
+      <c r="I49" s="136" t="s">
+        <v>96</v>
+      </c>
+      <c r="J49" s="136"/>
+      <c r="K49" s="135"/>
+      <c r="L49" s="134"/>
+      <c r="M49" s="133"/>
+      <c r="N49" s="133"/>
+      <c r="O49" s="133"/>
+      <c r="P49" s="133"/>
     </row>
     <row r="50" spans="1:16" ht="5.25" customHeight="1">
-      <c r="K50" s="138"/>
+      <c r="K50" s="129"/>
     </row>
     <row r="51" spans="1:16" ht="15.75">
-      <c r="A51" s="141" t="s">
+      <c r="A51" s="132" t="s">
         <v>95</v>
       </c>
-      <c r="B51" s="140"/>
-      <c r="C51" s="140"/>
-      <c r="D51" s="140"/>
-      <c r="E51" s="140"/>
-      <c r="F51" s="140"/>
-      <c r="G51" s="140"/>
-      <c r="H51" s="140"/>
-      <c r="I51" s="140"/>
-      <c r="J51" s="140"/>
-      <c r="K51" s="140"/>
-      <c r="L51" s="140"/>
-      <c r="M51" s="140"/>
-      <c r="N51" s="140"/>
-      <c r="O51" s="140"/>
-      <c r="P51" s="140"/>
+      <c r="B51" s="131"/>
+      <c r="C51" s="131"/>
+      <c r="D51" s="131"/>
+      <c r="E51" s="131"/>
+      <c r="F51" s="131"/>
+      <c r="G51" s="131"/>
+      <c r="H51" s="131"/>
+      <c r="I51" s="131"/>
+      <c r="J51" s="131"/>
+      <c r="K51" s="131"/>
+      <c r="L51" s="131"/>
+      <c r="M51" s="131"/>
+      <c r="N51" s="131"/>
+      <c r="O51" s="131"/>
+      <c r="P51" s="131"/>
     </row>
     <row r="52" spans="1:16" ht="5.25" customHeight="1"/>
     <row r="53" spans="1:16">
-      <c r="A53" s="139"/>
+      <c r="A53" s="130"/>
     </row>
     <row r="55" spans="1:16">
-      <c r="A55" s="138"/>
+      <c r="A55" s="129"/>
     </row>
     <row r="68" spans="1:1">
-      <c r="A68" s="137"/>
+      <c r="A68" s="128"/>
     </row>
     <row r="70" spans="1:1">
-      <c r="A70" s="137" t="s">
+      <c r="A70" s="128" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="71" spans="1:1">
-      <c r="A71" s="137"/>
+      <c r="A71" s="128"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>

<commit_message>
new FT pour LoA et Str
</commit_message>
<xml_diff>
--- a/lib/PHPExcel/templates/FT Loa.xlsx
+++ b/lib/PHPExcel/templates/FT Loa.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19226"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GPM\www\GPM\lib\PHPExcel\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{5A005903-52FA-461C-AB28-6449801FD071}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="0" windowWidth="9645" windowHeight="11955" activeTab="1"/>
+    <workbookView xWindow="15" yWindow="0" windowWidth="9645" windowHeight="11955" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FTLCFHCFEFF" sheetId="2" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="186">
   <si>
     <t>DONNEES EPROUVETTE</t>
   </si>
@@ -777,11 +778,20 @@
   <si>
     <t>Starting Time</t>
   </si>
+  <si>
+    <t>La règle le definissant est &lt; 35°C.</t>
+  </si>
+  <si>
+    <t>Dans le cas d'un essai &lt;35°C mais avec un suivi ou control strap, certains champs gris doivent être utilisés/remplis.</t>
+  </si>
+  <si>
+    <t>Special Instructions</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="6">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0.000"/>
@@ -790,7 +800,7 @@
     <numFmt numFmtId="168" formatCode="0.000"/>
     <numFmt numFmtId="169" formatCode="0.0"/>
   </numFmts>
-  <fonts count="39">
+  <fonts count="42">
     <font>
       <sz val="10"/>
       <name val="MS Sans Serif"/>
@@ -901,13 +911,6 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF223962"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="7"/>
       <color rgb="FF8497B0"/>
       <name val="Arial"/>
@@ -985,13 +988,6 @@
       <charset val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="8"/>
-      <color theme="3" tint="-0.499984740745262"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <vertAlign val="subscript"/>
       <sz val="7"/>
       <color rgb="FF8497B0"/>
@@ -1025,6 +1021,41 @@
     <font>
       <sz val="14"/>
       <color rgb="FF44546A"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="8"/>
+      <color rgb="FF203764"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF223962"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF203764"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="8"/>
+      <color theme="3" tint="-0.499984740745262"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1517,7 +1548,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="224">
+  <cellXfs count="229">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -1816,89 +1847,76 @@
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="22" fontId="18" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="18" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="34" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="20" fillId="0" borderId="32" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="34" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="1" fontId="21" fillId="0" borderId="32" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1907,130 +1925,133 @@
     <xf numFmtId="0" fontId="16" fillId="4" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="169" fontId="20" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="38" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="20" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="28" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="36" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="169" fontId="21" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="38" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="21" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="28" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="36" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="40" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="34" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="36" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="29" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="168" fontId="20" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="39" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="40" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="34" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="36" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="21" fillId="0" borderId="29" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="168" fontId="21" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" shrinkToFit="1"/>
+      <alignment horizontal="right" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2057,14 +2078,37 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" textRotation="90"/>
+    </xf>
+    <xf numFmtId="1" fontId="38" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="2" fontId="38" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="22" fontId="38" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Normal 3" xfId="2"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -2675,13 +2719,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Feuil1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:S60"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleNormal="98" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A16" zoomScaleNormal="98" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="M28" sqref="M28:M30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
@@ -2708,20 +2754,20 @@
     </row>
     <row r="4" spans="1:14" ht="13.5" thickBot="1"/>
     <row r="5" spans="1:14" ht="13.5" thickBot="1">
-      <c r="A5" s="214" t="s">
+      <c r="A5" s="210" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="215"/>
-      <c r="C5" s="215"/>
-      <c r="D5" s="215"/>
-      <c r="E5" s="215"/>
-      <c r="F5" s="216"/>
-      <c r="H5" s="214" t="s">
+      <c r="B5" s="211"/>
+      <c r="C5" s="211"/>
+      <c r="D5" s="211"/>
+      <c r="E5" s="211"/>
+      <c r="F5" s="212"/>
+      <c r="H5" s="210" t="s">
         <v>1</v>
       </c>
-      <c r="I5" s="215"/>
-      <c r="J5" s="215"/>
-      <c r="K5" s="216"/>
+      <c r="I5" s="211"/>
+      <c r="J5" s="211"/>
+      <c r="K5" s="212"/>
     </row>
     <row r="6" spans="1:14" ht="6.75" customHeight="1">
       <c r="A6" s="12"/>
@@ -2808,13 +2854,13 @@
       <c r="K11" s="60"/>
     </row>
     <row r="12" spans="1:14" ht="13.5" thickBot="1">
-      <c r="A12" s="214" t="s">
+      <c r="A12" s="210" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="215"/>
-      <c r="C12" s="215"/>
-      <c r="D12" s="215"/>
-      <c r="E12" s="215"/>
+      <c r="B12" s="211"/>
+      <c r="C12" s="211"/>
+      <c r="D12" s="211"/>
+      <c r="E12" s="211"/>
       <c r="F12" s="23"/>
       <c r="H12" s="18" t="s">
         <v>8</v>
@@ -2881,12 +2927,12 @@
       </c>
       <c r="E16" s="24"/>
       <c r="F16" s="62"/>
-      <c r="H16" s="214" t="s">
+      <c r="H16" s="210" t="s">
         <v>15</v>
       </c>
-      <c r="I16" s="215"/>
-      <c r="J16" s="215"/>
-      <c r="K16" s="216"/>
+      <c r="I16" s="211"/>
+      <c r="J16" s="211"/>
+      <c r="K16" s="212"/>
       <c r="N16" s="24"/>
     </row>
     <row r="17" spans="1:14">
@@ -2947,14 +2993,14 @@
       <c r="K20" s="86"/>
     </row>
     <row r="21" spans="1:14" ht="13.5" thickBot="1">
-      <c r="A21" s="214" t="s">
+      <c r="A21" s="210" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="215"/>
-      <c r="C21" s="215"/>
-      <c r="D21" s="215"/>
-      <c r="E21" s="215"/>
-      <c r="F21" s="216"/>
+      <c r="B21" s="211"/>
+      <c r="C21" s="211"/>
+      <c r="D21" s="211"/>
+      <c r="E21" s="211"/>
+      <c r="F21" s="212"/>
       <c r="H21" s="6"/>
       <c r="I21" s="87"/>
       <c r="J21" s="53" t="s">
@@ -3171,10 +3217,10 @@
       <c r="K33" s="114"/>
     </row>
     <row r="34" spans="1:19" ht="13.5" thickBot="1">
-      <c r="A34" s="219" t="s">
+      <c r="A34" s="215" t="s">
         <v>67</v>
       </c>
-      <c r="B34" s="220"/>
+      <c r="B34" s="216"/>
       <c r="C34" s="35"/>
       <c r="D34" s="55" t="s">
         <v>65</v>
@@ -3273,19 +3319,19 @@
       <c r="O39" s="32"/>
     </row>
     <row r="40" spans="1:19" ht="13.5" thickBot="1">
-      <c r="A40" s="214" t="s">
+      <c r="A40" s="210" t="s">
         <v>42</v>
       </c>
-      <c r="B40" s="215"/>
-      <c r="C40" s="215"/>
-      <c r="D40" s="215"/>
-      <c r="E40" s="215"/>
-      <c r="F40" s="215"/>
-      <c r="G40" s="215"/>
-      <c r="H40" s="215"/>
-      <c r="I40" s="215"/>
-      <c r="J40" s="215"/>
-      <c r="K40" s="216"/>
+      <c r="B40" s="211"/>
+      <c r="C40" s="211"/>
+      <c r="D40" s="211"/>
+      <c r="E40" s="211"/>
+      <c r="F40" s="211"/>
+      <c r="G40" s="211"/>
+      <c r="H40" s="211"/>
+      <c r="I40" s="211"/>
+      <c r="J40" s="211"/>
+      <c r="K40" s="212"/>
       <c r="M40" s="32"/>
       <c r="N40" s="32"/>
       <c r="O40" s="32"/>
@@ -3348,21 +3394,21 @@
       <c r="S43" s="32"/>
     </row>
     <row r="44" spans="1:19" ht="13.5" thickBot="1">
-      <c r="A44" s="214" t="s">
+      <c r="A44" s="210" t="s">
         <v>43</v>
       </c>
-      <c r="B44" s="215"/>
-      <c r="C44" s="215"/>
-      <c r="D44" s="215"/>
-      <c r="E44" s="215"/>
-      <c r="F44" s="215"/>
-      <c r="G44" s="215"/>
-      <c r="H44" s="215"/>
-      <c r="I44" s="216"/>
-      <c r="J44" s="221" t="s">
+      <c r="B44" s="211"/>
+      <c r="C44" s="211"/>
+      <c r="D44" s="211"/>
+      <c r="E44" s="211"/>
+      <c r="F44" s="211"/>
+      <c r="G44" s="211"/>
+      <c r="H44" s="211"/>
+      <c r="I44" s="212"/>
+      <c r="J44" s="217" t="s">
         <v>87</v>
       </c>
-      <c r="K44" s="222"/>
+      <c r="K44" s="218"/>
     </row>
     <row r="45" spans="1:19">
       <c r="A45" s="18" t="s">
@@ -3458,8 +3504,8 @@
       <c r="G50" s="20"/>
       <c r="H50" s="20"/>
       <c r="I50" s="20"/>
-      <c r="J50" s="217"/>
-      <c r="K50" s="218"/>
+      <c r="J50" s="213"/>
+      <c r="K50" s="214"/>
     </row>
     <row r="51" spans="1:12" ht="13.5" thickBot="1"/>
     <row r="52" spans="1:12">
@@ -3603,11 +3649,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31:J34"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A21" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
@@ -3618,135 +3664,135 @@
     <col min="19" max="16384" width="10.85546875" style="126"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="24.75" hidden="1" customHeight="1"/>
-    <row r="2" spans="1:18" ht="60.4" customHeight="1">
-      <c r="C2" s="198" t="s">
+    <row r="1" spans="1:19" ht="24.75" hidden="1" customHeight="1"/>
+    <row r="2" spans="1:19" ht="60.4" customHeight="1">
+      <c r="C2" s="191" t="s">
         <v>177</v>
       </c>
-      <c r="D2" s="197"/>
-      <c r="E2" s="197"/>
-      <c r="F2" s="197"/>
-      <c r="G2" s="197"/>
-      <c r="H2" s="197"/>
-      <c r="I2" s="197"/>
-      <c r="J2" s="197"/>
-      <c r="K2" s="197"/>
-      <c r="L2" s="197"/>
-      <c r="M2" s="197"/>
-      <c r="N2" s="196"/>
-      <c r="O2" s="223" t="s">
+      <c r="D2" s="190"/>
+      <c r="E2" s="190"/>
+      <c r="F2" s="190"/>
+      <c r="G2" s="190"/>
+      <c r="H2" s="190"/>
+      <c r="I2" s="190"/>
+      <c r="J2" s="190"/>
+      <c r="K2" s="190"/>
+      <c r="L2" s="190"/>
+      <c r="M2" s="190"/>
+      <c r="N2" s="189"/>
+      <c r="O2" s="219" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="18" customHeight="1">
-      <c r="O3" s="223"/>
-    </row>
-    <row r="4" spans="1:18" ht="18" customHeight="1">
-      <c r="A4" s="192" t="s">
+    <row r="3" spans="1:19" ht="18" customHeight="1">
+      <c r="O3" s="219"/>
+    </row>
+    <row r="4" spans="1:19" ht="18" customHeight="1">
+      <c r="A4" s="185" t="s">
         <v>175</v>
       </c>
-      <c r="B4" s="192"/>
-      <c r="C4" s="149"/>
-      <c r="D4" s="192" t="s">
+      <c r="B4" s="185"/>
+      <c r="C4" s="145"/>
+      <c r="D4" s="185" t="s">
         <v>174</v>
       </c>
-      <c r="E4" s="141"/>
-      <c r="F4" s="149"/>
-      <c r="G4" s="192" t="s">
+      <c r="E4" s="137"/>
+      <c r="F4" s="145"/>
+      <c r="G4" s="185" t="s">
         <v>173</v>
       </c>
-      <c r="H4" s="192"/>
-      <c r="I4" s="195"/>
-      <c r="J4" s="192" t="s">
+      <c r="H4" s="185"/>
+      <c r="I4" s="188"/>
+      <c r="J4" s="185" t="s">
         <v>172</v>
       </c>
-      <c r="K4" s="192"/>
-      <c r="L4" s="195"/>
-      <c r="M4" s="192"/>
-      <c r="N4" s="194" t="s">
+      <c r="K4" s="185"/>
+      <c r="L4" s="188"/>
+      <c r="M4" s="185"/>
+      <c r="N4" s="187" t="s">
         <v>171</v>
       </c>
-      <c r="O4" s="223"/>
-    </row>
-    <row r="5" spans="1:18" ht="18.95" customHeight="1">
-      <c r="A5" s="170"/>
-      <c r="B5" s="170"/>
-      <c r="C5" s="170" t="s">
-        <v>96</v>
-      </c>
-      <c r="D5" s="170"/>
-      <c r="E5" s="170"/>
-      <c r="F5" s="170" t="s">
-        <v>96</v>
-      </c>
-      <c r="G5" s="170"/>
-      <c r="H5" s="170"/>
-      <c r="I5" s="170" t="s">
-        <v>96</v>
-      </c>
-      <c r="J5" s="170"/>
-      <c r="K5" s="170"/>
-      <c r="L5" s="170" t="s">
-        <v>96</v>
-      </c>
-      <c r="M5" s="170"/>
-      <c r="N5" s="170"/>
-      <c r="O5" s="223"/>
-    </row>
-    <row r="6" spans="1:18" ht="18.95" customHeight="1">
-      <c r="A6" s="192" t="s">
+      <c r="O4" s="219"/>
+    </row>
+    <row r="5" spans="1:19" ht="18.95" customHeight="1">
+      <c r="A5" s="164"/>
+      <c r="B5" s="164"/>
+      <c r="C5" s="164" t="s">
+        <v>96</v>
+      </c>
+      <c r="D5" s="164"/>
+      <c r="E5" s="164"/>
+      <c r="F5" s="164" t="s">
+        <v>96</v>
+      </c>
+      <c r="G5" s="164"/>
+      <c r="H5" s="164"/>
+      <c r="I5" s="164" t="s">
+        <v>96</v>
+      </c>
+      <c r="J5" s="164"/>
+      <c r="K5" s="164"/>
+      <c r="L5" s="164" t="s">
+        <v>96</v>
+      </c>
+      <c r="M5" s="164"/>
+      <c r="N5" s="164"/>
+      <c r="O5" s="219"/>
+    </row>
+    <row r="6" spans="1:19" ht="18.95" customHeight="1">
+      <c r="A6" s="185" t="s">
         <v>170</v>
       </c>
-      <c r="B6" s="192"/>
-      <c r="C6" s="149"/>
-      <c r="D6" s="192" t="s">
+      <c r="B6" s="185"/>
+      <c r="C6" s="145"/>
+      <c r="D6" s="185" t="s">
         <v>169</v>
       </c>
-      <c r="E6" s="192"/>
-      <c r="F6" s="149"/>
-      <c r="G6" s="192" t="s">
+      <c r="E6" s="185"/>
+      <c r="F6" s="145"/>
+      <c r="G6" s="185" t="s">
         <v>99</v>
       </c>
-      <c r="H6" s="141"/>
-      <c r="I6" s="193"/>
-      <c r="J6" s="192" t="s">
+      <c r="H6" s="137"/>
+      <c r="I6" s="186"/>
+      <c r="J6" s="185" t="s">
         <v>168</v>
       </c>
-      <c r="K6" s="141"/>
-      <c r="L6" s="191"/>
-      <c r="M6" s="141"/>
-      <c r="N6" s="190" t="s">
+      <c r="K6" s="137"/>
+      <c r="L6" s="184"/>
+      <c r="M6" s="137"/>
+      <c r="N6" s="183" t="s">
         <v>167</v>
       </c>
-      <c r="O6" s="223"/>
-    </row>
-    <row r="7" spans="1:18" ht="18.95" customHeight="1">
-      <c r="A7" s="170"/>
-      <c r="B7" s="170"/>
-      <c r="C7" s="170" t="s">
-        <v>96</v>
-      </c>
-      <c r="D7" s="170"/>
-      <c r="E7" s="170"/>
-      <c r="F7" s="170" t="s">
-        <v>96</v>
-      </c>
-      <c r="G7" s="170"/>
-      <c r="H7" s="170"/>
-      <c r="I7" s="170" t="s">
-        <v>96</v>
-      </c>
-      <c r="J7" s="170"/>
-      <c r="K7" s="170"/>
-      <c r="L7" s="170" t="s">
-        <v>96</v>
-      </c>
-      <c r="M7" s="170"/>
-      <c r="N7" s="170"/>
-      <c r="O7" s="223"/>
-    </row>
-    <row r="8" spans="1:18" ht="6" customHeight="1"/>
-    <row r="9" spans="1:18" ht="15" customHeight="1">
+      <c r="O6" s="219"/>
+    </row>
+    <row r="7" spans="1:19" ht="18.95" customHeight="1">
+      <c r="A7" s="164"/>
+      <c r="B7" s="164"/>
+      <c r="C7" s="164" t="s">
+        <v>96</v>
+      </c>
+      <c r="D7" s="164"/>
+      <c r="E7" s="164"/>
+      <c r="F7" s="164" t="s">
+        <v>96</v>
+      </c>
+      <c r="G7" s="164"/>
+      <c r="H7" s="164"/>
+      <c r="I7" s="164" t="s">
+        <v>96</v>
+      </c>
+      <c r="J7" s="164"/>
+      <c r="K7" s="164"/>
+      <c r="L7" s="164" t="s">
+        <v>96</v>
+      </c>
+      <c r="M7" s="164"/>
+      <c r="N7" s="164"/>
+      <c r="O7" s="219"/>
+    </row>
+    <row r="8" spans="1:19" ht="6" customHeight="1"/>
+    <row r="9" spans="1:19" ht="15" customHeight="1">
       <c r="A9" s="131" t="s">
         <v>166</v>
       </c>
@@ -3766,167 +3812,176 @@
       <c r="O9" s="131"/>
       <c r="P9" s="131"/>
     </row>
-    <row r="10" spans="1:18" ht="5.25" customHeight="1"/>
-    <row r="11" spans="1:18" s="148" customFormat="1">
-      <c r="A11" s="141" t="s">
+    <row r="10" spans="1:19" ht="5.25" customHeight="1"/>
+    <row r="11" spans="1:19" s="144" customFormat="1">
+      <c r="A11" s="137" t="s">
         <v>165</v>
       </c>
-      <c r="B11" s="141"/>
-      <c r="C11" s="141" t="s">
+      <c r="B11" s="137"/>
+      <c r="C11" s="137" t="s">
         <v>164</v>
       </c>
-      <c r="D11" s="141"/>
-      <c r="E11" s="141" t="s">
+      <c r="D11" s="137"/>
+      <c r="E11" s="137" t="s">
         <v>163</v>
       </c>
-      <c r="F11" s="141"/>
-      <c r="G11" s="141" t="s">
+      <c r="F11" s="137"/>
+      <c r="G11" s="137" t="s">
         <v>162</v>
       </c>
-      <c r="H11" s="141"/>
-      <c r="I11" s="189"/>
-      <c r="J11" s="147" t="s">
+      <c r="H11" s="137"/>
+      <c r="I11" s="182"/>
+      <c r="J11" s="143" t="s">
         <v>161</v>
       </c>
-      <c r="K11" s="147" t="s">
+      <c r="K11" s="143" t="s">
         <v>160</v>
       </c>
-      <c r="L11" s="147" t="s">
+      <c r="L11" s="143" t="s">
         <v>159</v>
       </c>
-      <c r="M11" s="147" t="s">
+      <c r="M11" s="143" t="s">
         <v>158</v>
       </c>
-      <c r="N11" s="147" t="s">
+      <c r="N11" s="143" t="s">
         <v>157</v>
       </c>
-      <c r="O11" s="147" t="s">
+      <c r="O11" s="143" t="s">
         <v>156</v>
       </c>
-      <c r="P11" s="146" t="s">
+      <c r="P11" s="142" t="s">
         <v>155</v>
       </c>
       <c r="Q11" s="129"/>
       <c r="R11" s="129"/>
-    </row>
-    <row r="12" spans="1:18" ht="14.25">
-      <c r="A12" s="170"/>
-      <c r="B12" s="170"/>
-      <c r="C12" s="170"/>
-      <c r="D12" s="170"/>
-      <c r="E12" s="170"/>
-      <c r="F12" s="170"/>
-      <c r="G12" s="151" t="s">
+      <c r="S11" s="144" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="14.25">
+      <c r="A12" s="164"/>
+      <c r="B12" s="164"/>
+      <c r="C12" s="164"/>
+      <c r="D12" s="164"/>
+      <c r="E12" s="164"/>
+      <c r="F12" s="164"/>
+      <c r="G12" s="147" t="s">
         <v>57</v>
       </c>
-      <c r="H12" s="140"/>
-      <c r="I12" s="188" t="s">
+      <c r="H12" s="136"/>
+      <c r="I12" s="181" t="s">
         <v>123</v>
       </c>
-      <c r="J12" s="186" t="s">
-        <v>96</v>
-      </c>
-      <c r="K12" s="186" t="s">
-        <v>96</v>
-      </c>
-      <c r="L12" s="186" t="s">
-        <v>96</v>
-      </c>
-      <c r="M12" s="186" t="s">
-        <v>96</v>
-      </c>
-      <c r="N12" s="186" t="s">
-        <v>96</v>
-      </c>
-      <c r="O12" s="186" t="s">
-        <v>96</v>
-      </c>
-      <c r="P12" s="185" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" s="148" customFormat="1">
-      <c r="A13" s="141" t="s">
+      <c r="J12" s="179" t="s">
+        <v>96</v>
+      </c>
+      <c r="K12" s="179" t="s">
+        <v>96</v>
+      </c>
+      <c r="L12" s="179" t="s">
+        <v>96</v>
+      </c>
+      <c r="M12" s="179" t="s">
+        <v>96</v>
+      </c>
+      <c r="N12" s="179" t="s">
+        <v>96</v>
+      </c>
+      <c r="O12" s="179" t="s">
+        <v>96</v>
+      </c>
+      <c r="P12" s="178" t="s">
+        <v>96</v>
+      </c>
+      <c r="S12" s="126" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" s="144" customFormat="1">
+      <c r="A13" s="137" t="s">
         <v>154</v>
       </c>
-      <c r="B13" s="141"/>
-      <c r="C13" s="141" t="s">
+      <c r="B13" s="137"/>
+      <c r="C13" s="137" t="s">
         <v>180</v>
       </c>
-      <c r="D13" s="141" t="s">
+      <c r="D13" s="137" t="s">
         <v>140</v>
       </c>
-      <c r="E13" s="141" t="s">
+      <c r="E13" s="137" t="s">
         <v>153</v>
       </c>
-      <c r="F13" s="141"/>
-      <c r="G13" s="141"/>
-      <c r="H13" s="141"/>
-      <c r="I13" s="187" t="s">
+      <c r="F13" s="137"/>
+      <c r="G13" s="137"/>
+      <c r="H13" s="137"/>
+      <c r="I13" s="180" t="s">
         <v>152</v>
       </c>
-      <c r="J13" s="186" t="s">
-        <v>96</v>
-      </c>
-      <c r="K13" s="186" t="s">
-        <v>96</v>
-      </c>
-      <c r="L13" s="186" t="s">
-        <v>96</v>
-      </c>
-      <c r="M13" s="186" t="s">
-        <v>96</v>
-      </c>
-      <c r="N13" s="186" t="s">
-        <v>96</v>
-      </c>
-      <c r="O13" s="186" t="s">
-        <v>96</v>
-      </c>
-      <c r="P13" s="185" t="s">
+      <c r="J13" s="179" t="s">
+        <v>96</v>
+      </c>
+      <c r="K13" s="179" t="s">
+        <v>96</v>
+      </c>
+      <c r="L13" s="179" t="s">
+        <v>96</v>
+      </c>
+      <c r="M13" s="179" t="s">
+        <v>96</v>
+      </c>
+      <c r="N13" s="179" t="s">
+        <v>96</v>
+      </c>
+      <c r="O13" s="179" t="s">
+        <v>96</v>
+      </c>
+      <c r="P13" s="178" t="s">
         <v>96</v>
       </c>
       <c r="Q13" s="129"/>
       <c r="R13" s="129"/>
-    </row>
-    <row r="14" spans="1:18" ht="14.25">
-      <c r="A14" s="170"/>
-      <c r="B14" s="170"/>
-      <c r="C14" s="205"/>
-      <c r="D14" s="205" t="s">
-        <v>96</v>
-      </c>
-      <c r="E14" s="170"/>
-      <c r="F14" s="170"/>
-      <c r="G14" s="170"/>
-      <c r="H14" s="170"/>
-      <c r="I14" s="184" t="s">
+      <c r="S13" s="144" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="14.25">
+      <c r="A14" s="164"/>
+      <c r="B14" s="164"/>
+      <c r="C14" s="198"/>
+      <c r="D14" s="198" t="s">
+        <v>96</v>
+      </c>
+      <c r="E14" s="164"/>
+      <c r="F14" s="164"/>
+      <c r="G14" s="164"/>
+      <c r="H14" s="164"/>
+      <c r="I14" s="177" t="s">
         <v>151</v>
       </c>
-      <c r="J14" s="183" t="s">
-        <v>96</v>
-      </c>
-      <c r="K14" s="183" t="s">
-        <v>96</v>
-      </c>
-      <c r="L14" s="183" t="s">
-        <v>96</v>
-      </c>
-      <c r="M14" s="183" t="s">
-        <v>96</v>
-      </c>
-      <c r="N14" s="183" t="s">
-        <v>96</v>
-      </c>
-      <c r="O14" s="183" t="s">
-        <v>96</v>
-      </c>
-      <c r="P14" s="182"/>
-    </row>
-    <row r="15" spans="1:18" ht="6" customHeight="1">
-      <c r="A15" s="181"/>
-    </row>
-    <row r="16" spans="1:18" ht="15" customHeight="1">
+      <c r="J14" s="176" t="s">
+        <v>96</v>
+      </c>
+      <c r="K14" s="176" t="s">
+        <v>96</v>
+      </c>
+      <c r="L14" s="176" t="s">
+        <v>96</v>
+      </c>
+      <c r="M14" s="176" t="s">
+        <v>96</v>
+      </c>
+      <c r="N14" s="176" t="s">
+        <v>96</v>
+      </c>
+      <c r="O14" s="176" t="s">
+        <v>96</v>
+      </c>
+      <c r="P14" s="175"/>
+    </row>
+    <row r="15" spans="1:19" ht="6" customHeight="1">
+      <c r="A15" s="174"/>
+    </row>
+    <row r="16" spans="1:19" ht="15" customHeight="1">
       <c r="A16" s="132" t="s">
         <v>150</v>
       </c>
@@ -3947,310 +4002,312 @@
       <c r="P16" s="131"/>
     </row>
     <row r="17" spans="1:21" ht="5.25" customHeight="1">
-      <c r="K17" s="172"/>
-      <c r="L17" s="172"/>
-      <c r="M17" s="172"/>
-      <c r="N17" s="172"/>
-    </row>
-    <row r="18" spans="1:21" s="148" customFormat="1">
-      <c r="A18" s="141" t="s">
+      <c r="K17" s="166"/>
+      <c r="L17" s="166"/>
+      <c r="M17" s="166"/>
+      <c r="N17" s="166"/>
+    </row>
+    <row r="18" spans="1:21" s="144" customFormat="1">
+      <c r="A18" s="137" t="s">
         <v>149</v>
       </c>
-      <c r="B18" s="141"/>
-      <c r="C18" s="141" t="s">
+      <c r="B18" s="137"/>
+      <c r="C18" s="137" t="s">
         <v>148</v>
       </c>
-      <c r="D18" s="141"/>
-      <c r="E18" s="141" t="s">
+      <c r="D18" s="137"/>
+      <c r="E18" s="137" t="s">
         <v>147</v>
       </c>
-      <c r="F18" s="141"/>
-      <c r="G18" s="141" t="s">
+      <c r="F18" s="137"/>
+      <c r="G18" s="137" t="s">
         <v>146</v>
       </c>
-      <c r="H18" s="141"/>
-      <c r="I18" s="141" t="s">
+      <c r="H18" s="137"/>
+      <c r="I18" s="137" t="s">
         <v>145</v>
       </c>
-      <c r="J18" s="141"/>
-      <c r="K18" s="141" t="s">
+      <c r="J18" s="137"/>
+      <c r="K18" s="137" t="s">
         <v>144</v>
       </c>
-      <c r="L18" s="141"/>
-      <c r="M18" s="141" t="s">
+      <c r="L18" s="137"/>
+      <c r="M18" s="137" t="s">
         <v>143</v>
       </c>
-      <c r="N18" s="141"/>
-      <c r="O18" s="141" t="s">
+      <c r="N18" s="137"/>
+      <c r="O18" s="137" t="s">
         <v>142</v>
       </c>
-      <c r="P18" s="141"/>
+      <c r="P18" s="137"/>
       <c r="Q18" s="129"/>
     </row>
     <row r="19" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A19" s="170"/>
-      <c r="B19" s="170"/>
-      <c r="C19" s="170"/>
-      <c r="D19" s="170"/>
-      <c r="E19" s="170"/>
-      <c r="F19" s="170"/>
-      <c r="G19" s="170"/>
-      <c r="H19" s="170"/>
-      <c r="I19" s="170"/>
-      <c r="J19" s="170"/>
-      <c r="K19" s="170"/>
-      <c r="L19" s="170"/>
-      <c r="M19" s="170"/>
-      <c r="N19" s="170"/>
-      <c r="O19" s="170"/>
-      <c r="P19" s="170"/>
+      <c r="A19" s="164"/>
+      <c r="B19" s="164"/>
+      <c r="C19" s="164"/>
+      <c r="D19" s="164"/>
+      <c r="E19" s="164"/>
+      <c r="F19" s="164"/>
+      <c r="G19" s="164"/>
+      <c r="H19" s="164"/>
+      <c r="I19" s="164"/>
+      <c r="J19" s="164"/>
+      <c r="K19" s="164"/>
+      <c r="L19" s="164"/>
+      <c r="M19" s="164"/>
+      <c r="N19" s="164"/>
+      <c r="O19" s="164"/>
+      <c r="P19" s="164"/>
       <c r="R19" s="126"/>
     </row>
     <row r="20" spans="1:21" hidden="1">
-      <c r="A20" s="140"/>
-      <c r="B20" s="140"/>
-      <c r="C20" s="140"/>
-      <c r="D20" s="140"/>
-      <c r="E20" s="141" t="s">
+      <c r="A20" s="136"/>
+      <c r="B20" s="136"/>
+      <c r="C20" s="136"/>
+      <c r="D20" s="136"/>
+      <c r="E20" s="137" t="s">
         <v>112</v>
       </c>
-      <c r="F20" s="141"/>
-      <c r="G20" s="141"/>
-      <c r="H20" s="141"/>
-      <c r="I20" s="149"/>
-      <c r="J20" s="140"/>
-      <c r="K20" s="140"/>
-      <c r="L20" s="140"/>
-      <c r="M20" s="180"/>
-      <c r="N20" s="140"/>
-      <c r="O20" s="140"/>
-      <c r="P20" s="140"/>
-      <c r="R20" s="140" t="s">
-        <v>96</v>
-      </c>
-      <c r="S20" s="140"/>
-      <c r="T20" s="140" t="s">
-        <v>96</v>
-      </c>
-      <c r="U20" s="140"/>
-    </row>
-    <row r="21" spans="1:21" s="148" customFormat="1">
-      <c r="A21" s="141"/>
-      <c r="B21" s="179" t="s">
+      <c r="F20" s="137"/>
+      <c r="G20" s="137"/>
+      <c r="H20" s="137"/>
+      <c r="I20" s="145"/>
+      <c r="J20" s="136"/>
+      <c r="K20" s="136"/>
+      <c r="L20" s="136"/>
+      <c r="M20" s="173"/>
+      <c r="N20" s="136"/>
+      <c r="O20" s="136"/>
+      <c r="P20" s="136"/>
+      <c r="R20" s="136" t="s">
+        <v>96</v>
+      </c>
+      <c r="S20" s="136"/>
+      <c r="T20" s="136" t="s">
+        <v>96</v>
+      </c>
+      <c r="U20" s="136"/>
+    </row>
+    <row r="21" spans="1:21" s="144" customFormat="1">
+      <c r="A21" s="137"/>
+      <c r="B21" s="172" t="s">
         <v>97</v>
       </c>
-      <c r="C21" s="141" t="s">
+      <c r="C21" s="137" t="s">
         <v>141</v>
       </c>
-      <c r="D21" s="141"/>
-      <c r="E21" s="141" t="s">
+      <c r="D21" s="137"/>
+      <c r="E21" s="137" t="s">
         <v>111</v>
       </c>
-      <c r="F21" s="141"/>
-      <c r="G21" s="141" t="s">
+      <c r="F21" s="137"/>
+      <c r="G21" s="137" t="s">
         <v>110</v>
       </c>
-      <c r="H21" s="141"/>
-      <c r="I21" s="178"/>
-      <c r="J21" s="177" t="s">
+      <c r="H21" s="137"/>
+      <c r="I21" s="171"/>
+      <c r="J21" s="170" t="s">
         <v>179</v>
       </c>
-      <c r="K21" s="208" t="s">
+      <c r="K21" s="200" t="s">
         <v>53</v>
       </c>
-      <c r="L21" s="209"/>
-      <c r="M21" s="208" t="s">
+      <c r="L21" s="201"/>
+      <c r="M21" s="200" t="s">
         <v>54</v>
       </c>
-      <c r="N21" s="209"/>
-      <c r="O21" s="141" t="s">
+      <c r="N21" s="201"/>
+      <c r="O21" s="137" t="s">
         <v>181</v>
       </c>
-      <c r="P21" s="141"/>
+      <c r="P21" s="137"/>
       <c r="Q21" s="129"/>
       <c r="R21" s="129"/>
     </row>
     <row r="22" spans="1:21">
-      <c r="A22" s="176" t="s">
+      <c r="A22" s="169" t="s">
         <v>139</v>
       </c>
-      <c r="B22" s="175" t="s">
-        <v>96</v>
-      </c>
-      <c r="C22" s="174" t="s">
-        <v>96</v>
-      </c>
-      <c r="D22" s="174"/>
-      <c r="E22" s="170"/>
-      <c r="F22" s="170"/>
-      <c r="G22" s="173"/>
-      <c r="H22" s="170"/>
-      <c r="I22" s="172" t="s">
-        <v>96</v>
-      </c>
-      <c r="J22" s="171" t="s">
+      <c r="B22" s="226" t="s">
+        <v>96</v>
+      </c>
+      <c r="C22" s="168" t="s">
+        <v>96</v>
+      </c>
+      <c r="D22" s="168"/>
+      <c r="E22" s="164"/>
+      <c r="F22" s="164"/>
+      <c r="G22" s="167"/>
+      <c r="H22" s="164"/>
+      <c r="I22" s="166" t="s">
+        <v>96</v>
+      </c>
+      <c r="J22" s="165" t="s">
         <v>138</v>
       </c>
-      <c r="K22" s="210" t="s">
-        <v>96</v>
-      </c>
-      <c r="L22" s="211"/>
-      <c r="M22" s="210" t="s">
-        <v>96</v>
-      </c>
-      <c r="N22" s="211"/>
-      <c r="O22" s="213" t="s">
-        <v>96</v>
-      </c>
-      <c r="P22" s="170"/>
+      <c r="K22" s="202" t="s">
+        <v>96</v>
+      </c>
+      <c r="L22" s="203"/>
+      <c r="M22" s="202" t="s">
+        <v>96</v>
+      </c>
+      <c r="N22" s="203"/>
+      <c r="O22" s="205" t="s">
+        <v>96</v>
+      </c>
+      <c r="P22" s="164"/>
     </row>
     <row r="23" spans="1:21" ht="15.75">
-      <c r="A23" s="138" t="s">
+      <c r="A23" s="134" t="s">
         <v>137</v>
       </c>
-      <c r="B23" s="169" t="s">
-        <v>96</v>
-      </c>
-      <c r="C23" s="165" t="s">
-        <v>96</v>
-      </c>
-      <c r="D23" s="165"/>
-      <c r="E23" s="168" t="s">
+      <c r="B23" s="227" t="s">
+        <v>96</v>
+      </c>
+      <c r="C23" s="160" t="s">
+        <v>96</v>
+      </c>
+      <c r="D23" s="160"/>
+      <c r="E23" s="163" t="s">
         <v>136</v>
       </c>
-      <c r="F23" s="168"/>
-      <c r="G23" s="167"/>
-      <c r="H23" s="168"/>
-      <c r="I23" s="167"/>
-      <c r="J23" s="166" t="s">
+      <c r="F23" s="163"/>
+      <c r="G23" s="162"/>
+      <c r="H23" s="163"/>
+      <c r="I23" s="162"/>
+      <c r="J23" s="161" t="s">
         <v>135</v>
       </c>
-      <c r="K23" s="165" t="s">
-        <v>96</v>
-      </c>
-      <c r="L23" s="165"/>
-      <c r="M23" s="165" t="s">
-        <v>96</v>
-      </c>
-      <c r="N23" s="165"/>
-      <c r="O23" s="165" t="s">
-        <v>96</v>
-      </c>
-      <c r="P23" s="165"/>
+      <c r="K23" s="160" t="s">
+        <v>96</v>
+      </c>
+      <c r="L23" s="160"/>
+      <c r="M23" s="160" t="s">
+        <v>96</v>
+      </c>
+      <c r="N23" s="160"/>
+      <c r="O23" s="160" t="s">
+        <v>96</v>
+      </c>
+      <c r="P23" s="160"/>
     </row>
     <row r="24" spans="1:21" ht="5.25" customHeight="1">
-      <c r="A24" s="144"/>
-      <c r="B24" s="143"/>
-      <c r="C24" s="143"/>
-      <c r="D24" s="143"/>
-      <c r="E24" s="143"/>
-      <c r="F24" s="143"/>
-      <c r="G24" s="143"/>
-      <c r="H24" s="143"/>
-      <c r="I24" s="143"/>
-      <c r="J24" s="143"/>
-      <c r="K24" s="142"/>
-      <c r="L24" s="142"/>
-      <c r="M24" s="142"/>
-      <c r="N24" s="142"/>
-      <c r="O24" s="142"/>
-      <c r="P24" s="142"/>
+      <c r="A24" s="140"/>
+      <c r="B24" s="139"/>
+      <c r="C24" s="139"/>
+      <c r="D24" s="139"/>
+      <c r="E24" s="139"/>
+      <c r="F24" s="139"/>
+      <c r="G24" s="139"/>
+      <c r="H24" s="139"/>
+      <c r="I24" s="139"/>
+      <c r="J24" s="139"/>
+      <c r="K24" s="138"/>
+      <c r="L24" s="138"/>
+      <c r="M24" s="138"/>
+      <c r="N24" s="138"/>
+      <c r="O24" s="138"/>
+      <c r="P24" s="138"/>
     </row>
     <row r="25" spans="1:21">
-      <c r="A25" s="144" t="s">
+      <c r="A25" s="140" t="s">
         <v>134</v>
       </c>
-      <c r="B25" s="144"/>
-      <c r="C25" s="144" t="s">
+      <c r="B25" s="140"/>
+      <c r="C25" s="140" t="s">
         <v>133</v>
       </c>
-      <c r="D25" s="164"/>
-      <c r="E25" s="144" t="s">
+      <c r="D25" s="159"/>
+      <c r="E25" s="140" t="s">
         <v>132</v>
       </c>
-      <c r="F25" s="144"/>
-      <c r="G25" s="164"/>
-      <c r="H25" s="163" t="s">
+      <c r="F25" s="140"/>
+      <c r="G25" s="159"/>
+      <c r="H25" s="158" t="s">
         <v>131</v>
       </c>
-      <c r="I25" s="163"/>
-      <c r="J25" s="141" t="s">
+      <c r="I25" s="158"/>
+      <c r="J25" s="137" t="s">
         <v>81</v>
       </c>
-      <c r="K25" s="141"/>
-      <c r="L25" s="144" t="s">
+      <c r="K25" s="137"/>
+      <c r="L25" s="140" t="s">
         <v>130</v>
       </c>
-      <c r="M25" s="144"/>
-      <c r="N25" s="144"/>
-      <c r="O25" s="144"/>
-      <c r="P25" s="144"/>
+      <c r="M25" s="140"/>
+      <c r="N25" s="140"/>
+      <c r="O25" s="140"/>
+      <c r="P25" s="140"/>
     </row>
     <row r="26" spans="1:21">
-      <c r="A26" s="144" t="s">
+      <c r="A26" s="140" t="s">
         <v>40</v>
       </c>
-      <c r="B26" s="151" t="s">
+      <c r="B26" s="147" t="s">
         <v>57</v>
       </c>
-      <c r="C26" s="139" t="s">
-        <v>96</v>
-      </c>
-      <c r="D26" s="139" t="s">
-        <v>96</v>
-      </c>
-      <c r="E26" s="139" t="s">
-        <v>96</v>
-      </c>
-      <c r="F26" s="139"/>
-      <c r="G26" s="139"/>
-      <c r="H26" s="139" t="s">
-        <v>96</v>
-      </c>
-      <c r="I26" s="139"/>
-      <c r="J26" s="139" t="s">
-        <v>96</v>
-      </c>
-      <c r="K26" s="139"/>
-      <c r="L26" s="144" t="s">
+      <c r="C26" s="135" t="s">
+        <v>96</v>
+      </c>
+      <c r="D26" s="135" t="s">
+        <v>96</v>
+      </c>
+      <c r="E26" s="135" t="s">
+        <v>96</v>
+      </c>
+      <c r="F26" s="135"/>
+      <c r="G26" s="135"/>
+      <c r="H26" s="135" t="s">
+        <v>96</v>
+      </c>
+      <c r="I26" s="135"/>
+      <c r="J26" s="135" t="s">
+        <v>96</v>
+      </c>
+      <c r="K26" s="135"/>
+      <c r="L26" s="140" t="s">
         <v>108</v>
       </c>
-      <c r="M26" s="144"/>
-      <c r="N26" s="145" t="s">
+      <c r="M26" s="140"/>
+      <c r="N26" s="141" t="s">
         <v>107</v>
       </c>
-      <c r="O26" s="144" t="s">
+      <c r="O26" s="140" t="s">
         <v>106</v>
       </c>
-      <c r="P26" s="144"/>
+      <c r="P26" s="140"/>
     </row>
     <row r="27" spans="1:21">
-      <c r="A27" s="144" t="s">
+      <c r="A27" s="140" t="s">
         <v>129</v>
       </c>
-      <c r="B27" s="151" t="s">
+      <c r="B27" s="147" t="s">
         <v>57</v>
       </c>
-      <c r="C27" s="162"/>
-      <c r="D27" s="162"/>
-      <c r="E27" s="162"/>
-      <c r="F27" s="162"/>
-      <c r="G27" s="162"/>
-      <c r="H27" s="162"/>
-      <c r="I27" s="162"/>
-      <c r="J27" s="161"/>
-      <c r="K27" s="161"/>
-      <c r="L27" s="139" t="s">
-        <v>96</v>
-      </c>
-      <c r="M27" s="139" t="s">
-        <v>96</v>
-      </c>
-      <c r="N27" s="139" t="s">
-        <v>96</v>
-      </c>
-      <c r="O27" s="139"/>
-      <c r="P27" s="160"/>
+      <c r="C27" s="157"/>
+      <c r="D27" s="157"/>
+      <c r="E27" s="157"/>
+      <c r="F27" s="157"/>
+      <c r="G27" s="157"/>
+      <c r="H27" s="157"/>
+      <c r="I27" s="157"/>
+      <c r="J27" s="228" t="s">
+        <v>96</v>
+      </c>
+      <c r="K27" s="228"/>
+      <c r="L27" s="135" t="s">
+        <v>96</v>
+      </c>
+      <c r="M27" s="135" t="s">
+        <v>96</v>
+      </c>
+      <c r="N27" s="135" t="s">
+        <v>96</v>
+      </c>
+      <c r="O27" s="135"/>
+      <c r="P27" s="156"/>
     </row>
     <row r="28" spans="1:21" ht="6" customHeight="1"/>
     <row r="29" spans="1:21" ht="15.75">
@@ -4274,140 +4331,140 @@
       <c r="P29" s="131"/>
     </row>
     <row r="30" spans="1:21" ht="5.25" customHeight="1">
-      <c r="K30" s="149"/>
-      <c r="L30" s="149"/>
-      <c r="M30" s="149"/>
-      <c r="N30" s="149"/>
-      <c r="O30" s="149"/>
-      <c r="P30" s="149"/>
+      <c r="K30" s="145"/>
+      <c r="L30" s="145"/>
+      <c r="M30" s="145"/>
+      <c r="N30" s="145"/>
+      <c r="O30" s="145"/>
+      <c r="P30" s="145"/>
     </row>
     <row r="31" spans="1:21" ht="14.25">
-      <c r="A31" s="159" t="s">
+      <c r="A31" s="155" t="s">
         <v>127</v>
       </c>
-      <c r="B31" s="147" t="s">
+      <c r="B31" s="143" t="s">
         <v>53</v>
       </c>
-      <c r="C31" s="147" t="s">
+      <c r="C31" s="143" t="s">
         <v>54</v>
       </c>
-      <c r="H31" s="144" t="s">
+      <c r="H31" s="140" t="s">
         <v>126</v>
       </c>
-      <c r="I31" s="144"/>
-      <c r="J31" s="144"/>
-      <c r="K31" s="141" t="s">
+      <c r="I31" s="140"/>
+      <c r="J31" s="140"/>
+      <c r="K31" s="137" t="s">
         <v>125</v>
       </c>
-      <c r="L31" s="141"/>
-      <c r="M31" s="141" t="s">
+      <c r="L31" s="137"/>
+      <c r="M31" s="137" t="s">
         <v>60</v>
       </c>
-      <c r="N31" s="141"/>
-      <c r="O31" s="141" t="s">
+      <c r="N31" s="137"/>
+      <c r="O31" s="137" t="s">
         <v>124</v>
       </c>
-      <c r="P31" s="141"/>
+      <c r="P31" s="137"/>
     </row>
     <row r="32" spans="1:21">
-      <c r="A32" s="155" t="s">
+      <c r="A32" s="151" t="s">
         <v>123</v>
       </c>
-      <c r="B32" s="158" t="s">
-        <v>96</v>
-      </c>
-      <c r="C32" s="158" t="s">
-        <v>96</v>
-      </c>
-      <c r="D32" s="207" t="s">
+      <c r="B32" s="154" t="s">
+        <v>96</v>
+      </c>
+      <c r="C32" s="154" t="s">
+        <v>96</v>
+      </c>
+      <c r="D32" s="199" t="s">
         <v>122</v>
       </c>
-      <c r="E32" s="141" t="s">
+      <c r="E32" s="137" t="s">
         <v>182</v>
       </c>
-      <c r="F32" s="141"/>
-      <c r="H32" s="157" t="s">
+      <c r="F32" s="137"/>
+      <c r="H32" s="153" t="s">
         <v>121</v>
       </c>
-      <c r="I32" s="141"/>
-      <c r="J32" s="156" t="s">
+      <c r="I32" s="137"/>
+      <c r="J32" s="152" t="s">
         <v>120</v>
       </c>
-      <c r="K32" s="151" t="s">
+      <c r="K32" s="147" t="s">
         <v>57</v>
       </c>
-      <c r="L32" s="140"/>
-      <c r="M32" s="151" t="s">
+      <c r="L32" s="136"/>
+      <c r="M32" s="147" t="s">
         <v>57</v>
       </c>
-      <c r="N32" s="140"/>
-      <c r="O32" s="151" t="s">
+      <c r="N32" s="136"/>
+      <c r="O32" s="147" t="s">
         <v>57</v>
       </c>
-      <c r="P32" s="140"/>
+      <c r="P32" s="136"/>
     </row>
     <row r="33" spans="1:18" ht="14.25" customHeight="1">
-      <c r="A33" s="155" t="s">
+      <c r="A33" s="151" t="s">
         <v>109</v>
       </c>
-      <c r="B33" s="212" t="s">
-        <v>96</v>
-      </c>
-      <c r="C33" s="212" t="s">
-        <v>96</v>
-      </c>
-      <c r="D33" s="154" t="s">
+      <c r="B33" s="204" t="s">
+        <v>96</v>
+      </c>
+      <c r="C33" s="204" t="s">
+        <v>96</v>
+      </c>
+      <c r="D33" s="150" t="s">
         <v>19</v>
       </c>
-      <c r="E33" s="174" t="s">
-        <v>96</v>
-      </c>
-      <c r="F33" s="174"/>
-      <c r="H33" s="139"/>
-      <c r="I33" s="139" t="s">
+      <c r="E33" s="168" t="s">
+        <v>96</v>
+      </c>
+      <c r="F33" s="168"/>
+      <c r="H33" s="135"/>
+      <c r="I33" s="135" t="s">
         <v>119</v>
       </c>
-      <c r="J33" s="139" t="s">
-        <v>96</v>
-      </c>
-      <c r="K33" s="141" t="s">
+      <c r="J33" s="135" t="s">
+        <v>96</v>
+      </c>
+      <c r="K33" s="137" t="s">
         <v>118</v>
       </c>
-      <c r="L33" s="141"/>
-      <c r="M33" s="141" t="s">
+      <c r="L33" s="137"/>
+      <c r="M33" s="137" t="s">
         <v>88</v>
       </c>
-      <c r="N33" s="141"/>
-      <c r="O33" s="141" t="s">
+      <c r="N33" s="137"/>
+      <c r="O33" s="137" t="s">
         <v>117</v>
       </c>
-      <c r="P33" s="141"/>
+      <c r="P33" s="137"/>
     </row>
     <row r="34" spans="1:18">
-      <c r="A34" s="153" t="s">
+      <c r="A34" s="149" t="s">
         <v>116</v>
       </c>
-      <c r="B34" s="212" t="s">
-        <v>96</v>
-      </c>
-      <c r="C34" s="212" t="s">
-        <v>96</v>
-      </c>
-      <c r="D34" s="152" t="s">
+      <c r="B34" s="204" t="s">
+        <v>96</v>
+      </c>
+      <c r="C34" s="204" t="s">
+        <v>96</v>
+      </c>
+      <c r="D34" s="148" t="s">
         <v>115</v>
       </c>
-      <c r="K34" s="151" t="s">
+      <c r="K34" s="147" t="s">
         <v>57</v>
       </c>
-      <c r="L34" s="140"/>
-      <c r="M34" s="151" t="s">
+      <c r="L34" s="136"/>
+      <c r="M34" s="147" t="s">
         <v>57</v>
       </c>
-      <c r="N34" s="140"/>
-      <c r="O34" s="151" t="s">
+      <c r="N34" s="136"/>
+      <c r="O34" s="147" t="s">
         <v>57</v>
       </c>
-      <c r="P34" s="140"/>
+      <c r="P34" s="136"/>
     </row>
     <row r="35" spans="1:18" ht="6" customHeight="1">
       <c r="A35" s="129"/>
@@ -4434,232 +4491,232 @@
       <c r="P36" s="131"/>
     </row>
     <row r="37" spans="1:18" ht="5.25" customHeight="1"/>
-    <row r="38" spans="1:18" s="148" customFormat="1">
-      <c r="A38" s="150" t="s">
+    <row r="38" spans="1:18" s="144" customFormat="1">
+      <c r="A38" s="146" t="s">
         <v>114</v>
       </c>
-      <c r="B38" s="141"/>
-      <c r="C38" s="149"/>
-      <c r="D38" s="141" t="s">
+      <c r="B38" s="137"/>
+      <c r="C38" s="145"/>
+      <c r="D38" s="137" t="s">
         <v>113</v>
       </c>
-      <c r="E38" s="149"/>
-      <c r="F38" s="141" t="s">
+      <c r="E38" s="145"/>
+      <c r="F38" s="137" t="s">
         <v>5</v>
       </c>
-      <c r="G38" s="141"/>
-      <c r="H38" s="141" t="s">
+      <c r="G38" s="137"/>
+      <c r="H38" s="137" t="s">
         <v>99</v>
       </c>
-      <c r="I38" s="141"/>
-      <c r="K38" s="127"/>
-      <c r="L38" s="127"/>
-      <c r="M38" s="177"/>
-      <c r="N38" s="206"/>
-      <c r="O38" s="206"/>
-      <c r="P38" s="206"/>
+      <c r="I38" s="137"/>
+      <c r="K38" s="207"/>
+      <c r="L38" s="207"/>
+      <c r="M38" s="207"/>
+      <c r="N38" s="207"/>
+      <c r="O38" s="207"/>
+      <c r="P38" s="207"/>
       <c r="Q38" s="129"/>
       <c r="R38" s="129"/>
     </row>
-    <row r="39" spans="1:18" s="148" customFormat="1">
-      <c r="A39" s="150"/>
-      <c r="B39" s="141"/>
-      <c r="C39" s="149"/>
-      <c r="D39" s="141"/>
-      <c r="E39" s="149"/>
-      <c r="F39" s="141"/>
-      <c r="G39" s="141"/>
-      <c r="H39" s="141"/>
-      <c r="I39" s="141"/>
-      <c r="K39" s="127"/>
-      <c r="L39" s="127"/>
-      <c r="M39" s="177"/>
-      <c r="N39" s="206"/>
-      <c r="O39" s="206"/>
-      <c r="P39" s="206"/>
+    <row r="39" spans="1:18" s="144" customFormat="1">
+      <c r="A39" s="146"/>
+      <c r="B39" s="137"/>
+      <c r="C39" s="145"/>
+      <c r="D39" s="137"/>
+      <c r="E39" s="145"/>
+      <c r="F39" s="137"/>
+      <c r="G39" s="137"/>
+      <c r="H39" s="137"/>
+      <c r="I39" s="137"/>
+      <c r="K39" s="207"/>
+      <c r="L39" s="208"/>
+      <c r="M39" s="208"/>
+      <c r="N39" s="208"/>
+      <c r="O39" s="208"/>
+      <c r="P39" s="209"/>
       <c r="Q39" s="129"/>
       <c r="R39" s="129"/>
     </row>
-    <row r="40" spans="1:18" s="148" customFormat="1">
-      <c r="A40" s="150"/>
-      <c r="B40" s="141"/>
-      <c r="C40" s="149"/>
-      <c r="D40" s="141"/>
-      <c r="E40" s="149"/>
-      <c r="F40" s="141"/>
-      <c r="G40" s="141"/>
-      <c r="H40" s="141"/>
-      <c r="I40" s="141"/>
-      <c r="K40" s="127"/>
-      <c r="L40" s="127"/>
-      <c r="M40" s="177"/>
-      <c r="N40" s="206"/>
-      <c r="O40" s="206"/>
-      <c r="P40" s="206"/>
+    <row r="40" spans="1:18" s="144" customFormat="1">
+      <c r="A40" s="146"/>
+      <c r="B40" s="137"/>
+      <c r="C40" s="145"/>
+      <c r="D40" s="137"/>
+      <c r="E40" s="145"/>
+      <c r="F40" s="137"/>
+      <c r="G40" s="137"/>
+      <c r="H40" s="137"/>
+      <c r="I40" s="137"/>
+      <c r="K40" s="207"/>
+      <c r="L40" s="208"/>
+      <c r="M40" s="208"/>
+      <c r="N40" s="208"/>
+      <c r="O40" s="208"/>
+      <c r="P40" s="209"/>
       <c r="Q40" s="129"/>
       <c r="R40" s="129"/>
     </row>
-    <row r="41" spans="1:18" s="148" customFormat="1">
-      <c r="A41" s="150"/>
-      <c r="B41" s="141"/>
-      <c r="C41" s="149"/>
-      <c r="D41" s="141"/>
-      <c r="E41" s="149"/>
-      <c r="F41" s="141"/>
-      <c r="G41" s="141"/>
-      <c r="H41" s="141"/>
-      <c r="I41" s="141"/>
-      <c r="K41" s="127"/>
-      <c r="L41" s="127"/>
-      <c r="M41" s="177"/>
-      <c r="N41" s="206"/>
-      <c r="O41" s="206"/>
-      <c r="P41" s="206"/>
+    <row r="41" spans="1:18" s="144" customFormat="1">
+      <c r="A41" s="146"/>
+      <c r="B41" s="137"/>
+      <c r="C41" s="145"/>
+      <c r="D41" s="137"/>
+      <c r="E41" s="145"/>
+      <c r="F41" s="137"/>
+      <c r="G41" s="137"/>
+      <c r="H41" s="137"/>
+      <c r="I41" s="137"/>
+      <c r="K41" s="207"/>
+      <c r="L41" s="208"/>
+      <c r="M41" s="208"/>
+      <c r="N41" s="208"/>
+      <c r="O41" s="208"/>
+      <c r="P41" s="209"/>
       <c r="Q41" s="129"/>
       <c r="R41" s="129"/>
     </row>
-    <row r="42" spans="1:18" s="148" customFormat="1">
-      <c r="A42" s="150"/>
-      <c r="B42" s="141"/>
-      <c r="C42" s="149"/>
-      <c r="D42" s="141"/>
-      <c r="E42" s="149"/>
-      <c r="F42" s="141"/>
-      <c r="G42" s="141"/>
-      <c r="H42" s="141"/>
-      <c r="I42" s="141"/>
-      <c r="K42" s="127"/>
-      <c r="L42" s="127"/>
-      <c r="M42" s="177"/>
-      <c r="N42" s="206"/>
-      <c r="O42" s="206"/>
-      <c r="P42" s="206"/>
+    <row r="42" spans="1:18" s="144" customFormat="1">
+      <c r="A42" s="146"/>
+      <c r="B42" s="137"/>
+      <c r="C42" s="145"/>
+      <c r="D42" s="137"/>
+      <c r="E42" s="145"/>
+      <c r="F42" s="137"/>
+      <c r="G42" s="137"/>
+      <c r="H42" s="137"/>
+      <c r="I42" s="137"/>
+      <c r="K42" s="207"/>
+      <c r="L42" s="208"/>
+      <c r="M42" s="208"/>
+      <c r="N42" s="208"/>
+      <c r="O42" s="208"/>
+      <c r="P42" s="209"/>
       <c r="Q42" s="129"/>
       <c r="R42" s="129"/>
     </row>
-    <row r="43" spans="1:18" s="148" customFormat="1">
-      <c r="A43" s="150"/>
-      <c r="B43" s="141"/>
-      <c r="C43" s="149"/>
-      <c r="D43" s="141"/>
-      <c r="E43" s="149"/>
-      <c r="F43" s="141"/>
-      <c r="G43" s="141"/>
-      <c r="H43" s="141"/>
-      <c r="I43" s="141"/>
-      <c r="K43" s="127"/>
-      <c r="L43" s="127"/>
-      <c r="M43" s="177"/>
-      <c r="N43" s="206"/>
-      <c r="O43" s="206"/>
-      <c r="P43" s="206"/>
+    <row r="43" spans="1:18" s="144" customFormat="1">
+      <c r="A43" s="146"/>
+      <c r="B43" s="137"/>
+      <c r="C43" s="145"/>
+      <c r="D43" s="137"/>
+      <c r="E43" s="145"/>
+      <c r="F43" s="137"/>
+      <c r="G43" s="137"/>
+      <c r="H43" s="137"/>
+      <c r="I43" s="137"/>
+      <c r="K43" s="207"/>
+      <c r="L43" s="208"/>
+      <c r="M43" s="208"/>
+      <c r="N43" s="208"/>
+      <c r="O43" s="208"/>
+      <c r="P43" s="209"/>
       <c r="Q43" s="129"/>
       <c r="R43" s="129"/>
     </row>
     <row r="44" spans="1:18" hidden="1">
-      <c r="A44" s="140" t="s">
-        <v>96</v>
-      </c>
-      <c r="B44" s="140"/>
-      <c r="C44" s="140" t="s">
-        <v>96</v>
-      </c>
-      <c r="D44" s="140"/>
-      <c r="E44" s="140"/>
-      <c r="F44" s="139" t="s">
-        <v>96</v>
-      </c>
-      <c r="G44" s="139"/>
-      <c r="H44" s="139" t="s">
-        <v>96</v>
-      </c>
-      <c r="I44" s="139"/>
-      <c r="M44" s="204"/>
-      <c r="N44" s="205" t="s">
-        <v>96</v>
-      </c>
-      <c r="O44" s="205" t="s">
-        <v>96</v>
-      </c>
-      <c r="P44" s="205" t="s">
+      <c r="A44" s="136" t="s">
+        <v>96</v>
+      </c>
+      <c r="B44" s="136"/>
+      <c r="C44" s="136" t="s">
+        <v>96</v>
+      </c>
+      <c r="D44" s="136"/>
+      <c r="E44" s="136"/>
+      <c r="F44" s="135" t="s">
+        <v>96</v>
+      </c>
+      <c r="G44" s="135"/>
+      <c r="H44" s="135" t="s">
+        <v>96</v>
+      </c>
+      <c r="I44" s="135"/>
+      <c r="M44" s="197"/>
+      <c r="N44" s="198" t="s">
+        <v>96</v>
+      </c>
+      <c r="O44" s="198" t="s">
+        <v>96</v>
+      </c>
+      <c r="P44" s="198" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="45" spans="1:18" hidden="1">
-      <c r="A45" s="199"/>
-      <c r="B45" s="200"/>
-      <c r="C45" s="144"/>
-      <c r="D45" s="144"/>
-      <c r="E45" s="144"/>
-      <c r="F45" s="144"/>
-      <c r="G45" s="142"/>
-      <c r="M45" s="204"/>
-      <c r="N45" s="205" t="s">
-        <v>96</v>
-      </c>
-      <c r="O45" s="205" t="s">
-        <v>96</v>
-      </c>
-      <c r="P45" s="205" t="s">
+      <c r="A45" s="192"/>
+      <c r="B45" s="193"/>
+      <c r="C45" s="140"/>
+      <c r="D45" s="140"/>
+      <c r="E45" s="140"/>
+      <c r="F45" s="140"/>
+      <c r="G45" s="138"/>
+      <c r="M45" s="197"/>
+      <c r="N45" s="198" t="s">
+        <v>96</v>
+      </c>
+      <c r="O45" s="198" t="s">
+        <v>96</v>
+      </c>
+      <c r="P45" s="198" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="46" spans="1:18" hidden="1">
-      <c r="A46" s="199"/>
-      <c r="B46" s="200"/>
-      <c r="C46" s="144"/>
-      <c r="D46" s="144"/>
-      <c r="E46" s="144"/>
-      <c r="F46" s="144"/>
-      <c r="G46" s="142"/>
-      <c r="M46" s="204"/>
-      <c r="N46" s="205" t="s">
-        <v>96</v>
-      </c>
-      <c r="O46" s="205" t="s">
-        <v>96</v>
-      </c>
-      <c r="P46" s="205" t="s">
+      <c r="A46" s="192"/>
+      <c r="B46" s="193"/>
+      <c r="C46" s="140"/>
+      <c r="D46" s="140"/>
+      <c r="E46" s="140"/>
+      <c r="F46" s="140"/>
+      <c r="G46" s="138"/>
+      <c r="M46" s="197"/>
+      <c r="N46" s="198" t="s">
+        <v>96</v>
+      </c>
+      <c r="O46" s="198" t="s">
+        <v>96</v>
+      </c>
+      <c r="P46" s="198" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="47" spans="1:18" ht="14.25" hidden="1">
-      <c r="A47" s="201"/>
-      <c r="B47" s="202"/>
-      <c r="C47" s="203"/>
-      <c r="D47" s="203"/>
-      <c r="E47" s="203"/>
-      <c r="F47" s="203"/>
-      <c r="G47" s="142"/>
-      <c r="M47" s="204"/>
-      <c r="N47" s="205" t="s">
-        <v>96</v>
-      </c>
-      <c r="O47" s="205" t="s">
-        <v>96</v>
-      </c>
-      <c r="P47" s="205" t="s">
+      <c r="A47" s="194"/>
+      <c r="B47" s="195"/>
+      <c r="C47" s="196"/>
+      <c r="D47" s="196"/>
+      <c r="E47" s="196"/>
+      <c r="F47" s="196"/>
+      <c r="G47" s="138"/>
+      <c r="M47" s="197"/>
+      <c r="N47" s="198" t="s">
+        <v>96</v>
+      </c>
+      <c r="O47" s="198" t="s">
+        <v>96</v>
+      </c>
+      <c r="P47" s="198" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="48" spans="1:18" ht="14.25" hidden="1">
-      <c r="A48" s="201"/>
-      <c r="B48" s="202"/>
-      <c r="C48" s="203"/>
-      <c r="D48" s="203"/>
-      <c r="E48" s="203"/>
-      <c r="F48" s="203"/>
-      <c r="G48" s="142"/>
+      <c r="A48" s="194"/>
+      <c r="B48" s="195"/>
+      <c r="C48" s="196"/>
+      <c r="D48" s="196"/>
+      <c r="E48" s="196"/>
+      <c r="F48" s="196"/>
+      <c r="G48" s="138"/>
       <c r="H48" s="133"/>
       <c r="I48" s="133"/>
-      <c r="M48" s="204"/>
-      <c r="N48" s="205" t="s">
-        <v>96</v>
-      </c>
-      <c r="O48" s="205" t="s">
-        <v>96</v>
-      </c>
-      <c r="P48" s="205" t="s">
+      <c r="M48" s="197"/>
+      <c r="N48" s="198" t="s">
+        <v>96</v>
+      </c>
+      <c r="O48" s="198" t="s">
+        <v>96</v>
+      </c>
+      <c r="P48" s="198" t="s">
         <v>96</v>
       </c>
     </row>
@@ -4686,97 +4743,97 @@
     </row>
     <row r="51" spans="1:16" ht="5.25" customHeight="1"/>
     <row r="52" spans="1:16">
-      <c r="A52" s="141" t="s">
+      <c r="A52" s="137" t="s">
         <v>104</v>
       </c>
-      <c r="B52" s="141"/>
-      <c r="C52" s="141" t="s">
+      <c r="B52" s="137"/>
+      <c r="C52" s="137" t="s">
         <v>103</v>
       </c>
-      <c r="D52" s="141"/>
-      <c r="E52" s="141" t="s">
+      <c r="D52" s="137"/>
+      <c r="E52" s="137" t="s">
         <v>102</v>
       </c>
-      <c r="F52" s="141"/>
-      <c r="G52" s="141" t="s">
+      <c r="F52" s="137"/>
+      <c r="G52" s="137" t="s">
         <v>101</v>
       </c>
-      <c r="H52" s="141"/>
-      <c r="I52" s="141" t="s">
+      <c r="H52" s="137"/>
+      <c r="I52" s="137" t="s">
         <v>100</v>
       </c>
-      <c r="J52" s="141"/>
-      <c r="K52" s="141" t="s">
+      <c r="J52" s="137"/>
+      <c r="K52" s="137" t="s">
         <v>5</v>
       </c>
-      <c r="L52" s="141"/>
-      <c r="M52" s="141" t="s">
+      <c r="L52" s="137"/>
+      <c r="M52" s="137" t="s">
         <v>99</v>
       </c>
-      <c r="N52" s="141"/>
-      <c r="O52" s="141" t="s">
+      <c r="N52" s="137"/>
+      <c r="O52" s="137" t="s">
         <v>98</v>
       </c>
-      <c r="P52" s="141"/>
+      <c r="P52" s="137"/>
     </row>
     <row r="53" spans="1:16">
-      <c r="A53" s="140"/>
-      <c r="B53" s="140"/>
-      <c r="C53" s="139" t="s">
-        <v>96</v>
-      </c>
-      <c r="D53" s="139"/>
-      <c r="E53" s="139" t="s">
-        <v>96</v>
-      </c>
-      <c r="F53" s="139"/>
-      <c r="G53" s="139" t="s">
-        <v>96</v>
-      </c>
-      <c r="H53" s="139"/>
-      <c r="I53" s="139" t="s">
-        <v>96</v>
-      </c>
-      <c r="J53" s="139"/>
-      <c r="K53" s="139" t="s">
-        <v>96</v>
-      </c>
-      <c r="L53" s="139"/>
-      <c r="M53" s="139" t="s">
-        <v>96</v>
-      </c>
-      <c r="N53" s="139"/>
-      <c r="O53" s="139" t="s">
-        <v>96</v>
-      </c>
-      <c r="P53" s="139"/>
+      <c r="A53" s="136"/>
+      <c r="B53" s="136"/>
+      <c r="C53" s="135" t="s">
+        <v>96</v>
+      </c>
+      <c r="D53" s="135"/>
+      <c r="E53" s="135" t="s">
+        <v>96</v>
+      </c>
+      <c r="F53" s="135"/>
+      <c r="G53" s="135" t="s">
+        <v>96</v>
+      </c>
+      <c r="H53" s="135"/>
+      <c r="I53" s="135" t="s">
+        <v>96</v>
+      </c>
+      <c r="J53" s="135"/>
+      <c r="K53" s="135" t="s">
+        <v>96</v>
+      </c>
+      <c r="L53" s="135"/>
+      <c r="M53" s="135" t="s">
+        <v>96</v>
+      </c>
+      <c r="N53" s="135"/>
+      <c r="O53" s="135" t="s">
+        <v>96</v>
+      </c>
+      <c r="P53" s="135"/>
     </row>
     <row r="54" spans="1:16">
-      <c r="B54" s="138" t="s">
+      <c r="B54" s="134" t="s">
         <v>97</v>
       </c>
-      <c r="C54" s="137" t="s">
-        <v>96</v>
-      </c>
-      <c r="D54" s="134"/>
-      <c r="E54" s="134" t="s">
-        <v>96</v>
-      </c>
-      <c r="F54" s="134"/>
-      <c r="G54" s="136" t="s">
-        <v>96</v>
-      </c>
-      <c r="H54" s="136"/>
-      <c r="I54" s="136" t="s">
-        <v>96</v>
-      </c>
-      <c r="J54" s="136"/>
-      <c r="K54" s="135"/>
-      <c r="L54" s="134"/>
-      <c r="M54" s="133"/>
-      <c r="N54" s="133"/>
-      <c r="O54" s="133"/>
-      <c r="P54" s="133"/>
+      <c r="C54" s="220" t="s">
+        <v>96</v>
+      </c>
+      <c r="D54" s="221"/>
+      <c r="E54" s="222" t="s">
+        <v>96</v>
+      </c>
+      <c r="F54" s="221"/>
+      <c r="G54" s="223" t="s">
+        <v>96</v>
+      </c>
+      <c r="H54" s="223"/>
+      <c r="I54" s="223" t="s">
+        <v>96</v>
+      </c>
+      <c r="J54" s="223"/>
+      <c r="K54" s="224"/>
+      <c r="L54" s="221"/>
+      <c r="M54" s="225"/>
+      <c r="N54" s="225"/>
+      <c r="O54" s="225"/>
+      <c r="P54" s="225"/>
     </row>
     <row r="55" spans="1:16" ht="5.25" customHeight="1">
       <c r="K55" s="129"/>
@@ -4804,6 +4861,12 @@
     <row r="57" spans="1:16" ht="5.25" customHeight="1"/>
     <row r="58" spans="1:16">
       <c r="A58" s="130"/>
+      <c r="P58" s="170" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16">
+      <c r="P59" s="206"/>
     </row>
     <row r="60" spans="1:16">
       <c r="A60" s="129"/>

</xml_diff>